<commit_message>
Major refactoring, moved to VIC Bank 1
</commit_message>
<xml_diff>
--- a/Docs/Vortex Memory Map.xlsx
+++ b/Docs/Vortex Memory Map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>TOP OF MEMORY</t>
   </si>
@@ -163,12 +163,21 @@
   <si>
     <t>BANK 1</t>
   </si>
+  <si>
+    <t>Vortex Screen</t>
+  </si>
+  <si>
+    <t>Vortex Character Set</t>
+  </si>
+  <si>
+    <t>Vortex Sprites</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +189,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +251,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,8 +320,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -354,6 +388,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -388,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -396,7 +439,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -404,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -416,56 +459,66 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,13 +832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G171" sqref="G171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="54" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="58" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="5.140625" customWidth="1"/>
@@ -795,439 +848,439 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54"/>
-      <c r="C1" s="56" t="s">
+      <c r="A1" s="58"/>
+      <c r="C1" s="60" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="45"/>
+      <c r="F1" s="49"/>
       <c r="G1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="58" t="s">
         <v>38</v>
       </c>
       <c r="B2">
         <v>65536</v>
       </c>
-      <c r="C2" s="51" t="str">
+      <c r="C2" s="55" t="str">
         <f>DEC2HEX(B2-1)</f>
         <v>FFFF</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="46"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>B2-256</f>
         <v>65280</v>
       </c>
-      <c r="C3" s="52" t="str">
+      <c r="C3" s="56" t="str">
         <f t="shared" ref="C3:C66" si="0">DEC2HEX(B3)</f>
         <v>FF00</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" ref="B4:B67" si="1">B3-256</f>
         <v>65024</v>
       </c>
-      <c r="C4" s="52" t="str">
+      <c r="C4" s="56" t="str">
         <f t="shared" si="0"/>
         <v>FE00</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="46"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" si="1"/>
         <v>64768</v>
       </c>
-      <c r="C5" s="52" t="str">
+      <c r="C5" s="56" t="str">
         <f t="shared" si="0"/>
         <v>FD00</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="1"/>
         <v>64512</v>
       </c>
-      <c r="C6" s="52" t="str">
+      <c r="C6" s="56" t="str">
         <f t="shared" si="0"/>
         <v>FC00</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="50"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>64256</v>
       </c>
-      <c r="C7" s="52" t="str">
+      <c r="C7" s="56" t="str">
         <f t="shared" si="0"/>
         <v>FB00</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="50"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="1"/>
         <v>64000</v>
       </c>
-      <c r="C8" s="52" t="str">
+      <c r="C8" s="56" t="str">
         <f t="shared" si="0"/>
         <v>FA00</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>63744</v>
       </c>
-      <c r="C9" s="52" t="str">
+      <c r="C9" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F900</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="50"/>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>63488</v>
       </c>
-      <c r="C10" s="52" t="str">
+      <c r="C10" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F800</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>63232</v>
       </c>
-      <c r="C11" s="52" t="str">
+      <c r="C11" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F700</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="50"/>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>62976</v>
       </c>
-      <c r="C12" s="52" t="str">
+      <c r="C12" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F600</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>62720</v>
       </c>
-      <c r="C13" s="52" t="str">
+      <c r="C13" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F500</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="46"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>62464</v>
       </c>
-      <c r="C14" s="52" t="str">
+      <c r="C14" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F400</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="50"/>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>62208</v>
       </c>
-      <c r="C15" s="52" t="str">
+      <c r="C15" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F300</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="46"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>61952</v>
       </c>
-      <c r="C16" s="52" t="str">
+      <c r="C16" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F200</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="1"/>
         <v>61696</v>
       </c>
-      <c r="C17" s="52" t="str">
+      <c r="C17" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F100</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="46"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="1"/>
         <v>61440</v>
       </c>
-      <c r="C18" s="52" t="str">
+      <c r="C18" s="56" t="str">
         <f t="shared" si="0"/>
         <v>F000</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>61184</v>
       </c>
-      <c r="C19" s="52" t="str">
+      <c r="C19" s="56" t="str">
         <f t="shared" si="0"/>
         <v>EF00</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="46"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>60928</v>
       </c>
-      <c r="C20" s="52" t="str">
+      <c r="C20" s="56" t="str">
         <f t="shared" si="0"/>
         <v>EE00</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="46"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="50"/>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="55"/>
+      <c r="A21" s="59"/>
       <c r="B21">
         <f t="shared" si="1"/>
         <v>60672</v>
       </c>
-      <c r="C21" s="52" t="str">
+      <c r="C21" s="56" t="str">
         <f t="shared" si="0"/>
         <v>ED00</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="50"/>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="55"/>
+      <c r="A22" s="59"/>
       <c r="B22">
         <f t="shared" si="1"/>
         <v>60416</v>
       </c>
-      <c r="C22" s="52" t="str">
+      <c r="C22" s="56" t="str">
         <f t="shared" si="0"/>
         <v>EC00</v>
       </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="46"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="50"/>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="55"/>
+      <c r="A23" s="59"/>
       <c r="B23">
         <f t="shared" si="1"/>
         <v>60160</v>
       </c>
-      <c r="C23" s="52" t="str">
+      <c r="C23" s="56" t="str">
         <f t="shared" si="0"/>
         <v>EB00</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="50"/>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="55"/>
+      <c r="A24" s="59"/>
       <c r="B24">
         <f t="shared" si="1"/>
         <v>59904</v>
       </c>
-      <c r="C24" s="52" t="str">
+      <c r="C24" s="56" t="str">
         <f t="shared" si="0"/>
         <v>EA00</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="50"/>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="55"/>
+      <c r="A25" s="59"/>
       <c r="B25">
         <f t="shared" si="1"/>
         <v>59648</v>
       </c>
-      <c r="C25" s="52" t="str">
+      <c r="C25" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E900</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="55"/>
+      <c r="A26" s="59"/>
       <c r="B26">
         <f t="shared" si="1"/>
         <v>59392</v>
       </c>
-      <c r="C26" s="52" t="str">
+      <c r="C26" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E800</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="46"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="50"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="1"/>
         <v>59136</v>
       </c>
-      <c r="C27" s="52" t="str">
+      <c r="C27" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E700</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="46"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="50"/>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="1"/>
         <v>58880</v>
       </c>
-      <c r="C28" s="52" t="str">
+      <c r="C28" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E600</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="46"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="50"/>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="1"/>
         <v>58624</v>
       </c>
-      <c r="C29" s="52" t="str">
+      <c r="C29" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E500</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="46"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="50"/>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="1"/>
         <v>58368</v>
       </c>
-      <c r="C30" s="52" t="str">
+      <c r="C30" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E400</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="46"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="1"/>
         <v>58112</v>
       </c>
-      <c r="C31" s="52" t="str">
+      <c r="C31" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E300</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="50"/>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="1"/>
         <v>57856</v>
       </c>
-      <c r="C32" s="52" t="str">
+      <c r="C32" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E200</v>
       </c>
-      <c r="E32" s="43"/>
-      <c r="F32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="50"/>
     </row>
     <row r="33" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="1"/>
         <v>57600</v>
       </c>
-      <c r="C33" s="52" t="str">
+      <c r="C33" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E100</v>
       </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="50"/>
     </row>
     <row r="34" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C34" s="52" t="str">
+      <c r="C34" s="56" t="str">
         <f t="shared" si="0"/>
         <v>E000</v>
       </c>
-      <c r="E34" s="44" t="s">
+      <c r="E34" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="46"/>
+      <c r="F34" s="50"/>
     </row>
     <row r="35" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="1"/>
         <v>57088</v>
       </c>
-      <c r="C35" s="52" t="str">
+      <c r="C35" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DF00</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="47"/>
+      <c r="F35" s="51"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1235,12 +1288,12 @@
         <f t="shared" si="1"/>
         <v>56832</v>
       </c>
-      <c r="C36" s="52" t="str">
+      <c r="C36" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DE00</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="47"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="51"/>
       <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1248,11 +1301,11 @@
         <f t="shared" si="1"/>
         <v>56576</v>
       </c>
-      <c r="C37" s="52" t="str">
+      <c r="C37" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DD00</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="27" t="s">
         <v>32</v>
       </c>
       <c r="G37" s="13"/>
@@ -1262,11 +1315,11 @@
         <f t="shared" si="1"/>
         <v>56320</v>
       </c>
-      <c r="C38" s="52" t="str">
+      <c r="C38" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DC00</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="33" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="13"/>
@@ -1276,7 +1329,7 @@
         <f t="shared" si="1"/>
         <v>56064</v>
       </c>
-      <c r="C39" s="52" t="str">
+      <c r="C39" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DB00</v>
       </c>
@@ -1288,7 +1341,7 @@
         <f t="shared" si="1"/>
         <v>55808</v>
       </c>
-      <c r="C40" s="52" t="str">
+      <c r="C40" s="56" t="str">
         <f t="shared" si="0"/>
         <v>DA00</v>
       </c>
@@ -1300,7 +1353,7 @@
         <f t="shared" si="1"/>
         <v>55552</v>
       </c>
-      <c r="C41" s="52" t="str">
+      <c r="C41" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D900</v>
       </c>
@@ -1312,11 +1365,11 @@
         <f t="shared" si="1"/>
         <v>55296</v>
       </c>
-      <c r="C42" s="52" t="str">
+      <c r="C42" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D800</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G42" s="13"/>
@@ -1326,11 +1379,11 @@
         <f t="shared" si="1"/>
         <v>55040</v>
       </c>
-      <c r="C43" s="52" t="str">
+      <c r="C43" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D700</v>
       </c>
-      <c r="E43" s="24"/>
+      <c r="E43" s="28"/>
       <c r="G43" s="13"/>
     </row>
     <row r="44" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,11 +1391,11 @@
         <f t="shared" si="1"/>
         <v>54784</v>
       </c>
-      <c r="C44" s="52" t="str">
+      <c r="C44" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D600</v>
       </c>
-      <c r="E44" s="25"/>
+      <c r="E44" s="29"/>
       <c r="G44" s="13"/>
     </row>
     <row r="45" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1350,11 +1403,11 @@
         <f t="shared" si="1"/>
         <v>54528</v>
       </c>
-      <c r="C45" s="52" t="str">
+      <c r="C45" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D500</v>
       </c>
-      <c r="E45" s="25"/>
+      <c r="E45" s="29"/>
       <c r="G45" s="13"/>
     </row>
     <row r="46" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,11 +1415,11 @@
         <f t="shared" si="1"/>
         <v>54272</v>
       </c>
-      <c r="C46" s="52" t="str">
+      <c r="C46" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D400</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E46" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G46" s="13"/>
@@ -1376,11 +1429,11 @@
         <f t="shared" si="1"/>
         <v>54016</v>
       </c>
-      <c r="C47" s="52" t="str">
+      <c r="C47" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D300</v>
       </c>
-      <c r="E47" s="27"/>
+      <c r="E47" s="31"/>
       <c r="G47" s="13"/>
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,11 +1441,11 @@
         <f t="shared" si="1"/>
         <v>53760</v>
       </c>
-      <c r="C48" s="52" t="str">
+      <c r="C48" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D200</v>
       </c>
-      <c r="E48" s="28"/>
+      <c r="E48" s="32"/>
       <c r="G48" s="13"/>
     </row>
     <row r="49" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1400,11 +1453,11 @@
         <f t="shared" si="1"/>
         <v>53504</v>
       </c>
-      <c r="C49" s="52" t="str">
+      <c r="C49" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D100</v>
       </c>
-      <c r="E49" s="28"/>
+      <c r="E49" s="32"/>
       <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,11 +1465,11 @@
         <f t="shared" si="1"/>
         <v>53248</v>
       </c>
-      <c r="C50" s="52" t="str">
+      <c r="C50" s="56" t="str">
         <f t="shared" si="0"/>
         <v>D000</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="32" t="s">
         <v>30</v>
       </c>
       <c r="G50" s="14" t="s">
@@ -1428,7 +1481,7 @@
         <f t="shared" si="1"/>
         <v>52992</v>
       </c>
-      <c r="C51" s="52" t="str">
+      <c r="C51" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CF00</v>
       </c>
@@ -1439,7 +1492,7 @@
         <f t="shared" si="1"/>
         <v>52736</v>
       </c>
-      <c r="C52" s="52" t="str">
+      <c r="C52" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CE00</v>
       </c>
@@ -1450,7 +1503,7 @@
         <f t="shared" si="1"/>
         <v>52480</v>
       </c>
-      <c r="C53" s="52" t="str">
+      <c r="C53" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CD00</v>
       </c>
@@ -1461,7 +1514,7 @@
         <f t="shared" si="1"/>
         <v>52224</v>
       </c>
-      <c r="C54" s="52" t="str">
+      <c r="C54" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CC00</v>
       </c>
@@ -1472,7 +1525,7 @@
         <f t="shared" si="1"/>
         <v>51968</v>
       </c>
-      <c r="C55" s="52" t="str">
+      <c r="C55" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CB00</v>
       </c>
@@ -1483,7 +1536,7 @@
         <f t="shared" si="1"/>
         <v>51712</v>
       </c>
-      <c r="C56" s="52" t="str">
+      <c r="C56" s="56" t="str">
         <f t="shared" si="0"/>
         <v>CA00</v>
       </c>
@@ -1494,7 +1547,7 @@
         <f t="shared" si="1"/>
         <v>51456</v>
       </c>
-      <c r="C57" s="52" t="str">
+      <c r="C57" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C900</v>
       </c>
@@ -1505,7 +1558,7 @@
         <f t="shared" si="1"/>
         <v>51200</v>
       </c>
-      <c r="C58" s="52" t="str">
+      <c r="C58" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C800</v>
       </c>
@@ -1516,7 +1569,7 @@
         <f t="shared" si="1"/>
         <v>50944</v>
       </c>
-      <c r="C59" s="52" t="str">
+      <c r="C59" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C700</v>
       </c>
@@ -1527,7 +1580,7 @@
         <f t="shared" si="1"/>
         <v>50688</v>
       </c>
-      <c r="C60" s="52" t="str">
+      <c r="C60" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C600</v>
       </c>
@@ -1538,7 +1591,7 @@
         <f t="shared" si="1"/>
         <v>50432</v>
       </c>
-      <c r="C61" s="52" t="str">
+      <c r="C61" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C500</v>
       </c>
@@ -1549,7 +1602,7 @@
         <f t="shared" si="1"/>
         <v>50176</v>
       </c>
-      <c r="C62" s="52" t="str">
+      <c r="C62" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C400</v>
       </c>
@@ -1560,7 +1613,7 @@
         <f t="shared" si="1"/>
         <v>49920</v>
       </c>
-      <c r="C63" s="52" t="str">
+      <c r="C63" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C300</v>
       </c>
@@ -1571,7 +1624,7 @@
         <f t="shared" si="1"/>
         <v>49664</v>
       </c>
-      <c r="C64" s="52" t="str">
+      <c r="C64" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C200</v>
       </c>
@@ -1582,386 +1635,386 @@
         <f t="shared" si="1"/>
         <v>49408</v>
       </c>
-      <c r="C65" s="52" t="str">
+      <c r="C65" s="56" t="str">
         <f t="shared" si="0"/>
         <v>C100</v>
       </c>
       <c r="E65" s="19"/>
     </row>
     <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="58" t="s">
         <v>38</v>
       </c>
       <c r="B66">
         <f t="shared" si="1"/>
         <v>49152</v>
       </c>
-      <c r="C66" s="53" t="str">
+      <c r="C66" s="57" t="str">
         <f t="shared" si="0"/>
         <v>C000</v>
       </c>
-      <c r="E66" s="33"/>
+      <c r="E66" s="37"/>
     </row>
     <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="58" t="s">
         <v>39</v>
       </c>
       <c r="B67">
         <f t="shared" si="1"/>
         <v>48896</v>
       </c>
-      <c r="C67" s="48" t="str">
+      <c r="C67" s="52" t="str">
         <f t="shared" ref="C67:C130" si="2">DEC2HEX(B67)</f>
         <v>BF00</v>
       </c>
-      <c r="E67" s="30"/>
+      <c r="E67" s="34"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" ref="B68:B131" si="3">B67-256</f>
         <v>48640</v>
       </c>
-      <c r="C68" s="49" t="str">
+      <c r="C68" s="53" t="str">
         <f t="shared" si="2"/>
         <v>BE00</v>
       </c>
-      <c r="E68" s="31"/>
+      <c r="E68" s="35"/>
     </row>
     <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="3"/>
         <v>48384</v>
       </c>
-      <c r="C69" s="49" t="str">
+      <c r="C69" s="53" t="str">
         <f t="shared" si="2"/>
         <v>BD00</v>
       </c>
-      <c r="E69" s="31"/>
+      <c r="E69" s="35"/>
     </row>
     <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="3"/>
         <v>48128</v>
       </c>
-      <c r="C70" s="49" t="str">
+      <c r="C70" s="53" t="str">
         <f t="shared" si="2"/>
         <v>BC00</v>
       </c>
-      <c r="E70" s="31"/>
+      <c r="E70" s="35"/>
     </row>
     <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="3"/>
         <v>47872</v>
       </c>
-      <c r="C71" s="49" t="str">
+      <c r="C71" s="53" t="str">
         <f t="shared" si="2"/>
         <v>BB00</v>
       </c>
-      <c r="E71" s="31"/>
+      <c r="E71" s="35"/>
     </row>
     <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="3"/>
         <v>47616</v>
       </c>
-      <c r="C72" s="49" t="str">
+      <c r="C72" s="53" t="str">
         <f t="shared" si="2"/>
         <v>BA00</v>
       </c>
-      <c r="E72" s="31"/>
+      <c r="E72" s="35"/>
     </row>
     <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="3"/>
         <v>47360</v>
       </c>
-      <c r="C73" s="49" t="str">
+      <c r="C73" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B900</v>
       </c>
-      <c r="E73" s="31"/>
+      <c r="E73" s="35"/>
     </row>
     <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="3"/>
         <v>47104</v>
       </c>
-      <c r="C74" s="49" t="str">
+      <c r="C74" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B800</v>
       </c>
-      <c r="E74" s="31"/>
+      <c r="E74" s="35"/>
     </row>
     <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="3"/>
         <v>46848</v>
       </c>
-      <c r="C75" s="49" t="str">
+      <c r="C75" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B700</v>
       </c>
-      <c r="E75" s="31"/>
+      <c r="E75" s="35"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="3"/>
         <v>46592</v>
       </c>
-      <c r="C76" s="49" t="str">
+      <c r="C76" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B600</v>
       </c>
-      <c r="E76" s="31"/>
+      <c r="E76" s="35"/>
     </row>
     <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="3"/>
         <v>46336</v>
       </c>
-      <c r="C77" s="49" t="str">
+      <c r="C77" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B500</v>
       </c>
-      <c r="E77" s="31"/>
+      <c r="E77" s="35"/>
     </row>
     <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="3"/>
         <v>46080</v>
       </c>
-      <c r="C78" s="49" t="str">
+      <c r="C78" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B400</v>
       </c>
-      <c r="E78" s="31"/>
+      <c r="E78" s="35"/>
     </row>
     <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="3"/>
         <v>45824</v>
       </c>
-      <c r="C79" s="49" t="str">
+      <c r="C79" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B300</v>
       </c>
-      <c r="E79" s="31"/>
+      <c r="E79" s="35"/>
     </row>
     <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="3"/>
         <v>45568</v>
       </c>
-      <c r="C80" s="49" t="str">
+      <c r="C80" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B200</v>
       </c>
-      <c r="E80" s="31"/>
+      <c r="E80" s="35"/>
     </row>
     <row r="81" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="3"/>
         <v>45312</v>
       </c>
-      <c r="C81" s="49" t="str">
+      <c r="C81" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B100</v>
       </c>
-      <c r="E81" s="31"/>
+      <c r="E81" s="35"/>
     </row>
     <row r="82" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="3"/>
         <v>45056</v>
       </c>
-      <c r="C82" s="49" t="str">
+      <c r="C82" s="53" t="str">
         <f t="shared" si="2"/>
         <v>B000</v>
       </c>
-      <c r="E82" s="31"/>
+      <c r="E82" s="35"/>
     </row>
     <row r="83" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="3"/>
         <v>44800</v>
       </c>
-      <c r="C83" s="49" t="str">
+      <c r="C83" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AF00</v>
       </c>
-      <c r="E83" s="31"/>
+      <c r="E83" s="35"/>
     </row>
     <row r="84" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="3"/>
         <v>44544</v>
       </c>
-      <c r="C84" s="49" t="str">
+      <c r="C84" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AE00</v>
       </c>
-      <c r="E84" s="31"/>
+      <c r="E84" s="35"/>
     </row>
     <row r="85" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" si="3"/>
         <v>44288</v>
       </c>
-      <c r="C85" s="49" t="str">
+      <c r="C85" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AD00</v>
       </c>
-      <c r="E85" s="31"/>
+      <c r="E85" s="35"/>
     </row>
     <row r="86" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="3"/>
         <v>44032</v>
       </c>
-      <c r="C86" s="49" t="str">
+      <c r="C86" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AC00</v>
       </c>
-      <c r="E86" s="31"/>
+      <c r="E86" s="35"/>
     </row>
     <row r="87" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="3"/>
         <v>43776</v>
       </c>
-      <c r="C87" s="49" t="str">
+      <c r="C87" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AB00</v>
       </c>
-      <c r="E87" s="31"/>
+      <c r="E87" s="35"/>
     </row>
     <row r="88" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="3"/>
         <v>43520</v>
       </c>
-      <c r="C88" s="49" t="str">
+      <c r="C88" s="53" t="str">
         <f t="shared" si="2"/>
         <v>AA00</v>
       </c>
-      <c r="E88" s="31"/>
+      <c r="E88" s="35"/>
     </row>
     <row r="89" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="3"/>
         <v>43264</v>
       </c>
-      <c r="C89" s="49" t="str">
+      <c r="C89" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A900</v>
       </c>
-      <c r="E89" s="31"/>
+      <c r="E89" s="35"/>
     </row>
     <row r="90" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="3"/>
         <v>43008</v>
       </c>
-      <c r="C90" s="49" t="str">
+      <c r="C90" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A800</v>
       </c>
-      <c r="E90" s="31"/>
+      <c r="E90" s="35"/>
     </row>
     <row r="91" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="3"/>
         <v>42752</v>
       </c>
-      <c r="C91" s="49" t="str">
+      <c r="C91" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A700</v>
       </c>
-      <c r="E91" s="31"/>
+      <c r="E91" s="35"/>
     </row>
     <row r="92" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="3"/>
         <v>42496</v>
       </c>
-      <c r="C92" s="49" t="str">
+      <c r="C92" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A600</v>
       </c>
-      <c r="E92" s="31"/>
+      <c r="E92" s="35"/>
     </row>
     <row r="93" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="55"/>
+      <c r="A93" s="59"/>
       <c r="B93">
         <f t="shared" si="3"/>
         <v>42240</v>
       </c>
-      <c r="C93" s="49" t="str">
+      <c r="C93" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A500</v>
       </c>
-      <c r="E93" s="31"/>
+      <c r="E93" s="35"/>
     </row>
     <row r="94" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="55"/>
+      <c r="A94" s="59"/>
       <c r="B94">
         <f t="shared" si="3"/>
         <v>41984</v>
       </c>
-      <c r="C94" s="49" t="str">
+      <c r="C94" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A400</v>
       </c>
-      <c r="E94" s="31"/>
+      <c r="E94" s="35"/>
     </row>
     <row r="95" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="55"/>
+      <c r="A95" s="59"/>
       <c r="B95">
         <f t="shared" si="3"/>
         <v>41728</v>
       </c>
-      <c r="C95" s="49" t="str">
+      <c r="C95" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A300</v>
       </c>
-      <c r="E95" s="31"/>
+      <c r="E95" s="35"/>
     </row>
     <row r="96" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="55"/>
+      <c r="A96" s="59"/>
       <c r="B96">
         <f t="shared" si="3"/>
         <v>41472</v>
       </c>
-      <c r="C96" s="49" t="str">
+      <c r="C96" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A200</v>
       </c>
-      <c r="E96" s="31"/>
+      <c r="E96" s="35"/>
     </row>
     <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="55"/>
+      <c r="A97" s="59"/>
       <c r="B97">
         <f t="shared" si="3"/>
         <v>41216</v>
       </c>
-      <c r="C97" s="49" t="str">
+      <c r="C97" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A100</v>
       </c>
-      <c r="E97" s="31"/>
+      <c r="E97" s="35"/>
     </row>
     <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="55"/>
+      <c r="A98" s="59"/>
       <c r="B98">
         <f t="shared" si="3"/>
         <v>40960</v>
       </c>
-      <c r="C98" s="49" t="str">
+      <c r="C98" s="53" t="str">
         <f t="shared" si="2"/>
         <v>A000</v>
       </c>
-      <c r="E98" s="32" t="s">
+      <c r="E98" s="36" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1970,192 +2023,192 @@
         <f t="shared" si="3"/>
         <v>40704</v>
       </c>
-      <c r="C99" s="49" t="str">
+      <c r="C99" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9F00</v>
       </c>
       <c r="E99" s="19"/>
-      <c r="G99" s="34"/>
+      <c r="G99" s="38"/>
     </row>
     <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100">
         <f t="shared" si="3"/>
         <v>40448</v>
       </c>
-      <c r="C100" s="49" t="str">
+      <c r="C100" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9E00</v>
       </c>
       <c r="E100" s="19"/>
-      <c r="G100" s="35"/>
+      <c r="G100" s="39"/>
     </row>
     <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101">
         <f t="shared" si="3"/>
         <v>40192</v>
       </c>
-      <c r="C101" s="49" t="str">
+      <c r="C101" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9D00</v>
       </c>
       <c r="E101" s="19"/>
-      <c r="G101" s="35"/>
+      <c r="G101" s="39"/>
     </row>
     <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102">
         <f t="shared" si="3"/>
         <v>39936</v>
       </c>
-      <c r="C102" s="49" t="str">
+      <c r="C102" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9C00</v>
       </c>
       <c r="E102" s="19"/>
-      <c r="G102" s="35"/>
+      <c r="G102" s="39"/>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103">
         <f t="shared" si="3"/>
         <v>39680</v>
       </c>
-      <c r="C103" s="49" t="str">
+      <c r="C103" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9B00</v>
       </c>
       <c r="E103" s="19"/>
-      <c r="G103" s="35"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104">
         <f t="shared" si="3"/>
         <v>39424</v>
       </c>
-      <c r="C104" s="49" t="str">
+      <c r="C104" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9A00</v>
       </c>
       <c r="E104" s="19"/>
-      <c r="G104" s="35"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105">
         <f t="shared" si="3"/>
         <v>39168</v>
       </c>
-      <c r="C105" s="49" t="str">
+      <c r="C105" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9900</v>
       </c>
       <c r="E105" s="19"/>
-      <c r="G105" s="35"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106">
         <f t="shared" si="3"/>
         <v>38912</v>
       </c>
-      <c r="C106" s="49" t="str">
+      <c r="C106" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9800</v>
       </c>
       <c r="E106" s="19"/>
-      <c r="G106" s="35"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107">
         <f t="shared" si="3"/>
         <v>38656</v>
       </c>
-      <c r="C107" s="49" t="str">
+      <c r="C107" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9700</v>
       </c>
       <c r="E107" s="19"/>
-      <c r="G107" s="35"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108">
         <f t="shared" si="3"/>
         <v>38400</v>
       </c>
-      <c r="C108" s="49" t="str">
+      <c r="C108" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9600</v>
       </c>
       <c r="E108" s="19"/>
-      <c r="G108" s="35"/>
+      <c r="G108" s="39"/>
     </row>
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109">
         <f t="shared" si="3"/>
         <v>38144</v>
       </c>
-      <c r="C109" s="49" t="str">
+      <c r="C109" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9500</v>
       </c>
       <c r="E109" s="19"/>
-      <c r="G109" s="35"/>
+      <c r="G109" s="39"/>
     </row>
     <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110">
         <f t="shared" si="3"/>
         <v>37888</v>
       </c>
-      <c r="C110" s="49" t="str">
+      <c r="C110" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9400</v>
       </c>
       <c r="E110" s="19"/>
-      <c r="G110" s="35"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111">
         <f t="shared" si="3"/>
         <v>37632</v>
       </c>
-      <c r="C111" s="49" t="str">
+      <c r="C111" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9300</v>
       </c>
       <c r="E111" s="19"/>
-      <c r="G111" s="35"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112">
         <f t="shared" si="3"/>
         <v>37376</v>
       </c>
-      <c r="C112" s="49" t="str">
+      <c r="C112" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9200</v>
       </c>
       <c r="E112" s="19"/>
-      <c r="G112" s="35"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113">
         <f t="shared" si="3"/>
         <v>37120</v>
       </c>
-      <c r="C113" s="49" t="str">
+      <c r="C113" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9100</v>
       </c>
       <c r="E113" s="19"/>
-      <c r="G113" s="35"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114">
         <f t="shared" si="3"/>
         <v>36864</v>
       </c>
-      <c r="C114" s="49" t="str">
+      <c r="C114" s="53" t="str">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
       <c r="E114" s="19"/>
-      <c r="G114" s="36" t="s">
+      <c r="G114" s="40" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2164,7 +2217,7 @@
         <f t="shared" si="3"/>
         <v>36608</v>
       </c>
-      <c r="C115" s="49" t="str">
+      <c r="C115" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8F00</v>
       </c>
@@ -2175,7 +2228,7 @@
         <f t="shared" si="3"/>
         <v>36352</v>
       </c>
-      <c r="C116" s="49" t="str">
+      <c r="C116" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8E00</v>
       </c>
@@ -2186,7 +2239,7 @@
         <f t="shared" si="3"/>
         <v>36096</v>
       </c>
-      <c r="C117" s="49" t="str">
+      <c r="C117" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8D00</v>
       </c>
@@ -2197,7 +2250,7 @@
         <f t="shared" si="3"/>
         <v>35840</v>
       </c>
-      <c r="C118" s="49" t="str">
+      <c r="C118" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8C00</v>
       </c>
@@ -2208,7 +2261,7 @@
         <f t="shared" si="3"/>
         <v>35584</v>
       </c>
-      <c r="C119" s="49" t="str">
+      <c r="C119" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8B00</v>
       </c>
@@ -2219,7 +2272,7 @@
         <f t="shared" si="3"/>
         <v>35328</v>
       </c>
-      <c r="C120" s="49" t="str">
+      <c r="C120" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8A00</v>
       </c>
@@ -2230,7 +2283,7 @@
         <f t="shared" si="3"/>
         <v>35072</v>
       </c>
-      <c r="C121" s="49" t="str">
+      <c r="C121" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8900</v>
       </c>
@@ -2241,7 +2294,7 @@
         <f t="shared" si="3"/>
         <v>34816</v>
       </c>
-      <c r="C122" s="49" t="str">
+      <c r="C122" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8800</v>
       </c>
@@ -2252,7 +2305,7 @@
         <f t="shared" si="3"/>
         <v>34560</v>
       </c>
-      <c r="C123" s="49" t="str">
+      <c r="C123" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8700</v>
       </c>
@@ -2263,7 +2316,7 @@
         <f t="shared" si="3"/>
         <v>34304</v>
       </c>
-      <c r="C124" s="49" t="str">
+      <c r="C124" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8600</v>
       </c>
@@ -2274,7 +2327,7 @@
         <f t="shared" si="3"/>
         <v>34048</v>
       </c>
-      <c r="C125" s="49" t="str">
+      <c r="C125" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8500</v>
       </c>
@@ -2285,7 +2338,7 @@
         <f t="shared" si="3"/>
         <v>33792</v>
       </c>
-      <c r="C126" s="49" t="str">
+      <c r="C126" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8400</v>
       </c>
@@ -2296,7 +2349,7 @@
         <f t="shared" si="3"/>
         <v>33536</v>
       </c>
-      <c r="C127" s="49" t="str">
+      <c r="C127" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8300</v>
       </c>
@@ -2307,7 +2360,7 @@
         <f t="shared" si="3"/>
         <v>33280</v>
       </c>
-      <c r="C128" s="49" t="str">
+      <c r="C128" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8200</v>
       </c>
@@ -2318,35 +2371,35 @@
         <f t="shared" si="3"/>
         <v>33024</v>
       </c>
-      <c r="C129" s="49" t="str">
+      <c r="C129" s="53" t="str">
         <f t="shared" si="2"/>
         <v>8100</v>
       </c>
       <c r="E129" s="19"/>
     </row>
     <row r="130" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="54" t="s">
+      <c r="A130" s="58" t="s">
         <v>39</v>
       </c>
       <c r="B130">
         <f t="shared" si="3"/>
         <v>32768</v>
       </c>
-      <c r="C130" s="50" t="str">
+      <c r="C130" s="54" t="str">
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
       <c r="E130" s="19"/>
     </row>
     <row r="131" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="54" t="s">
+      <c r="A131" s="58" t="s">
         <v>40</v>
       </c>
       <c r="B131">
         <f t="shared" si="3"/>
         <v>32512</v>
       </c>
-      <c r="C131" s="51" t="str">
+      <c r="C131" s="55" t="str">
         <f t="shared" ref="C131:C194" si="4">DEC2HEX(B131)</f>
         <v>7F00</v>
       </c>
@@ -2357,7 +2410,7 @@
         <f t="shared" ref="B132:B195" si="5">B131-256</f>
         <v>32256</v>
       </c>
-      <c r="C132" s="52" t="str">
+      <c r="C132" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7E00</v>
       </c>
@@ -2368,7 +2421,7 @@
         <f t="shared" si="5"/>
         <v>32000</v>
       </c>
-      <c r="C133" s="52" t="str">
+      <c r="C133" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7D00</v>
       </c>
@@ -2379,7 +2432,7 @@
         <f t="shared" si="5"/>
         <v>31744</v>
       </c>
-      <c r="C134" s="52" t="str">
+      <c r="C134" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7C00</v>
       </c>
@@ -2390,7 +2443,7 @@
         <f t="shared" si="5"/>
         <v>31488</v>
       </c>
-      <c r="C135" s="52" t="str">
+      <c r="C135" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7B00</v>
       </c>
@@ -2401,7 +2454,7 @@
         <f t="shared" si="5"/>
         <v>31232</v>
       </c>
-      <c r="C136" s="52" t="str">
+      <c r="C136" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7A00</v>
       </c>
@@ -2412,7 +2465,7 @@
         <f t="shared" si="5"/>
         <v>30976</v>
       </c>
-      <c r="C137" s="52" t="str">
+      <c r="C137" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7900</v>
       </c>
@@ -2423,7 +2476,7 @@
         <f t="shared" si="5"/>
         <v>30720</v>
       </c>
-      <c r="C138" s="52" t="str">
+      <c r="C138" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7800</v>
       </c>
@@ -2434,7 +2487,7 @@
         <f t="shared" si="5"/>
         <v>30464</v>
       </c>
-      <c r="C139" s="52" t="str">
+      <c r="C139" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7700</v>
       </c>
@@ -2445,7 +2498,7 @@
         <f t="shared" si="5"/>
         <v>30208</v>
       </c>
-      <c r="C140" s="52" t="str">
+      <c r="C140" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7600</v>
       </c>
@@ -2456,7 +2509,7 @@
         <f t="shared" si="5"/>
         <v>29952</v>
       </c>
-      <c r="C141" s="52" t="str">
+      <c r="C141" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7500</v>
       </c>
@@ -2467,7 +2520,7 @@
         <f t="shared" si="5"/>
         <v>29696</v>
       </c>
-      <c r="C142" s="52" t="str">
+      <c r="C142" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7400</v>
       </c>
@@ -2478,7 +2531,7 @@
         <f t="shared" si="5"/>
         <v>29440</v>
       </c>
-      <c r="C143" s="52" t="str">
+      <c r="C143" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7300</v>
       </c>
@@ -2489,7 +2542,7 @@
         <f t="shared" si="5"/>
         <v>29184</v>
       </c>
-      <c r="C144" s="52" t="str">
+      <c r="C144" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7200</v>
       </c>
@@ -2500,7 +2553,7 @@
         <f t="shared" si="5"/>
         <v>28928</v>
       </c>
-      <c r="C145" s="52" t="str">
+      <c r="C145" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7100</v>
       </c>
@@ -2511,7 +2564,7 @@
         <f t="shared" si="5"/>
         <v>28672</v>
       </c>
-      <c r="C146" s="52" t="str">
+      <c r="C146" s="56" t="str">
         <f t="shared" si="4"/>
         <v>7000</v>
       </c>
@@ -2522,7 +2575,7 @@
         <f t="shared" si="5"/>
         <v>28416</v>
       </c>
-      <c r="C147" s="52" t="str">
+      <c r="C147" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6F00</v>
       </c>
@@ -2533,679 +2586,686 @@
         <f t="shared" si="5"/>
         <v>28160</v>
       </c>
-      <c r="C148" s="52" t="str">
+      <c r="C148" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6E00</v>
       </c>
-      <c r="E148" s="19"/>
+      <c r="E148" s="24"/>
     </row>
     <row r="149" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A149" s="55"/>
+      <c r="A149" s="59"/>
       <c r="B149">
         <f t="shared" si="5"/>
         <v>27904</v>
       </c>
-      <c r="C149" s="52" t="str">
+      <c r="C149" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6D00</v>
       </c>
-      <c r="E149" s="19"/>
+      <c r="E149" s="24"/>
     </row>
     <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A150" s="55"/>
+      <c r="A150" s="59"/>
       <c r="B150">
         <f t="shared" si="5"/>
         <v>27648</v>
       </c>
-      <c r="C150" s="52" t="str">
+      <c r="C150" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6C00</v>
       </c>
-      <c r="E150" s="19"/>
+      <c r="E150" s="24"/>
     </row>
     <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A151" s="55"/>
+      <c r="A151" s="59"/>
       <c r="B151">
         <f t="shared" si="5"/>
         <v>27392</v>
       </c>
-      <c r="C151" s="52" t="str">
+      <c r="C151" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6B00</v>
       </c>
-      <c r="E151" s="19"/>
+      <c r="E151" s="24"/>
     </row>
     <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A152" s="55"/>
+      <c r="A152" s="59"/>
       <c r="B152">
         <f t="shared" si="5"/>
         <v>27136</v>
       </c>
-      <c r="C152" s="52" t="str">
+      <c r="C152" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6A00</v>
       </c>
-      <c r="E152" s="19"/>
+      <c r="E152" s="24"/>
     </row>
     <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A153" s="55"/>
+      <c r="A153" s="59"/>
       <c r="B153">
         <f t="shared" si="5"/>
         <v>26880</v>
       </c>
-      <c r="C153" s="52" t="str">
+      <c r="C153" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6900</v>
       </c>
-      <c r="E153" s="19"/>
+      <c r="E153" s="24"/>
     </row>
     <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A154" s="55"/>
+      <c r="A154" s="59"/>
       <c r="B154">
         <f t="shared" si="5"/>
         <v>26624</v>
       </c>
-      <c r="C154" s="52" t="str">
+      <c r="C154" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6800</v>
       </c>
-      <c r="E154" s="19"/>
+      <c r="E154" s="24"/>
     </row>
     <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155">
         <f t="shared" si="5"/>
         <v>26368</v>
       </c>
-      <c r="C155" s="52" t="str">
+      <c r="C155" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6700</v>
       </c>
-      <c r="E155" s="19"/>
+      <c r="E155" s="24"/>
     </row>
     <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156">
         <f t="shared" si="5"/>
         <v>26112</v>
       </c>
-      <c r="C156" s="52" t="str">
+      <c r="C156" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6600</v>
       </c>
-      <c r="E156" s="19"/>
+      <c r="E156" s="24"/>
     </row>
     <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157">
         <f t="shared" si="5"/>
         <v>25856</v>
       </c>
-      <c r="C157" s="52" t="str">
+      <c r="C157" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6500</v>
       </c>
-      <c r="E157" s="19"/>
+      <c r="E157" s="24"/>
     </row>
     <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158">
         <f t="shared" si="5"/>
         <v>25600</v>
       </c>
-      <c r="C158" s="52" t="str">
+      <c r="C158" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6400</v>
       </c>
-      <c r="E158" s="19"/>
+      <c r="E158" s="24"/>
     </row>
     <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159">
         <f t="shared" si="5"/>
         <v>25344</v>
       </c>
-      <c r="C159" s="52" t="str">
+      <c r="C159" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6300</v>
       </c>
-      <c r="E159" s="19"/>
+      <c r="E159" s="24"/>
     </row>
     <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160">
         <f t="shared" si="5"/>
         <v>25088</v>
       </c>
-      <c r="C160" s="52" t="str">
+      <c r="C160" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6200</v>
       </c>
-      <c r="E160" s="19"/>
+      <c r="E160" s="24"/>
     </row>
     <row r="161" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161">
         <f t="shared" si="5"/>
         <v>24832</v>
       </c>
-      <c r="C161" s="52" t="str">
+      <c r="C161" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6100</v>
       </c>
-      <c r="E161" s="19"/>
+      <c r="E161" s="24"/>
     </row>
     <row r="162" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162">
         <f t="shared" si="5"/>
         <v>24576</v>
       </c>
-      <c r="C162" s="52" t="str">
+      <c r="C162" s="56" t="str">
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
-      <c r="E162" s="19"/>
+      <c r="E162" s="24"/>
     </row>
     <row r="163" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163">
         <f t="shared" si="5"/>
         <v>24320</v>
       </c>
-      <c r="C163" s="52" t="str">
+      <c r="C163" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5F00</v>
       </c>
-      <c r="E163" s="19"/>
+      <c r="E163" s="24"/>
     </row>
     <row r="164" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164">
         <f t="shared" si="5"/>
         <v>24064</v>
       </c>
-      <c r="C164" s="52" t="str">
+      <c r="C164" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5E00</v>
       </c>
-      <c r="E164" s="19"/>
+      <c r="E164" s="24"/>
     </row>
     <row r="165" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165">
         <f t="shared" si="5"/>
         <v>23808</v>
       </c>
-      <c r="C165" s="52" t="str">
+      <c r="C165" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5D00</v>
       </c>
-      <c r="E165" s="19"/>
+      <c r="E165" s="24"/>
     </row>
     <row r="166" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166">
         <f t="shared" si="5"/>
         <v>23552</v>
       </c>
-      <c r="C166" s="52" t="str">
+      <c r="C166" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5C00</v>
       </c>
-      <c r="E166" s="19"/>
+      <c r="E166" s="24"/>
     </row>
     <row r="167" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167">
         <f t="shared" si="5"/>
         <v>23296</v>
       </c>
-      <c r="C167" s="52" t="str">
+      <c r="C167" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5B00</v>
       </c>
-      <c r="E167" s="19"/>
+      <c r="E167" s="24"/>
     </row>
     <row r="168" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168">
         <f t="shared" si="5"/>
         <v>23040</v>
       </c>
-      <c r="C168" s="52" t="str">
+      <c r="C168" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5A00</v>
       </c>
-      <c r="E168" s="19"/>
+      <c r="E168" s="24"/>
     </row>
     <row r="169" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169">
         <f t="shared" si="5"/>
         <v>22784</v>
       </c>
-      <c r="C169" s="52" t="str">
+      <c r="C169" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5900</v>
       </c>
-      <c r="E169" s="19"/>
+      <c r="E169" s="24"/>
     </row>
     <row r="170" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170">
         <f t="shared" si="5"/>
         <v>22528</v>
       </c>
-      <c r="C170" s="52" t="str">
+      <c r="C170" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5800</v>
       </c>
-      <c r="E170" s="19"/>
+      <c r="E170" s="24"/>
     </row>
     <row r="171" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171">
         <f t="shared" si="5"/>
         <v>22272</v>
       </c>
-      <c r="C171" s="52" t="str">
+      <c r="C171" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5700</v>
       </c>
-      <c r="E171" s="19"/>
+      <c r="E171" s="24"/>
     </row>
     <row r="172" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172">
         <f t="shared" si="5"/>
         <v>22016</v>
       </c>
-      <c r="C172" s="52" t="str">
+      <c r="C172" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5600</v>
       </c>
-      <c r="E172" s="19"/>
+      <c r="E172" s="24"/>
     </row>
     <row r="173" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173">
         <f t="shared" si="5"/>
         <v>21760</v>
       </c>
-      <c r="C173" s="52" t="str">
+      <c r="C173" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5500</v>
       </c>
-      <c r="E173" s="19"/>
+      <c r="E173" s="24"/>
     </row>
     <row r="174" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174">
         <f t="shared" si="5"/>
         <v>21504</v>
       </c>
-      <c r="C174" s="52" t="str">
+      <c r="C174" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5400</v>
       </c>
-      <c r="E174" s="19"/>
+      <c r="E174" s="24"/>
     </row>
     <row r="175" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175">
         <f t="shared" si="5"/>
         <v>21248</v>
       </c>
-      <c r="C175" s="52" t="str">
+      <c r="C175" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5300</v>
       </c>
-      <c r="E175" s="19"/>
+      <c r="E175" s="24"/>
     </row>
     <row r="176" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176">
         <f t="shared" si="5"/>
         <v>20992</v>
       </c>
-      <c r="C176" s="52" t="str">
+      <c r="C176" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5200</v>
       </c>
-      <c r="E176" s="19"/>
+      <c r="E176" s="24"/>
     </row>
     <row r="177" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177">
         <f t="shared" si="5"/>
         <v>20736</v>
       </c>
-      <c r="C177" s="52" t="str">
+      <c r="C177" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5100</v>
       </c>
-      <c r="E177" s="19"/>
+      <c r="E177" s="24"/>
     </row>
     <row r="178" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178">
         <f t="shared" si="5"/>
         <v>20480</v>
       </c>
-      <c r="C178" s="52" t="str">
+      <c r="C178" s="56" t="str">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
-      <c r="E178" s="19"/>
+      <c r="E178" s="24"/>
     </row>
     <row r="179" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179">
         <f t="shared" si="5"/>
         <v>20224</v>
       </c>
-      <c r="C179" s="52" t="str">
+      <c r="C179" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4F00</v>
       </c>
-      <c r="E179" s="19"/>
+      <c r="E179" s="24"/>
     </row>
     <row r="180" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180">
         <f t="shared" si="5"/>
         <v>19968</v>
       </c>
-      <c r="C180" s="52" t="str">
+      <c r="C180" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4E00</v>
       </c>
-      <c r="E180" s="19"/>
+      <c r="E180" s="24"/>
     </row>
     <row r="181" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181">
         <f t="shared" si="5"/>
         <v>19712</v>
       </c>
-      <c r="C181" s="52" t="str">
+      <c r="C181" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4D00</v>
       </c>
-      <c r="E181" s="19"/>
+      <c r="E181" s="24"/>
     </row>
     <row r="182" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182">
         <f t="shared" si="5"/>
         <v>19456</v>
       </c>
-      <c r="C182" s="52" t="str">
+      <c r="C182" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4C00</v>
       </c>
-      <c r="E182" s="19"/>
+      <c r="E182" s="24" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="183" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183">
         <f t="shared" si="5"/>
         <v>19200</v>
       </c>
-      <c r="C183" s="52" t="str">
+      <c r="C183" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4B00</v>
       </c>
-      <c r="E183" s="19"/>
+      <c r="E183" s="65"/>
     </row>
     <row r="184" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184">
         <f t="shared" si="5"/>
         <v>18944</v>
       </c>
-      <c r="C184" s="52" t="str">
+      <c r="C184" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4A00</v>
       </c>
-      <c r="E184" s="19"/>
+      <c r="E184" s="64"/>
     </row>
     <row r="185" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185">
         <f t="shared" si="5"/>
         <v>18688</v>
       </c>
-      <c r="C185" s="52" t="str">
+      <c r="C185" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4900</v>
       </c>
-      <c r="E185" s="19"/>
+      <c r="E185" s="64"/>
     </row>
     <row r="186" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186">
         <f t="shared" si="5"/>
         <v>18432</v>
       </c>
-      <c r="C186" s="52" t="str">
+      <c r="C186" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4800</v>
       </c>
-      <c r="E186" s="19"/>
+      <c r="E186" s="66" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="187" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187">
         <f t="shared" si="5"/>
         <v>18176</v>
       </c>
-      <c r="C187" s="52" t="str">
+      <c r="C187" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4700</v>
       </c>
-      <c r="E187" s="19"/>
+      <c r="E187" s="21"/>
     </row>
     <row r="188" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188">
         <f t="shared" si="5"/>
         <v>17920</v>
       </c>
-      <c r="C188" s="52" t="str">
+      <c r="C188" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4600</v>
       </c>
-      <c r="E188" s="19"/>
+      <c r="E188" s="22"/>
     </row>
     <row r="189" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189">
         <f t="shared" si="5"/>
         <v>17664</v>
       </c>
-      <c r="C189" s="52" t="str">
+      <c r="C189" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4500</v>
       </c>
-      <c r="E189" s="19"/>
+      <c r="E189" s="22"/>
     </row>
     <row r="190" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190">
         <f t="shared" si="5"/>
         <v>17408</v>
       </c>
-      <c r="C190" s="52" t="str">
+      <c r="C190" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4400</v>
       </c>
-      <c r="E190" s="19"/>
+      <c r="E190" s="22"/>
     </row>
     <row r="191" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191">
         <f t="shared" si="5"/>
         <v>17152</v>
       </c>
-      <c r="C191" s="52" t="str">
+      <c r="C191" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4300</v>
       </c>
-      <c r="E191" s="19"/>
+      <c r="E191" s="22"/>
     </row>
     <row r="192" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192">
         <f t="shared" si="5"/>
         <v>16896</v>
       </c>
-      <c r="C192" s="52" t="str">
+      <c r="C192" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4200</v>
       </c>
-      <c r="E192" s="19"/>
-    </row>
-    <row r="193" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E192" s="22"/>
+    </row>
+    <row r="193" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193">
         <f t="shared" si="5"/>
         <v>16640</v>
       </c>
-      <c r="C193" s="52" t="str">
+      <c r="C193" s="56" t="str">
         <f t="shared" si="4"/>
         <v>4100</v>
       </c>
-      <c r="E193" s="19"/>
-    </row>
-    <row r="194" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="54" t="s">
+      <c r="E193" s="22"/>
+    </row>
+    <row r="194" spans="1:7" s="62" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="62">
         <f t="shared" si="5"/>
         <v>16384</v>
       </c>
-      <c r="C194" s="53" t="str">
+      <c r="C194" s="57" t="str">
         <f t="shared" si="4"/>
         <v>4000</v>
       </c>
-      <c r="E194" s="19"/>
-    </row>
-    <row r="195" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="54" t="s">
+      <c r="E194" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G194" s="63"/>
+    </row>
+    <row r="195" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="58" t="s">
         <v>36</v>
       </c>
       <c r="B195">
         <f t="shared" si="5"/>
         <v>16128</v>
       </c>
-      <c r="C195" s="48" t="str">
+      <c r="C195" s="53" t="str">
         <f t="shared" ref="C195:C258" si="6">DEC2HEX(B195)</f>
         <v>3F00</v>
       </c>
       <c r="E195" s="19"/>
     </row>
-    <row r="196" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196">
         <f>B195-256</f>
         <v>15872</v>
       </c>
-      <c r="C196" s="49" t="str">
+      <c r="C196" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3E00</v>
       </c>
       <c r="E196" s="19"/>
     </row>
-    <row r="197" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197">
         <f>B196-256</f>
         <v>15616</v>
       </c>
-      <c r="C197" s="49" t="str">
+      <c r="C197" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3D00</v>
       </c>
       <c r="E197" s="19"/>
     </row>
-    <row r="198" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198">
         <f>B197-256</f>
         <v>15360</v>
       </c>
-      <c r="C198" s="49" t="str">
+      <c r="C198" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3C00</v>
       </c>
       <c r="E198" s="19"/>
     </row>
-    <row r="199" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199">
         <f>B198-256</f>
         <v>15104</v>
       </c>
-      <c r="C199" s="49" t="str">
+      <c r="C199" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3B00</v>
       </c>
       <c r="E199" s="19"/>
     </row>
-    <row r="200" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200">
         <f>B199-256</f>
         <v>14848</v>
       </c>
-      <c r="C200" s="49" t="str">
+      <c r="C200" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3A00</v>
       </c>
       <c r="E200" s="19"/>
     </row>
-    <row r="201" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201">
         <f>B200-256</f>
         <v>14592</v>
       </c>
-      <c r="C201" s="49" t="str">
+      <c r="C201" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3900</v>
       </c>
       <c r="E201" s="19"/>
     </row>
-    <row r="202" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202">
         <f>B201-256</f>
         <v>14336</v>
       </c>
-      <c r="C202" s="49" t="str">
+      <c r="C202" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3800</v>
       </c>
       <c r="E202" s="19"/>
     </row>
-    <row r="203" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203">
         <f>B202-256</f>
         <v>14080</v>
       </c>
-      <c r="C203" s="49" t="str">
+      <c r="C203" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3700</v>
       </c>
       <c r="E203" s="19"/>
     </row>
-    <row r="204" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204">
         <f>B203-256</f>
         <v>13824</v>
       </c>
-      <c r="C204" s="49" t="str">
+      <c r="C204" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3600</v>
       </c>
       <c r="E204" s="19"/>
     </row>
-    <row r="205" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205">
         <f>B204-256</f>
         <v>13568</v>
       </c>
-      <c r="C205" s="49" t="str">
+      <c r="C205" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3500</v>
       </c>
       <c r="E205" s="19"/>
     </row>
-    <row r="206" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206">
         <f>B205-256</f>
         <v>13312</v>
       </c>
-      <c r="C206" s="49" t="str">
+      <c r="C206" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3400</v>
       </c>
       <c r="E206" s="19"/>
     </row>
-    <row r="207" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207">
         <f>B206-256</f>
         <v>13056</v>
       </c>
-      <c r="C207" s="49" t="str">
+      <c r="C207" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3300</v>
       </c>
       <c r="E207" s="19"/>
     </row>
-    <row r="208" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208">
         <f>B207-256</f>
         <v>12800</v>
       </c>
-      <c r="C208" s="49" t="str">
+      <c r="C208" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3200</v>
       </c>
@@ -3216,7 +3276,7 @@
         <f>B208-256</f>
         <v>12544</v>
       </c>
-      <c r="C209" s="49" t="str">
+      <c r="C209" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3100</v>
       </c>
@@ -3230,7 +3290,7 @@
         <f>B209-256</f>
         <v>12288</v>
       </c>
-      <c r="C210" s="49" t="str">
+      <c r="C210" s="53" t="str">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
@@ -3246,7 +3306,7 @@
         <f>B210-256</f>
         <v>12032</v>
       </c>
-      <c r="C211" s="49" t="str">
+      <c r="C211" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2F00</v>
       </c>
@@ -3259,7 +3319,7 @@
         <f>B211-256</f>
         <v>11776</v>
       </c>
-      <c r="C212" s="49" t="str">
+      <c r="C212" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2E00</v>
       </c>
@@ -3275,7 +3335,7 @@
         <f>B212-256</f>
         <v>11520</v>
       </c>
-      <c r="C213" s="49" t="str">
+      <c r="C213" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2D00</v>
       </c>
@@ -3288,11 +3348,11 @@
         <f>B213-256</f>
         <v>11264</v>
       </c>
-      <c r="C214" s="49" t="str">
+      <c r="C214" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2C00</v>
       </c>
-      <c r="E214" s="40"/>
+      <c r="E214" s="44"/>
       <c r="M214" s="5" t="s">
         <v>10</v>
       </c>
@@ -3302,11 +3362,11 @@
         <f>B214-256</f>
         <v>11008</v>
       </c>
-      <c r="C215" s="49" t="str">
+      <c r="C215" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2B00</v>
       </c>
-      <c r="E215" s="41"/>
+      <c r="E215" s="45"/>
       <c r="M215" s="5" t="s">
         <v>11</v>
       </c>
@@ -3316,120 +3376,120 @@
         <f>B215-256</f>
         <v>10752</v>
       </c>
-      <c r="C216" s="49" t="str">
+      <c r="C216" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2A00</v>
       </c>
-      <c r="E216" s="41"/>
+      <c r="E216" s="45"/>
       <c r="M216" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="55"/>
+      <c r="A217" s="59"/>
       <c r="B217">
         <f>B216-256</f>
         <v>10496</v>
       </c>
-      <c r="C217" s="49" t="str">
+      <c r="C217" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2900</v>
       </c>
-      <c r="E217" s="41"/>
+      <c r="E217" s="45"/>
       <c r="M217" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A218" s="55"/>
+      <c r="A218" s="59"/>
       <c r="B218">
         <f>B217-256</f>
         <v>10240</v>
       </c>
-      <c r="C218" s="49" t="str">
+      <c r="C218" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2800</v>
       </c>
-      <c r="E218" s="41"/>
+      <c r="E218" s="45"/>
       <c r="M218" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A219" s="55"/>
+      <c r="A219" s="59"/>
       <c r="B219">
         <f>B218-256</f>
         <v>9984</v>
       </c>
-      <c r="C219" s="49" t="str">
+      <c r="C219" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2700</v>
       </c>
-      <c r="E219" s="41"/>
+      <c r="E219" s="45"/>
       <c r="M219" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="55"/>
+      <c r="A220" s="59"/>
       <c r="B220">
         <f>B219-256</f>
         <v>9728</v>
       </c>
-      <c r="C220" s="49" t="str">
+      <c r="C220" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2600</v>
       </c>
-      <c r="E220" s="41"/>
+      <c r="E220" s="45"/>
       <c r="M220" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="221" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A221" s="55"/>
+      <c r="A221" s="59"/>
       <c r="B221">
         <f>B220-256</f>
         <v>9472</v>
       </c>
-      <c r="C221" s="49" t="str">
+      <c r="C221" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2500</v>
       </c>
-      <c r="E221" s="41"/>
+      <c r="E221" s="45"/>
     </row>
     <row r="222" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A222" s="55"/>
+      <c r="A222" s="59"/>
       <c r="B222">
         <f>B221-256</f>
         <v>9216</v>
       </c>
-      <c r="C222" s="49" t="str">
+      <c r="C222" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2400</v>
       </c>
-      <c r="E222" s="41"/>
+      <c r="E222" s="45"/>
     </row>
     <row r="223" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223">
         <f>B222-256</f>
         <v>8960</v>
       </c>
-      <c r="C223" s="49" t="str">
+      <c r="C223" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2300</v>
       </c>
-      <c r="E223" s="41"/>
+      <c r="E223" s="45"/>
     </row>
     <row r="224" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224">
         <f>B223-256</f>
         <v>8704</v>
       </c>
-      <c r="C224" s="49" t="str">
+      <c r="C224" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2200</v>
       </c>
-      <c r="E224" s="41" t="s">
+      <c r="E224" s="45" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3438,216 +3498,216 @@
         <f>B224-256</f>
         <v>8448</v>
       </c>
-      <c r="C225" s="49" t="str">
+      <c r="C225" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2100</v>
       </c>
-      <c r="E225" s="41"/>
+      <c r="E225" s="45"/>
     </row>
     <row r="226" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226">
         <f>B225-256</f>
         <v>8192</v>
       </c>
-      <c r="C226" s="49" t="str">
+      <c r="C226" s="53" t="str">
         <f t="shared" si="6"/>
         <v>2000</v>
       </c>
-      <c r="E226" s="41"/>
+      <c r="E226" s="45"/>
     </row>
     <row r="227" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227">
         <f>B226-256</f>
         <v>7936</v>
       </c>
-      <c r="C227" s="49" t="str">
+      <c r="C227" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1F00</v>
       </c>
-      <c r="E227" s="41"/>
-      <c r="G227" s="34"/>
+      <c r="E227" s="45"/>
+      <c r="G227" s="38"/>
     </row>
     <row r="228" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228">
         <f>B227-256</f>
         <v>7680</v>
       </c>
-      <c r="C228" s="49" t="str">
+      <c r="C228" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1E00</v>
       </c>
-      <c r="E228" s="41"/>
-      <c r="G228" s="35"/>
+      <c r="E228" s="45"/>
+      <c r="G228" s="39"/>
     </row>
     <row r="229" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229">
         <f>B228-256</f>
         <v>7424</v>
       </c>
-      <c r="C229" s="49" t="str">
+      <c r="C229" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1D00</v>
       </c>
-      <c r="E229" s="41"/>
-      <c r="G229" s="35"/>
+      <c r="E229" s="45"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B230">
         <f>B229-256</f>
         <v>7168</v>
       </c>
-      <c r="C230" s="49" t="str">
+      <c r="C230" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1C00</v>
       </c>
-      <c r="E230" s="41"/>
-      <c r="G230" s="35"/>
+      <c r="E230" s="45"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B231">
         <f>B230-256</f>
         <v>6912</v>
       </c>
-      <c r="C231" s="49" t="str">
+      <c r="C231" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1B00</v>
       </c>
-      <c r="E231" s="41" t="s">
+      <c r="E231" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G231" s="35"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B232">
         <f>B231-256</f>
         <v>6656</v>
       </c>
-      <c r="C232" s="49" t="str">
+      <c r="C232" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1A00</v>
       </c>
-      <c r="E232" s="37"/>
-      <c r="G232" s="35"/>
+      <c r="E232" s="41"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B233">
         <f>B232-256</f>
         <v>6400</v>
       </c>
-      <c r="C233" s="49" t="str">
+      <c r="C233" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1900</v>
       </c>
-      <c r="E233" s="38"/>
-      <c r="G233" s="35"/>
+      <c r="E233" s="42"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234">
         <f>B233-256</f>
         <v>6144</v>
       </c>
-      <c r="C234" s="49" t="str">
+      <c r="C234" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1800</v>
       </c>
-      <c r="E234" s="38"/>
-      <c r="G234" s="35"/>
+      <c r="E234" s="42"/>
+      <c r="G234" s="39"/>
     </row>
     <row r="235" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B235">
         <f>B234-256</f>
         <v>5888</v>
       </c>
-      <c r="C235" s="49" t="str">
+      <c r="C235" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1700</v>
       </c>
-      <c r="E235" s="38"/>
-      <c r="G235" s="35"/>
+      <c r="E235" s="42"/>
+      <c r="G235" s="39"/>
     </row>
     <row r="236" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B236">
         <f>B235-256</f>
         <v>5632</v>
       </c>
-      <c r="C236" s="49" t="str">
+      <c r="C236" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1600</v>
       </c>
-      <c r="E236" s="38"/>
-      <c r="G236" s="35"/>
+      <c r="E236" s="42"/>
+      <c r="G236" s="39"/>
     </row>
     <row r="237" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B237">
         <f>B236-256</f>
         <v>5376</v>
       </c>
-      <c r="C237" s="49" t="str">
+      <c r="C237" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
-      <c r="E237" s="38"/>
-      <c r="G237" s="35"/>
+      <c r="E237" s="42"/>
+      <c r="G237" s="39"/>
     </row>
     <row r="238" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238">
         <f>B237-256</f>
         <v>5120</v>
       </c>
-      <c r="C238" s="49" t="str">
+      <c r="C238" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1400</v>
       </c>
-      <c r="E238" s="38"/>
-      <c r="G238" s="35"/>
+      <c r="E238" s="42"/>
+      <c r="G238" s="39"/>
     </row>
     <row r="239" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B239">
         <f>B238-256</f>
         <v>4864</v>
       </c>
-      <c r="C239" s="49" t="str">
+      <c r="C239" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1300</v>
       </c>
-      <c r="E239" s="38"/>
-      <c r="G239" s="35"/>
+      <c r="E239" s="42"/>
+      <c r="G239" s="39"/>
     </row>
     <row r="240" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240">
         <f>B239-256</f>
         <v>4608</v>
       </c>
-      <c r="C240" s="49" t="str">
+      <c r="C240" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1200</v>
       </c>
-      <c r="E240" s="38"/>
-      <c r="G240" s="35"/>
+      <c r="E240" s="42"/>
+      <c r="G240" s="39"/>
     </row>
     <row r="241" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B241">
         <f>B240-256</f>
         <v>4352</v>
       </c>
-      <c r="C241" s="49" t="str">
+      <c r="C241" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1100</v>
       </c>
-      <c r="E241" s="38"/>
-      <c r="G241" s="35"/>
+      <c r="E241" s="42"/>
+      <c r="G241" s="39"/>
     </row>
     <row r="242" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242">
         <f>B241-256</f>
         <v>4096</v>
       </c>
-      <c r="C242" s="49" t="str">
+      <c r="C242" s="53" t="str">
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="E242" s="38"/>
-      <c r="G242" s="36" t="s">
+      <c r="E242" s="42"/>
+      <c r="G242" s="40" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3656,88 +3716,88 @@
         <f>B242-256</f>
         <v>3840</v>
       </c>
-      <c r="C243" s="49" t="str">
+      <c r="C243" s="53" t="str">
         <f t="shared" si="6"/>
         <v>F00</v>
       </c>
-      <c r="E243" s="38"/>
+      <c r="E243" s="42"/>
     </row>
     <row r="244" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244">
         <f>B243-256</f>
         <v>3584</v>
       </c>
-      <c r="C244" s="49" t="str">
+      <c r="C244" s="53" t="str">
         <f t="shared" si="6"/>
         <v>E00</v>
       </c>
-      <c r="E244" s="38"/>
+      <c r="E244" s="42"/>
     </row>
     <row r="245" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B245">
         <f>B244-256</f>
         <v>3328</v>
       </c>
-      <c r="C245" s="49" t="str">
+      <c r="C245" s="53" t="str">
         <f t="shared" si="6"/>
         <v>D00</v>
       </c>
-      <c r="E245" s="38"/>
+      <c r="E245" s="42"/>
     </row>
     <row r="246" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B246">
         <f>B245-256</f>
         <v>3072</v>
       </c>
-      <c r="C246" s="49" t="str">
+      <c r="C246" s="53" t="str">
         <f t="shared" si="6"/>
         <v>C00</v>
       </c>
-      <c r="E246" s="38"/>
+      <c r="E246" s="42"/>
     </row>
     <row r="247" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247">
         <f>B246-256</f>
         <v>2816</v>
       </c>
-      <c r="C247" s="49" t="str">
+      <c r="C247" s="53" t="str">
         <f t="shared" si="6"/>
         <v>B00</v>
       </c>
-      <c r="E247" s="38"/>
+      <c r="E247" s="42"/>
     </row>
     <row r="248" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B248">
         <f>B247-256</f>
         <v>2560</v>
       </c>
-      <c r="C248" s="49" t="str">
+      <c r="C248" s="53" t="str">
         <f t="shared" si="6"/>
         <v>A00</v>
       </c>
-      <c r="E248" s="38"/>
+      <c r="E248" s="42"/>
     </row>
     <row r="249" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B249">
         <f>B248-256</f>
         <v>2304</v>
       </c>
-      <c r="C249" s="49" t="str">
+      <c r="C249" s="53" t="str">
         <f t="shared" si="6"/>
         <v>900</v>
       </c>
-      <c r="E249" s="38"/>
+      <c r="E249" s="42"/>
     </row>
     <row r="250" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B250">
         <f>B249-256</f>
         <v>2048</v>
       </c>
-      <c r="C250" s="49" t="str">
+      <c r="C250" s="53" t="str">
         <f t="shared" si="6"/>
         <v>800</v>
       </c>
-      <c r="E250" s="39" t="s">
+      <c r="E250" s="43" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3746,7 +3806,7 @@
         <f>B250-256</f>
         <v>1792</v>
       </c>
-      <c r="C251" s="49" t="str">
+      <c r="C251" s="53" t="str">
         <f t="shared" si="6"/>
         <v>700</v>
       </c>
@@ -3757,7 +3817,7 @@
         <f>B251-256</f>
         <v>1536</v>
       </c>
-      <c r="C252" s="49" t="str">
+      <c r="C252" s="53" t="str">
         <f t="shared" si="6"/>
         <v>600</v>
       </c>
@@ -3770,7 +3830,7 @@
         <f>B252-256</f>
         <v>1280</v>
       </c>
-      <c r="C253" s="49" t="str">
+      <c r="C253" s="53" t="str">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
@@ -3783,7 +3843,7 @@
         <f>B253-256</f>
         <v>1024</v>
       </c>
-      <c r="C254" s="49" t="str">
+      <c r="C254" s="53" t="str">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
@@ -3794,7 +3854,7 @@
         <f>B254-256</f>
         <v>768</v>
       </c>
-      <c r="C255" s="49" t="str">
+      <c r="C255" s="53" t="str">
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
@@ -3807,7 +3867,7 @@
         <f>B255-256</f>
         <v>512</v>
       </c>
-      <c r="C256" s="49" t="str">
+      <c r="C256" s="53" t="str">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
@@ -3820,7 +3880,7 @@
         <f>B256-256</f>
         <v>256</v>
       </c>
-      <c r="C257" s="49" t="str">
+      <c r="C257" s="53" t="str">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
@@ -3829,14 +3889,14 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="54" t="s">
+      <c r="A258" s="58" t="s">
         <v>36</v>
       </c>
       <c r="B258">
         <f>B257-256</f>
         <v>0</v>
       </c>
-      <c r="C258" s="50" t="str">
+      <c r="C258" s="54" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added NewEntities Queue and Torpedos
</commit_message>
<xml_diff>
--- a/Docs/Vortex Memory Map.xlsx
+++ b/Docs/Vortex Memory Map.xlsx
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E184" sqref="E184"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J166" sqref="J166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="E152" s="25"/>
     </row>
-    <row r="153" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="58"/>
       <c r="B153">
         <f t="shared" si="5"/>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="E153" s="25"/>
     </row>
-    <row r="154" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="58"/>
       <c r="B154">
         <f t="shared" si="5"/>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="E154" s="25"/>
     </row>
-    <row r="155" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155">
         <f t="shared" si="5"/>
         <v>26368</v>
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E155" s="25"/>
     </row>
-    <row r="156" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156">
         <f t="shared" si="5"/>
         <v>26112</v>
@@ -2703,7 +2703,7 @@
       </c>
       <c r="E156" s="25"/>
     </row>
-    <row r="157" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157">
         <f t="shared" si="5"/>
         <v>25856</v>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="E157" s="25"/>
     </row>
-    <row r="158" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158">
         <f t="shared" si="5"/>
         <v>25600</v>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="E158" s="25"/>
     </row>
-    <row r="159" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159">
         <f t="shared" si="5"/>
         <v>25344</v>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="E159" s="25"/>
     </row>
-    <row r="160" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160">
         <f t="shared" si="5"/>
         <v>25088</v>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="E160" s="25"/>
     </row>
-    <row r="161" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161">
         <f t="shared" si="5"/>
         <v>24832</v>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="E161" s="25"/>
     </row>
-    <row r="162" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162">
         <f t="shared" si="5"/>
         <v>24576</v>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="E162" s="25"/>
     </row>
-    <row r="163" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163">
         <f t="shared" si="5"/>
         <v>24320</v>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="E163" s="25"/>
     </row>
-    <row r="164" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164">
         <f t="shared" si="5"/>
         <v>24064</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="E164" s="25"/>
     </row>
-    <row r="165" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165">
         <f t="shared" si="5"/>
         <v>23808</v>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E165" s="25"/>
     </row>
-    <row r="166" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166">
         <f t="shared" si="5"/>
         <v>23552</v>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="E166" s="25"/>
     </row>
-    <row r="167" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167">
         <f t="shared" si="5"/>
         <v>23296</v>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="E167" s="25"/>
     </row>
-    <row r="168" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168">
         <f t="shared" si="5"/>
         <v>23040</v>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="E168" s="25"/>
     </row>
-    <row r="169" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169">
         <f t="shared" si="5"/>
         <v>22784</v>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="E169" s="25"/>
     </row>
-    <row r="170" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170">
         <f t="shared" si="5"/>
         <v>22528</v>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="E170" s="25"/>
     </row>
-    <row r="171" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171">
         <f t="shared" si="5"/>
         <v>22272</v>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="E171" s="25"/>
     </row>
-    <row r="172" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172">
         <f t="shared" si="5"/>
         <v>22016</v>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="E172" s="25"/>
     </row>
-    <row r="173" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173">
         <f t="shared" si="5"/>
         <v>21760</v>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="E173" s="25"/>
     </row>
-    <row r="174" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174">
         <f t="shared" si="5"/>
         <v>21504</v>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="E174" s="25"/>
     </row>
-    <row r="175" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175">
         <f t="shared" si="5"/>
         <v>21248</v>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="E175" s="25"/>
     </row>
-    <row r="176" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176">
         <f t="shared" si="5"/>
         <v>20992</v>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="E176" s="25"/>
     </row>
-    <row r="177" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177">
         <f t="shared" si="5"/>
         <v>20736</v>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="E177" s="25"/>
     </row>
-    <row r="178" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178">
         <f t="shared" si="5"/>
         <v>20480</v>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="E178" s="25"/>
     </row>
-    <row r="179" spans="2:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179">
         <f t="shared" si="5"/>
         <v>20224</v>

</xml_diff>

<commit_message>
New Sprites and Music
</commit_message>
<xml_diff>
--- a/Docs/Vortex Memory Map.xlsx
+++ b/Docs/Vortex Memory Map.xlsx
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Address</t>
-  </si>
-  <si>
-    <t>Free RAM</t>
   </si>
   <si>
     <t>Colour RAM</t>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>4BF8 Sprite Pointers</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -495,7 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,6 +535,8 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,13 +850,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J166" sqref="J166"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="57" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="56" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="5.140625" customWidth="1"/>
@@ -865,439 +866,439 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="C1" s="59" t="s">
+      <c r="A1" s="56"/>
+      <c r="C1" s="58" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="48"/>
+        <v>33</v>
+      </c>
+      <c r="F1" s="47"/>
       <c r="G1" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>37</v>
+      <c r="A2" s="56" t="s">
+        <v>36</v>
       </c>
       <c r="B2">
         <v>65536</v>
       </c>
-      <c r="C2" s="54" t="str">
+      <c r="C2" s="53" t="str">
         <f>DEC2HEX(B2-1)</f>
         <v>FFFF</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="49"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>B2-256</f>
         <v>65280</v>
       </c>
-      <c r="C3" s="55" t="str">
+      <c r="C3" s="54" t="str">
         <f t="shared" ref="C3:C66" si="0">DEC2HEX(B3)</f>
         <v>FF00</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="49"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" ref="B4:B67" si="1">B3-256</f>
         <v>65024</v>
       </c>
-      <c r="C4" s="55" t="str">
+      <c r="C4" s="54" t="str">
         <f t="shared" si="0"/>
         <v>FE00</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="49"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" si="1"/>
         <v>64768</v>
       </c>
-      <c r="C5" s="55" t="str">
+      <c r="C5" s="54" t="str">
         <f t="shared" si="0"/>
         <v>FD00</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="49"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="1"/>
         <v>64512</v>
       </c>
-      <c r="C6" s="55" t="str">
+      <c r="C6" s="54" t="str">
         <f t="shared" si="0"/>
         <v>FC00</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="49"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>64256</v>
       </c>
-      <c r="C7" s="55" t="str">
+      <c r="C7" s="54" t="str">
         <f t="shared" si="0"/>
         <v>FB00</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="49"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="1"/>
         <v>64000</v>
       </c>
-      <c r="C8" s="55" t="str">
+      <c r="C8" s="54" t="str">
         <f t="shared" si="0"/>
         <v>FA00</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="49"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>63744</v>
       </c>
-      <c r="C9" s="55" t="str">
+      <c r="C9" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F900</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="49"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>63488</v>
       </c>
-      <c r="C10" s="55" t="str">
+      <c r="C10" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F800</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="49"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>63232</v>
       </c>
-      <c r="C11" s="55" t="str">
+      <c r="C11" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F700</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="49"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>62976</v>
       </c>
-      <c r="C12" s="55" t="str">
+      <c r="C12" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F600</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="49"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>62720</v>
       </c>
-      <c r="C13" s="55" t="str">
+      <c r="C13" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F500</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="49"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>62464</v>
       </c>
-      <c r="C14" s="55" t="str">
+      <c r="C14" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F400</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="49"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>62208</v>
       </c>
-      <c r="C15" s="55" t="str">
+      <c r="C15" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F300</v>
       </c>
-      <c r="E15" s="46"/>
-      <c r="F15" s="49"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>61952</v>
       </c>
-      <c r="C16" s="55" t="str">
+      <c r="C16" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F200</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="49"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="1"/>
         <v>61696</v>
       </c>
-      <c r="C17" s="55" t="str">
+      <c r="C17" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F100</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="49"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="1"/>
         <v>61440</v>
       </c>
-      <c r="C18" s="55" t="str">
+      <c r="C18" s="54" t="str">
         <f t="shared" si="0"/>
         <v>F000</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="49"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>61184</v>
       </c>
-      <c r="C19" s="55" t="str">
+      <c r="C19" s="54" t="str">
         <f t="shared" si="0"/>
         <v>EF00</v>
       </c>
-      <c r="E19" s="46"/>
-      <c r="F19" s="49"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="48"/>
     </row>
     <row r="20" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>60928</v>
       </c>
-      <c r="C20" s="55" t="str">
+      <c r="C20" s="54" t="str">
         <f t="shared" si="0"/>
         <v>EE00</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="49"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="48"/>
     </row>
     <row r="21" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="58"/>
+      <c r="A21" s="57"/>
       <c r="B21">
         <f t="shared" si="1"/>
         <v>60672</v>
       </c>
-      <c r="C21" s="55" t="str">
+      <c r="C21" s="54" t="str">
         <f t="shared" si="0"/>
         <v>ED00</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="49"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="48"/>
     </row>
     <row r="22" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="58"/>
+      <c r="A22" s="57"/>
       <c r="B22">
         <f t="shared" si="1"/>
         <v>60416</v>
       </c>
-      <c r="C22" s="55" t="str">
+      <c r="C22" s="54" t="str">
         <f t="shared" si="0"/>
         <v>EC00</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="49"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="48"/>
     </row>
     <row r="23" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="58"/>
+      <c r="A23" s="57"/>
       <c r="B23">
         <f t="shared" si="1"/>
         <v>60160</v>
       </c>
-      <c r="C23" s="55" t="str">
+      <c r="C23" s="54" t="str">
         <f t="shared" si="0"/>
         <v>EB00</v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="49"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="48"/>
     </row>
     <row r="24" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="58"/>
+      <c r="A24" s="57"/>
       <c r="B24">
         <f t="shared" si="1"/>
         <v>59904</v>
       </c>
-      <c r="C24" s="55" t="str">
+      <c r="C24" s="54" t="str">
         <f t="shared" si="0"/>
         <v>EA00</v>
       </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="49"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="48"/>
     </row>
     <row r="25" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="58"/>
+      <c r="A25" s="57"/>
       <c r="B25">
         <f t="shared" si="1"/>
         <v>59648</v>
       </c>
-      <c r="C25" s="55" t="str">
+      <c r="C25" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E900</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="49"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="48"/>
     </row>
     <row r="26" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="58"/>
+      <c r="A26" s="57"/>
       <c r="B26">
         <f t="shared" si="1"/>
         <v>59392</v>
       </c>
-      <c r="C26" s="55" t="str">
+      <c r="C26" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E800</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="49"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="1"/>
         <v>59136</v>
       </c>
-      <c r="C27" s="55" t="str">
+      <c r="C27" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E700</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="49"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="48"/>
     </row>
     <row r="28" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="1"/>
         <v>58880</v>
       </c>
-      <c r="C28" s="55" t="str">
+      <c r="C28" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E600</v>
       </c>
-      <c r="E28" s="46"/>
-      <c r="F28" s="49"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="48"/>
     </row>
     <row r="29" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="1"/>
         <v>58624</v>
       </c>
-      <c r="C29" s="55" t="str">
+      <c r="C29" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E500</v>
       </c>
-      <c r="E29" s="46"/>
-      <c r="F29" s="49"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="48"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="1"/>
         <v>58368</v>
       </c>
-      <c r="C30" s="55" t="str">
+      <c r="C30" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E400</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="F30" s="49"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="48"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="1"/>
         <v>58112</v>
       </c>
-      <c r="C31" s="55" t="str">
+      <c r="C31" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E300</v>
       </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="49"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="48"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="1"/>
         <v>57856</v>
       </c>
-      <c r="C32" s="55" t="str">
+      <c r="C32" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E200</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="49"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="1"/>
         <v>57600</v>
       </c>
-      <c r="C33" s="55" t="str">
+      <c r="C33" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E100</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="F33" s="49"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="48"/>
     </row>
     <row r="34" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C34" s="55" t="str">
+      <c r="C34" s="54" t="str">
         <f t="shared" si="0"/>
         <v>E000</v>
       </c>
-      <c r="E34" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="49"/>
+      <c r="E34" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="1"/>
         <v>57088</v>
       </c>
-      <c r="C35" s="55" t="str">
+      <c r="C35" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DF00</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="50"/>
+        <v>31</v>
+      </c>
+      <c r="F35" s="49"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1305,12 +1306,12 @@
         <f t="shared" si="1"/>
         <v>56832</v>
       </c>
-      <c r="C36" s="55" t="str">
+      <c r="C36" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DE00</v>
       </c>
       <c r="E36" s="29"/>
-      <c r="F36" s="50"/>
+      <c r="F36" s="49"/>
       <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1318,12 +1319,12 @@
         <f t="shared" si="1"/>
         <v>56576</v>
       </c>
-      <c r="C37" s="55" t="str">
+      <c r="C37" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DD00</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" s="13"/>
     </row>
@@ -1332,12 +1333,12 @@
         <f t="shared" si="1"/>
         <v>56320</v>
       </c>
-      <c r="C38" s="55" t="str">
+      <c r="C38" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DC00</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G38" s="13"/>
     </row>
@@ -1346,7 +1347,7 @@
         <f t="shared" si="1"/>
         <v>56064</v>
       </c>
-      <c r="C39" s="55" t="str">
+      <c r="C39" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DB00</v>
       </c>
@@ -1358,7 +1359,7 @@
         <f t="shared" si="1"/>
         <v>55808</v>
       </c>
-      <c r="C40" s="55" t="str">
+      <c r="C40" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DA00</v>
       </c>
@@ -1370,7 +1371,7 @@
         <f t="shared" si="1"/>
         <v>55552</v>
       </c>
-      <c r="C41" s="55" t="str">
+      <c r="C41" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D900</v>
       </c>
@@ -1382,12 +1383,12 @@
         <f t="shared" si="1"/>
         <v>55296</v>
       </c>
-      <c r="C42" s="55" t="str">
+      <c r="C42" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D800</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G42" s="13"/>
     </row>
@@ -1396,7 +1397,7 @@
         <f t="shared" si="1"/>
         <v>55040</v>
       </c>
-      <c r="C43" s="55" t="str">
+      <c r="C43" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D700</v>
       </c>
@@ -1408,7 +1409,7 @@
         <f t="shared" si="1"/>
         <v>54784</v>
       </c>
-      <c r="C44" s="55" t="str">
+      <c r="C44" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D600</v>
       </c>
@@ -1420,7 +1421,7 @@
         <f t="shared" si="1"/>
         <v>54528</v>
       </c>
-      <c r="C45" s="55" t="str">
+      <c r="C45" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D500</v>
       </c>
@@ -1432,12 +1433,12 @@
         <f t="shared" si="1"/>
         <v>54272</v>
       </c>
-      <c r="C46" s="55" t="str">
+      <c r="C46" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D400</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G46" s="13"/>
     </row>
@@ -1446,7 +1447,7 @@
         <f t="shared" si="1"/>
         <v>54016</v>
       </c>
-      <c r="C47" s="55" t="str">
+      <c r="C47" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D300</v>
       </c>
@@ -1458,7 +1459,7 @@
         <f t="shared" si="1"/>
         <v>53760</v>
       </c>
-      <c r="C48" s="55" t="str">
+      <c r="C48" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D200</v>
       </c>
@@ -1470,7 +1471,7 @@
         <f t="shared" si="1"/>
         <v>53504</v>
       </c>
-      <c r="C49" s="55" t="str">
+      <c r="C49" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D100</v>
       </c>
@@ -1482,15 +1483,15 @@
         <f t="shared" si="1"/>
         <v>53248</v>
       </c>
-      <c r="C50" s="55" t="str">
+      <c r="C50" s="54" t="str">
         <f t="shared" si="0"/>
         <v>D000</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1498,7 +1499,7 @@
         <f t="shared" si="1"/>
         <v>52992</v>
       </c>
-      <c r="C51" s="55" t="str">
+      <c r="C51" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CF00</v>
       </c>
@@ -1509,7 +1510,7 @@
         <f t="shared" si="1"/>
         <v>52736</v>
       </c>
-      <c r="C52" s="55" t="str">
+      <c r="C52" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CE00</v>
       </c>
@@ -1520,7 +1521,7 @@
         <f t="shared" si="1"/>
         <v>52480</v>
       </c>
-      <c r="C53" s="55" t="str">
+      <c r="C53" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CD00</v>
       </c>
@@ -1531,7 +1532,7 @@
         <f t="shared" si="1"/>
         <v>52224</v>
       </c>
-      <c r="C54" s="55" t="str">
+      <c r="C54" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CC00</v>
       </c>
@@ -1542,7 +1543,7 @@
         <f t="shared" si="1"/>
         <v>51968</v>
       </c>
-      <c r="C55" s="55" t="str">
+      <c r="C55" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CB00</v>
       </c>
@@ -1553,7 +1554,7 @@
         <f t="shared" si="1"/>
         <v>51712</v>
       </c>
-      <c r="C56" s="55" t="str">
+      <c r="C56" s="54" t="str">
         <f t="shared" si="0"/>
         <v>CA00</v>
       </c>
@@ -1564,7 +1565,7 @@
         <f t="shared" si="1"/>
         <v>51456</v>
       </c>
-      <c r="C57" s="55" t="str">
+      <c r="C57" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C900</v>
       </c>
@@ -1575,7 +1576,7 @@
         <f t="shared" si="1"/>
         <v>51200</v>
       </c>
-      <c r="C58" s="55" t="str">
+      <c r="C58" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C800</v>
       </c>
@@ -1586,7 +1587,7 @@
         <f t="shared" si="1"/>
         <v>50944</v>
       </c>
-      <c r="C59" s="55" t="str">
+      <c r="C59" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C700</v>
       </c>
@@ -1597,7 +1598,7 @@
         <f t="shared" si="1"/>
         <v>50688</v>
       </c>
-      <c r="C60" s="55" t="str">
+      <c r="C60" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C600</v>
       </c>
@@ -1608,7 +1609,7 @@
         <f t="shared" si="1"/>
         <v>50432</v>
       </c>
-      <c r="C61" s="55" t="str">
+      <c r="C61" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C500</v>
       </c>
@@ -1619,7 +1620,7 @@
         <f t="shared" si="1"/>
         <v>50176</v>
       </c>
-      <c r="C62" s="55" t="str">
+      <c r="C62" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C400</v>
       </c>
@@ -1630,7 +1631,7 @@
         <f t="shared" si="1"/>
         <v>49920</v>
       </c>
-      <c r="C63" s="55" t="str">
+      <c r="C63" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C300</v>
       </c>
@@ -1641,7 +1642,7 @@
         <f t="shared" si="1"/>
         <v>49664</v>
       </c>
-      <c r="C64" s="55" t="str">
+      <c r="C64" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C200</v>
       </c>
@@ -1652,387 +1653,387 @@
         <f t="shared" si="1"/>
         <v>49408</v>
       </c>
-      <c r="C65" s="55" t="str">
+      <c r="C65" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C100</v>
       </c>
       <c r="E65" s="19"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="57" t="s">
+      <c r="A66" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+      <c r="C66" s="55" t="str">
+        <f t="shared" si="0"/>
+        <v>C000</v>
+      </c>
+      <c r="E66" s="36"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B66">
-        <f t="shared" si="1"/>
-        <v>49152</v>
-      </c>
-      <c r="C66" s="56" t="str">
-        <f t="shared" si="0"/>
-        <v>C000</v>
-      </c>
-      <c r="E66" s="36"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="57" t="s">
-        <v>38</v>
-      </c>
       <c r="B67">
         <f t="shared" si="1"/>
         <v>48896</v>
       </c>
-      <c r="C67" s="51" t="str">
+      <c r="C67" s="50" t="str">
         <f t="shared" ref="C67:C130" si="2">DEC2HEX(B67)</f>
         <v>BF00</v>
       </c>
-      <c r="E67" s="65"/>
+      <c r="E67" s="64"/>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" ref="B68:B131" si="3">B67-256</f>
         <v>48640</v>
       </c>
-      <c r="C68" s="52" t="str">
+      <c r="C68" s="51" t="str">
         <f t="shared" si="2"/>
         <v>BE00</v>
       </c>
-      <c r="E68" s="66"/>
+      <c r="E68" s="65"/>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="3"/>
         <v>48384</v>
       </c>
-      <c r="C69" s="52" t="str">
+      <c r="C69" s="51" t="str">
         <f t="shared" si="2"/>
         <v>BD00</v>
       </c>
-      <c r="E69" s="66"/>
+      <c r="E69" s="65"/>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="3"/>
         <v>48128</v>
       </c>
-      <c r="C70" s="52" t="str">
+      <c r="C70" s="51" t="str">
         <f t="shared" si="2"/>
         <v>BC00</v>
       </c>
-      <c r="E70" s="66"/>
+      <c r="E70" s="65"/>
     </row>
     <row r="71" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="3"/>
         <v>47872</v>
       </c>
-      <c r="C71" s="52" t="str">
+      <c r="C71" s="51" t="str">
         <f t="shared" si="2"/>
         <v>BB00</v>
       </c>
-      <c r="E71" s="66"/>
+      <c r="E71" s="65"/>
     </row>
     <row r="72" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="3"/>
         <v>47616</v>
       </c>
-      <c r="C72" s="52" t="str">
+      <c r="C72" s="51" t="str">
         <f t="shared" si="2"/>
         <v>BA00</v>
       </c>
-      <c r="E72" s="66"/>
+      <c r="E72" s="65"/>
     </row>
     <row r="73" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="3"/>
         <v>47360</v>
       </c>
-      <c r="C73" s="52" t="str">
+      <c r="C73" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B900</v>
       </c>
-      <c r="E73" s="66"/>
+      <c r="E73" s="65"/>
     </row>
     <row r="74" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="3"/>
         <v>47104</v>
       </c>
-      <c r="C74" s="52" t="str">
+      <c r="C74" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B800</v>
       </c>
-      <c r="E74" s="66"/>
+      <c r="E74" s="65"/>
     </row>
     <row r="75" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="3"/>
         <v>46848</v>
       </c>
-      <c r="C75" s="52" t="str">
+      <c r="C75" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B700</v>
       </c>
-      <c r="E75" s="66"/>
+      <c r="E75" s="65"/>
     </row>
     <row r="76" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="3"/>
         <v>46592</v>
       </c>
-      <c r="C76" s="52" t="str">
+      <c r="C76" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B600</v>
       </c>
-      <c r="E76" s="66"/>
+      <c r="E76" s="65"/>
     </row>
     <row r="77" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="3"/>
         <v>46336</v>
       </c>
-      <c r="C77" s="52" t="str">
+      <c r="C77" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B500</v>
       </c>
-      <c r="E77" s="66"/>
+      <c r="E77" s="65"/>
     </row>
     <row r="78" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="3"/>
         <v>46080</v>
       </c>
-      <c r="C78" s="52" t="str">
+      <c r="C78" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B400</v>
       </c>
-      <c r="E78" s="66"/>
+      <c r="E78" s="65"/>
     </row>
     <row r="79" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="3"/>
         <v>45824</v>
       </c>
-      <c r="C79" s="52" t="str">
+      <c r="C79" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B300</v>
       </c>
-      <c r="E79" s="66"/>
+      <c r="E79" s="65"/>
     </row>
     <row r="80" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="3"/>
         <v>45568</v>
       </c>
-      <c r="C80" s="52" t="str">
+      <c r="C80" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B200</v>
       </c>
-      <c r="E80" s="66"/>
+      <c r="E80" s="65"/>
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="3"/>
         <v>45312</v>
       </c>
-      <c r="C81" s="52" t="str">
+      <c r="C81" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B100</v>
       </c>
-      <c r="E81" s="66"/>
+      <c r="E81" s="65"/>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="3"/>
         <v>45056</v>
       </c>
-      <c r="C82" s="52" t="str">
+      <c r="C82" s="51" t="str">
         <f t="shared" si="2"/>
         <v>B000</v>
       </c>
-      <c r="E82" s="66"/>
+      <c r="E82" s="65"/>
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="3"/>
         <v>44800</v>
       </c>
-      <c r="C83" s="52" t="str">
+      <c r="C83" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AF00</v>
       </c>
-      <c r="E83" s="66"/>
+      <c r="E83" s="65"/>
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="3"/>
         <v>44544</v>
       </c>
-      <c r="C84" s="52" t="str">
+      <c r="C84" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AE00</v>
       </c>
-      <c r="E84" s="66"/>
+      <c r="E84" s="65"/>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" si="3"/>
         <v>44288</v>
       </c>
-      <c r="C85" s="52" t="str">
+      <c r="C85" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AD00</v>
       </c>
-      <c r="E85" s="66"/>
+      <c r="E85" s="65"/>
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="3"/>
         <v>44032</v>
       </c>
-      <c r="C86" s="52" t="str">
+      <c r="C86" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AC00</v>
       </c>
-      <c r="E86" s="66"/>
+      <c r="E86" s="65"/>
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="3"/>
         <v>43776</v>
       </c>
-      <c r="C87" s="52" t="str">
+      <c r="C87" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AB00</v>
       </c>
-      <c r="E87" s="66"/>
+      <c r="E87" s="65"/>
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="3"/>
         <v>43520</v>
       </c>
-      <c r="C88" s="52" t="str">
+      <c r="C88" s="51" t="str">
         <f t="shared" si="2"/>
         <v>AA00</v>
       </c>
-      <c r="E88" s="66"/>
+      <c r="E88" s="65"/>
     </row>
     <row r="89" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="3"/>
         <v>43264</v>
       </c>
-      <c r="C89" s="52" t="str">
+      <c r="C89" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A900</v>
       </c>
-      <c r="E89" s="66"/>
+      <c r="E89" s="65"/>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="3"/>
         <v>43008</v>
       </c>
-      <c r="C90" s="52" t="str">
+      <c r="C90" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A800</v>
       </c>
-      <c r="E90" s="66"/>
+      <c r="E90" s="65"/>
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="3"/>
         <v>42752</v>
       </c>
-      <c r="C91" s="52" t="str">
+      <c r="C91" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A700</v>
       </c>
-      <c r="E91" s="66"/>
+      <c r="E91" s="65"/>
     </row>
     <row r="92" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="3"/>
         <v>42496</v>
       </c>
-      <c r="C92" s="52" t="str">
+      <c r="C92" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A600</v>
       </c>
-      <c r="E92" s="66"/>
+      <c r="E92" s="65"/>
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="58"/>
+      <c r="A93" s="57"/>
       <c r="B93">
         <f t="shared" si="3"/>
         <v>42240</v>
       </c>
-      <c r="C93" s="52" t="str">
+      <c r="C93" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A500</v>
       </c>
-      <c r="E93" s="66"/>
+      <c r="E93" s="65"/>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="58"/>
+      <c r="A94" s="57"/>
       <c r="B94">
         <f t="shared" si="3"/>
         <v>41984</v>
       </c>
-      <c r="C94" s="52" t="str">
+      <c r="C94" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A400</v>
       </c>
-      <c r="E94" s="66"/>
+      <c r="E94" s="65"/>
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="58"/>
+      <c r="A95" s="57"/>
       <c r="B95">
         <f t="shared" si="3"/>
         <v>41728</v>
       </c>
-      <c r="C95" s="52" t="str">
+      <c r="C95" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A300</v>
       </c>
-      <c r="E95" s="66"/>
+      <c r="E95" s="65"/>
     </row>
     <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="58"/>
+      <c r="A96" s="57"/>
       <c r="B96">
         <f t="shared" si="3"/>
         <v>41472</v>
       </c>
-      <c r="C96" s="52" t="str">
+      <c r="C96" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A200</v>
       </c>
-      <c r="E96" s="66"/>
+      <c r="E96" s="65"/>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="58"/>
+      <c r="A97" s="57"/>
       <c r="B97">
         <f t="shared" si="3"/>
         <v>41216</v>
       </c>
-      <c r="C97" s="52" t="str">
+      <c r="C97" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A100</v>
       </c>
-      <c r="E97" s="66"/>
+      <c r="E97" s="65"/>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="58"/>
+      <c r="A98" s="57"/>
       <c r="B98">
         <f t="shared" si="3"/>
         <v>40960</v>
       </c>
-      <c r="C98" s="52" t="str">
+      <c r="C98" s="51" t="str">
         <f t="shared" si="2"/>
         <v>A000</v>
       </c>
-      <c r="E98" s="67" t="s">
-        <v>43</v>
+      <c r="E98" s="66" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2040,7 +2041,7 @@
         <f t="shared" si="3"/>
         <v>40704</v>
       </c>
-      <c r="C99" s="52" t="str">
+      <c r="C99" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9F00</v>
       </c>
@@ -2052,7 +2053,7 @@
         <f t="shared" si="3"/>
         <v>40448</v>
       </c>
-      <c r="C100" s="52" t="str">
+      <c r="C100" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9E00</v>
       </c>
@@ -2064,7 +2065,7 @@
         <f t="shared" si="3"/>
         <v>40192</v>
       </c>
-      <c r="C101" s="52" t="str">
+      <c r="C101" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9D00</v>
       </c>
@@ -2076,7 +2077,7 @@
         <f t="shared" si="3"/>
         <v>39936</v>
       </c>
-      <c r="C102" s="52" t="str">
+      <c r="C102" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9C00</v>
       </c>
@@ -2088,7 +2089,7 @@
         <f t="shared" si="3"/>
         <v>39680</v>
       </c>
-      <c r="C103" s="52" t="str">
+      <c r="C103" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9B00</v>
       </c>
@@ -2100,7 +2101,7 @@
         <f t="shared" si="3"/>
         <v>39424</v>
       </c>
-      <c r="C104" s="52" t="str">
+      <c r="C104" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9A00</v>
       </c>
@@ -2112,7 +2113,7 @@
         <f t="shared" si="3"/>
         <v>39168</v>
       </c>
-      <c r="C105" s="52" t="str">
+      <c r="C105" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9900</v>
       </c>
@@ -2124,7 +2125,7 @@
         <f t="shared" si="3"/>
         <v>38912</v>
       </c>
-      <c r="C106" s="52" t="str">
+      <c r="C106" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9800</v>
       </c>
@@ -2136,7 +2137,7 @@
         <f t="shared" si="3"/>
         <v>38656</v>
       </c>
-      <c r="C107" s="52" t="str">
+      <c r="C107" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9700</v>
       </c>
@@ -2148,7 +2149,7 @@
         <f t="shared" si="3"/>
         <v>38400</v>
       </c>
-      <c r="C108" s="52" t="str">
+      <c r="C108" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9600</v>
       </c>
@@ -2160,7 +2161,7 @@
         <f t="shared" si="3"/>
         <v>38144</v>
       </c>
-      <c r="C109" s="52" t="str">
+      <c r="C109" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9500</v>
       </c>
@@ -2172,7 +2173,7 @@
         <f t="shared" si="3"/>
         <v>37888</v>
       </c>
-      <c r="C110" s="52" t="str">
+      <c r="C110" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9400</v>
       </c>
@@ -2184,7 +2185,7 @@
         <f t="shared" si="3"/>
         <v>37632</v>
       </c>
-      <c r="C111" s="52" t="str">
+      <c r="C111" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9300</v>
       </c>
@@ -2196,7 +2197,7 @@
         <f t="shared" si="3"/>
         <v>37376</v>
       </c>
-      <c r="C112" s="52" t="str">
+      <c r="C112" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9200</v>
       </c>
@@ -2208,7 +2209,7 @@
         <f t="shared" si="3"/>
         <v>37120</v>
       </c>
-      <c r="C113" s="52" t="str">
+      <c r="C113" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9100</v>
       </c>
@@ -2220,7 +2221,7 @@
         <f t="shared" si="3"/>
         <v>36864</v>
       </c>
-      <c r="C114" s="52" t="str">
+      <c r="C114" s="51" t="str">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
@@ -2234,7 +2235,7 @@
         <f t="shared" si="3"/>
         <v>36608</v>
       </c>
-      <c r="C115" s="52" t="str">
+      <c r="C115" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8F00</v>
       </c>
@@ -2245,7 +2246,7 @@
         <f t="shared" si="3"/>
         <v>36352</v>
       </c>
-      <c r="C116" s="52" t="str">
+      <c r="C116" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8E00</v>
       </c>
@@ -2256,7 +2257,7 @@
         <f t="shared" si="3"/>
         <v>36096</v>
       </c>
-      <c r="C117" s="52" t="str">
+      <c r="C117" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8D00</v>
       </c>
@@ -2267,7 +2268,7 @@
         <f t="shared" si="3"/>
         <v>35840</v>
       </c>
-      <c r="C118" s="52" t="str">
+      <c r="C118" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8C00</v>
       </c>
@@ -2278,7 +2279,7 @@
         <f t="shared" si="3"/>
         <v>35584</v>
       </c>
-      <c r="C119" s="52" t="str">
+      <c r="C119" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8B00</v>
       </c>
@@ -2289,7 +2290,7 @@
         <f t="shared" si="3"/>
         <v>35328</v>
       </c>
-      <c r="C120" s="52" t="str">
+      <c r="C120" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8A00</v>
       </c>
@@ -2300,7 +2301,7 @@
         <f t="shared" si="3"/>
         <v>35072</v>
       </c>
-      <c r="C121" s="52" t="str">
+      <c r="C121" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8900</v>
       </c>
@@ -2311,7 +2312,7 @@
         <f t="shared" si="3"/>
         <v>34816</v>
       </c>
-      <c r="C122" s="52" t="str">
+      <c r="C122" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8800</v>
       </c>
@@ -2322,7 +2323,7 @@
         <f t="shared" si="3"/>
         <v>34560</v>
       </c>
-      <c r="C123" s="52" t="str">
+      <c r="C123" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8700</v>
       </c>
@@ -2333,7 +2334,7 @@
         <f t="shared" si="3"/>
         <v>34304</v>
       </c>
-      <c r="C124" s="52" t="str">
+      <c r="C124" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8600</v>
       </c>
@@ -2344,7 +2345,7 @@
         <f t="shared" si="3"/>
         <v>34048</v>
       </c>
-      <c r="C125" s="52" t="str">
+      <c r="C125" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8500</v>
       </c>
@@ -2355,7 +2356,7 @@
         <f t="shared" si="3"/>
         <v>33792</v>
       </c>
-      <c r="C126" s="52" t="str">
+      <c r="C126" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8400</v>
       </c>
@@ -2366,7 +2367,7 @@
         <f t="shared" si="3"/>
         <v>33536</v>
       </c>
-      <c r="C127" s="52" t="str">
+      <c r="C127" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8300</v>
       </c>
@@ -2377,7 +2378,7 @@
         <f t="shared" si="3"/>
         <v>33280</v>
       </c>
-      <c r="C128" s="52" t="str">
+      <c r="C128" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8200</v>
       </c>
@@ -2388,35 +2389,35 @@
         <f t="shared" si="3"/>
         <v>33024</v>
       </c>
-      <c r="C129" s="52" t="str">
+      <c r="C129" s="51" t="str">
         <f t="shared" si="2"/>
         <v>8100</v>
       </c>
       <c r="E129" s="19"/>
     </row>
     <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
+      <c r="A130" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+      <c r="C130" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+      <c r="E130" s="19"/>
+    </row>
+    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B130">
-        <f t="shared" si="3"/>
-        <v>32768</v>
-      </c>
-      <c r="C130" s="53" t="str">
-        <f t="shared" si="2"/>
-        <v>8000</v>
-      </c>
-      <c r="E130" s="19"/>
-    </row>
-    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
-        <v>39</v>
-      </c>
       <c r="B131">
         <f t="shared" si="3"/>
         <v>32512</v>
       </c>
-      <c r="C131" s="54" t="str">
+      <c r="C131" s="53" t="str">
         <f t="shared" ref="C131:C194" si="4">DEC2HEX(B131)</f>
         <v>7F00</v>
       </c>
@@ -2427,7 +2428,7 @@
         <f t="shared" ref="B132:B195" si="5">B131-256</f>
         <v>32256</v>
       </c>
-      <c r="C132" s="55" t="str">
+      <c r="C132" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7E00</v>
       </c>
@@ -2438,7 +2439,7 @@
         <f t="shared" si="5"/>
         <v>32000</v>
       </c>
-      <c r="C133" s="55" t="str">
+      <c r="C133" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7D00</v>
       </c>
@@ -2449,7 +2450,7 @@
         <f t="shared" si="5"/>
         <v>31744</v>
       </c>
-      <c r="C134" s="55" t="str">
+      <c r="C134" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7C00</v>
       </c>
@@ -2460,7 +2461,7 @@
         <f t="shared" si="5"/>
         <v>31488</v>
       </c>
-      <c r="C135" s="55" t="str">
+      <c r="C135" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7B00</v>
       </c>
@@ -2471,7 +2472,7 @@
         <f t="shared" si="5"/>
         <v>31232</v>
       </c>
-      <c r="C136" s="55" t="str">
+      <c r="C136" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7A00</v>
       </c>
@@ -2482,7 +2483,7 @@
         <f t="shared" si="5"/>
         <v>30976</v>
       </c>
-      <c r="C137" s="55" t="str">
+      <c r="C137" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7900</v>
       </c>
@@ -2493,7 +2494,7 @@
         <f t="shared" si="5"/>
         <v>30720</v>
       </c>
-      <c r="C138" s="55" t="str">
+      <c r="C138" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7800</v>
       </c>
@@ -2504,7 +2505,7 @@
         <f t="shared" si="5"/>
         <v>30464</v>
       </c>
-      <c r="C139" s="55" t="str">
+      <c r="C139" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7700</v>
       </c>
@@ -2515,7 +2516,7 @@
         <f t="shared" si="5"/>
         <v>30208</v>
       </c>
-      <c r="C140" s="55" t="str">
+      <c r="C140" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7600</v>
       </c>
@@ -2526,7 +2527,7 @@
         <f t="shared" si="5"/>
         <v>29952</v>
       </c>
-      <c r="C141" s="55" t="str">
+      <c r="C141" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7500</v>
       </c>
@@ -2537,7 +2538,7 @@
         <f t="shared" si="5"/>
         <v>29696</v>
       </c>
-      <c r="C142" s="55" t="str">
+      <c r="C142" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7400</v>
       </c>
@@ -2548,7 +2549,7 @@
         <f t="shared" si="5"/>
         <v>29440</v>
       </c>
-      <c r="C143" s="55" t="str">
+      <c r="C143" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7300</v>
       </c>
@@ -2559,7 +2560,7 @@
         <f t="shared" si="5"/>
         <v>29184</v>
       </c>
-      <c r="C144" s="55" t="str">
+      <c r="C144" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7200</v>
       </c>
@@ -2570,7 +2571,7 @@
         <f t="shared" si="5"/>
         <v>28928</v>
       </c>
-      <c r="C145" s="55" t="str">
+      <c r="C145" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7100</v>
       </c>
@@ -2581,7 +2582,7 @@
         <f t="shared" si="5"/>
         <v>28672</v>
       </c>
-      <c r="C146" s="55" t="str">
+      <c r="C146" s="54" t="str">
         <f t="shared" si="4"/>
         <v>7000</v>
       </c>
@@ -2592,7 +2593,7 @@
         <f t="shared" si="5"/>
         <v>28416</v>
       </c>
-      <c r="C147" s="55" t="str">
+      <c r="C147" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6F00</v>
       </c>
@@ -2603,79 +2604,79 @@
         <f t="shared" si="5"/>
         <v>28160</v>
       </c>
-      <c r="C148" s="55" t="str">
+      <c r="C148" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6E00</v>
       </c>
       <c r="E148" s="19"/>
     </row>
     <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A149" s="58"/>
+      <c r="A149" s="57"/>
       <c r="B149">
         <f t="shared" si="5"/>
         <v>27904</v>
       </c>
-      <c r="C149" s="55" t="str">
+      <c r="C149" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6D00</v>
       </c>
       <c r="E149" s="19"/>
     </row>
     <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A150" s="58"/>
+      <c r="A150" s="57"/>
       <c r="B150">
         <f t="shared" si="5"/>
         <v>27648</v>
       </c>
-      <c r="C150" s="55" t="str">
+      <c r="C150" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6C00</v>
       </c>
       <c r="E150" s="24"/>
     </row>
     <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A151" s="58"/>
+      <c r="A151" s="57"/>
       <c r="B151">
         <f t="shared" si="5"/>
         <v>27392</v>
       </c>
-      <c r="C151" s="55" t="str">
+      <c r="C151" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6B00</v>
       </c>
       <c r="E151" s="25"/>
     </row>
     <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A152" s="58"/>
+      <c r="A152" s="57"/>
       <c r="B152">
         <f t="shared" si="5"/>
         <v>27136</v>
       </c>
-      <c r="C152" s="55" t="str">
+      <c r="C152" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6A00</v>
       </c>
       <c r="E152" s="25"/>
     </row>
     <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A153" s="58"/>
+      <c r="A153" s="57"/>
       <c r="B153">
         <f t="shared" si="5"/>
         <v>26880</v>
       </c>
-      <c r="C153" s="55" t="str">
+      <c r="C153" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6900</v>
       </c>
       <c r="E153" s="25"/>
     </row>
     <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A154" s="58"/>
+      <c r="A154" s="57"/>
       <c r="B154">
         <f t="shared" si="5"/>
         <v>26624</v>
       </c>
-      <c r="C154" s="55" t="str">
+      <c r="C154" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6800</v>
       </c>
@@ -2686,7 +2687,7 @@
         <f t="shared" si="5"/>
         <v>26368</v>
       </c>
-      <c r="C155" s="55" t="str">
+      <c r="C155" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6700</v>
       </c>
@@ -2697,7 +2698,7 @@
         <f t="shared" si="5"/>
         <v>26112</v>
       </c>
-      <c r="C156" s="55" t="str">
+      <c r="C156" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6600</v>
       </c>
@@ -2708,7 +2709,7 @@
         <f t="shared" si="5"/>
         <v>25856</v>
       </c>
-      <c r="C157" s="55" t="str">
+      <c r="C157" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6500</v>
       </c>
@@ -2719,7 +2720,7 @@
         <f t="shared" si="5"/>
         <v>25600</v>
       </c>
-      <c r="C158" s="55" t="str">
+      <c r="C158" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6400</v>
       </c>
@@ -2730,7 +2731,7 @@
         <f t="shared" si="5"/>
         <v>25344</v>
       </c>
-      <c r="C159" s="55" t="str">
+      <c r="C159" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6300</v>
       </c>
@@ -2741,7 +2742,7 @@
         <f t="shared" si="5"/>
         <v>25088</v>
       </c>
-      <c r="C160" s="55" t="str">
+      <c r="C160" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6200</v>
       </c>
@@ -2752,7 +2753,7 @@
         <f t="shared" si="5"/>
         <v>24832</v>
       </c>
-      <c r="C161" s="55" t="str">
+      <c r="C161" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6100</v>
       </c>
@@ -2763,7 +2764,7 @@
         <f t="shared" si="5"/>
         <v>24576</v>
       </c>
-      <c r="C162" s="55" t="str">
+      <c r="C162" s="54" t="str">
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
@@ -2774,7 +2775,7 @@
         <f t="shared" si="5"/>
         <v>24320</v>
       </c>
-      <c r="C163" s="55" t="str">
+      <c r="C163" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5F00</v>
       </c>
@@ -2785,7 +2786,7 @@
         <f t="shared" si="5"/>
         <v>24064</v>
       </c>
-      <c r="C164" s="55" t="str">
+      <c r="C164" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5E00</v>
       </c>
@@ -2796,7 +2797,7 @@
         <f t="shared" si="5"/>
         <v>23808</v>
       </c>
-      <c r="C165" s="55" t="str">
+      <c r="C165" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5D00</v>
       </c>
@@ -2807,7 +2808,7 @@
         <f t="shared" si="5"/>
         <v>23552</v>
       </c>
-      <c r="C166" s="55" t="str">
+      <c r="C166" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5C00</v>
       </c>
@@ -2818,7 +2819,7 @@
         <f t="shared" si="5"/>
         <v>23296</v>
       </c>
-      <c r="C167" s="55" t="str">
+      <c r="C167" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5B00</v>
       </c>
@@ -2829,7 +2830,7 @@
         <f t="shared" si="5"/>
         <v>23040</v>
       </c>
-      <c r="C168" s="55" t="str">
+      <c r="C168" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5A00</v>
       </c>
@@ -2840,7 +2841,7 @@
         <f t="shared" si="5"/>
         <v>22784</v>
       </c>
-      <c r="C169" s="55" t="str">
+      <c r="C169" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5900</v>
       </c>
@@ -2851,7 +2852,7 @@
         <f t="shared" si="5"/>
         <v>22528</v>
       </c>
-      <c r="C170" s="55" t="str">
+      <c r="C170" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5800</v>
       </c>
@@ -2862,7 +2863,7 @@
         <f t="shared" si="5"/>
         <v>22272</v>
       </c>
-      <c r="C171" s="55" t="str">
+      <c r="C171" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5700</v>
       </c>
@@ -2873,7 +2874,7 @@
         <f t="shared" si="5"/>
         <v>22016</v>
       </c>
-      <c r="C172" s="55" t="str">
+      <c r="C172" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5600</v>
       </c>
@@ -2884,7 +2885,7 @@
         <f t="shared" si="5"/>
         <v>21760</v>
       </c>
-      <c r="C173" s="55" t="str">
+      <c r="C173" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5500</v>
       </c>
@@ -2895,7 +2896,7 @@
         <f t="shared" si="5"/>
         <v>21504</v>
       </c>
-      <c r="C174" s="55" t="str">
+      <c r="C174" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5400</v>
       </c>
@@ -2906,7 +2907,7 @@
         <f t="shared" si="5"/>
         <v>21248</v>
       </c>
-      <c r="C175" s="55" t="str">
+      <c r="C175" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5300</v>
       </c>
@@ -2917,7 +2918,7 @@
         <f t="shared" si="5"/>
         <v>20992</v>
       </c>
-      <c r="C176" s="55" t="str">
+      <c r="C176" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5200</v>
       </c>
@@ -2928,7 +2929,7 @@
         <f t="shared" si="5"/>
         <v>20736</v>
       </c>
-      <c r="C177" s="55" t="str">
+      <c r="C177" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5100</v>
       </c>
@@ -2939,7 +2940,7 @@
         <f t="shared" si="5"/>
         <v>20480</v>
       </c>
-      <c r="C178" s="55" t="str">
+      <c r="C178" s="54" t="str">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
@@ -2950,7 +2951,7 @@
         <f t="shared" si="5"/>
         <v>20224</v>
       </c>
-      <c r="C179" s="55" t="str">
+      <c r="C179" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4F00</v>
       </c>
@@ -2961,7 +2962,7 @@
         <f t="shared" si="5"/>
         <v>19968</v>
       </c>
-      <c r="C180" s="55" t="str">
+      <c r="C180" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4E00</v>
       </c>
@@ -2972,7 +2973,7 @@
         <f t="shared" si="5"/>
         <v>19712</v>
       </c>
-      <c r="C181" s="55" t="str">
+      <c r="C181" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4D00</v>
       </c>
@@ -2983,12 +2984,12 @@
         <f t="shared" si="5"/>
         <v>19456</v>
       </c>
-      <c r="C182" s="55" t="str">
+      <c r="C182" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4C00</v>
       </c>
       <c r="E182" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="183" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2996,12 +2997,12 @@
         <f t="shared" si="5"/>
         <v>19200</v>
       </c>
-      <c r="C183" s="55" t="str">
+      <c r="C183" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4B00</v>
       </c>
-      <c r="E183" s="68" t="s">
-        <v>44</v>
+      <c r="E183" s="67" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="184" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3009,34 +3010,34 @@
         <f t="shared" si="5"/>
         <v>18944</v>
       </c>
-      <c r="C184" s="55" t="str">
+      <c r="C184" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4A00</v>
       </c>
-      <c r="E184" s="63"/>
+      <c r="E184" s="62"/>
     </row>
     <row r="185" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185">
         <f t="shared" si="5"/>
         <v>18688</v>
       </c>
-      <c r="C185" s="55" t="str">
+      <c r="C185" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4900</v>
       </c>
-      <c r="E185" s="63"/>
+      <c r="E185" s="62"/>
     </row>
     <row r="186" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186">
         <f t="shared" si="5"/>
         <v>18432</v>
       </c>
-      <c r="C186" s="55" t="str">
+      <c r="C186" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4800</v>
       </c>
-      <c r="E186" s="64" t="s">
-        <v>40</v>
+      <c r="E186" s="63" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="187" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3044,7 +3045,7 @@
         <f t="shared" si="5"/>
         <v>18176</v>
       </c>
-      <c r="C187" s="55" t="str">
+      <c r="C187" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4700</v>
       </c>
@@ -3055,7 +3056,7 @@
         <f t="shared" si="5"/>
         <v>17920</v>
       </c>
-      <c r="C188" s="55" t="str">
+      <c r="C188" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4600</v>
       </c>
@@ -3066,7 +3067,7 @@
         <f t="shared" si="5"/>
         <v>17664</v>
       </c>
-      <c r="C189" s="55" t="str">
+      <c r="C189" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4500</v>
       </c>
@@ -3077,7 +3078,7 @@
         <f t="shared" si="5"/>
         <v>17408</v>
       </c>
-      <c r="C190" s="55" t="str">
+      <c r="C190" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4400</v>
       </c>
@@ -3088,7 +3089,7 @@
         <f t="shared" si="5"/>
         <v>17152</v>
       </c>
-      <c r="C191" s="55" t="str">
+      <c r="C191" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4300</v>
       </c>
@@ -3099,7 +3100,7 @@
         <f t="shared" si="5"/>
         <v>16896</v>
       </c>
-      <c r="C192" s="55" t="str">
+      <c r="C192" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4200</v>
       </c>
@@ -3110,38 +3111,38 @@
         <f t="shared" si="5"/>
         <v>16640</v>
       </c>
-      <c r="C193" s="55" t="str">
+      <c r="C193" s="54" t="str">
         <f t="shared" si="4"/>
         <v>4100</v>
       </c>
       <c r="E193" s="22"/>
     </row>
-    <row r="194" spans="1:7" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B194" s="61">
+    <row r="194" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B194" s="60">
         <f t="shared" si="5"/>
         <v>16384</v>
       </c>
-      <c r="C194" s="56" t="str">
+      <c r="C194" s="55" t="str">
         <f t="shared" si="4"/>
         <v>4000</v>
       </c>
       <c r="E194" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G194" s="62"/>
+        <v>40</v>
+      </c>
+      <c r="G194" s="61"/>
     </row>
     <row r="195" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="57" t="s">
-        <v>35</v>
+      <c r="A195" s="56" t="s">
+        <v>34</v>
       </c>
       <c r="B195">
         <f t="shared" si="5"/>
         <v>16128</v>
       </c>
-      <c r="C195" s="52" t="str">
+      <c r="C195" s="51" t="str">
         <f t="shared" ref="C195:C258" si="6">DEC2HEX(B195)</f>
         <v>3F00</v>
       </c>
@@ -3152,7 +3153,7 @@
         <f t="shared" ref="B196:B227" si="7">B195-256</f>
         <v>15872</v>
       </c>
-      <c r="C196" s="52" t="str">
+      <c r="C196" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3E00</v>
       </c>
@@ -3163,7 +3164,7 @@
         <f t="shared" si="7"/>
         <v>15616</v>
       </c>
-      <c r="C197" s="52" t="str">
+      <c r="C197" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3D00</v>
       </c>
@@ -3174,7 +3175,7 @@
         <f t="shared" si="7"/>
         <v>15360</v>
       </c>
-      <c r="C198" s="52" t="str">
+      <c r="C198" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3C00</v>
       </c>
@@ -3185,7 +3186,7 @@
         <f t="shared" si="7"/>
         <v>15104</v>
       </c>
-      <c r="C199" s="52" t="str">
+      <c r="C199" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3B00</v>
       </c>
@@ -3196,7 +3197,7 @@
         <f t="shared" si="7"/>
         <v>14848</v>
       </c>
-      <c r="C200" s="52" t="str">
+      <c r="C200" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3A00</v>
       </c>
@@ -3207,7 +3208,7 @@
         <f t="shared" si="7"/>
         <v>14592</v>
       </c>
-      <c r="C201" s="52" t="str">
+      <c r="C201" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3900</v>
       </c>
@@ -3218,7 +3219,7 @@
         <f t="shared" si="7"/>
         <v>14336</v>
       </c>
-      <c r="C202" s="52" t="str">
+      <c r="C202" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3800</v>
       </c>
@@ -3229,7 +3230,7 @@
         <f t="shared" si="7"/>
         <v>14080</v>
       </c>
-      <c r="C203" s="52" t="str">
+      <c r="C203" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3700</v>
       </c>
@@ -3240,7 +3241,7 @@
         <f t="shared" si="7"/>
         <v>13824</v>
       </c>
-      <c r="C204" s="52" t="str">
+      <c r="C204" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3600</v>
       </c>
@@ -3251,7 +3252,7 @@
         <f t="shared" si="7"/>
         <v>13568</v>
       </c>
-      <c r="C205" s="52" t="str">
+      <c r="C205" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3500</v>
       </c>
@@ -3262,7 +3263,7 @@
         <f t="shared" si="7"/>
         <v>13312</v>
       </c>
-      <c r="C206" s="52" t="str">
+      <c r="C206" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3400</v>
       </c>
@@ -3273,7 +3274,7 @@
         <f t="shared" si="7"/>
         <v>13056</v>
       </c>
-      <c r="C207" s="52" t="str">
+      <c r="C207" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3300</v>
       </c>
@@ -3284,7 +3285,7 @@
         <f t="shared" si="7"/>
         <v>12800</v>
       </c>
-      <c r="C208" s="52" t="str">
+      <c r="C208" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3200</v>
       </c>
@@ -3295,7 +3296,7 @@
         <f t="shared" si="7"/>
         <v>12544</v>
       </c>
-      <c r="C209" s="52" t="str">
+      <c r="C209" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3100</v>
       </c>
@@ -3309,12 +3310,12 @@
         <f t="shared" si="7"/>
         <v>12288</v>
       </c>
-      <c r="C210" s="52" t="str">
+      <c r="C210" s="51" t="str">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
       <c r="E210" s="20" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="M210" s="5" t="s">
         <v>6</v>
@@ -3325,7 +3326,7 @@
         <f t="shared" si="7"/>
         <v>12032</v>
       </c>
-      <c r="C211" s="52" t="str">
+      <c r="C211" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2F00</v>
       </c>
@@ -3338,7 +3339,7 @@
         <f t="shared" si="7"/>
         <v>11776</v>
       </c>
-      <c r="C212" s="52" t="str">
+      <c r="C212" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2E00</v>
       </c>
@@ -3354,7 +3355,7 @@
         <f t="shared" si="7"/>
         <v>11520</v>
       </c>
-      <c r="C213" s="52" t="str">
+      <c r="C213" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2D00</v>
       </c>
@@ -3367,11 +3368,11 @@
         <f t="shared" si="7"/>
         <v>11264</v>
       </c>
-      <c r="C214" s="52" t="str">
+      <c r="C214" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2C00</v>
       </c>
-      <c r="E214" s="43"/>
+      <c r="E214" s="42"/>
       <c r="M214" s="5" t="s">
         <v>10</v>
       </c>
@@ -3381,11 +3382,11 @@
         <f t="shared" si="7"/>
         <v>11008</v>
       </c>
-      <c r="C215" s="52" t="str">
+      <c r="C215" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2B00</v>
       </c>
-      <c r="E215" s="44"/>
+      <c r="E215" s="43"/>
       <c r="M215" s="5" t="s">
         <v>11</v>
       </c>
@@ -3395,120 +3396,120 @@
         <f t="shared" si="7"/>
         <v>10752</v>
       </c>
-      <c r="C216" s="52" t="str">
+      <c r="C216" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2A00</v>
       </c>
-      <c r="E216" s="44"/>
+      <c r="E216" s="43"/>
       <c r="M216" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="58"/>
+      <c r="A217" s="57"/>
       <c r="B217">
         <f t="shared" si="7"/>
         <v>10496</v>
       </c>
-      <c r="C217" s="52" t="str">
+      <c r="C217" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2900</v>
       </c>
-      <c r="E217" s="44"/>
+      <c r="E217" s="43"/>
       <c r="M217" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A218" s="58"/>
+      <c r="A218" s="57"/>
       <c r="B218">
         <f t="shared" si="7"/>
         <v>10240</v>
       </c>
-      <c r="C218" s="52" t="str">
+      <c r="C218" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2800</v>
       </c>
-      <c r="E218" s="44"/>
+      <c r="E218" s="43"/>
       <c r="M218" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A219" s="58"/>
+      <c r="A219" s="57"/>
       <c r="B219">
         <f t="shared" si="7"/>
         <v>9984</v>
       </c>
-      <c r="C219" s="52" t="str">
+      <c r="C219" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2700</v>
       </c>
-      <c r="E219" s="44"/>
+      <c r="E219" s="43"/>
       <c r="M219" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="58"/>
+      <c r="A220" s="57"/>
       <c r="B220">
         <f t="shared" si="7"/>
         <v>9728</v>
       </c>
-      <c r="C220" s="52" t="str">
+      <c r="C220" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2600</v>
       </c>
-      <c r="E220" s="44"/>
+      <c r="E220" s="43"/>
       <c r="M220" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="221" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A221" s="58"/>
+      <c r="A221" s="57"/>
       <c r="B221">
         <f t="shared" si="7"/>
         <v>9472</v>
       </c>
-      <c r="C221" s="52" t="str">
+      <c r="C221" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2500</v>
       </c>
-      <c r="E221" s="44"/>
+      <c r="E221" s="43"/>
     </row>
     <row r="222" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A222" s="58"/>
+      <c r="A222" s="57"/>
       <c r="B222">
         <f t="shared" si="7"/>
         <v>9216</v>
       </c>
-      <c r="C222" s="52" t="str">
+      <c r="C222" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2400</v>
       </c>
-      <c r="E222" s="44"/>
+      <c r="E222" s="43"/>
     </row>
     <row r="223" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223">
         <f t="shared" si="7"/>
         <v>8960</v>
       </c>
-      <c r="C223" s="52" t="str">
+      <c r="C223" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2300</v>
       </c>
-      <c r="E223" s="44"/>
+      <c r="E223" s="43"/>
     </row>
     <row r="224" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224">
         <f t="shared" si="7"/>
         <v>8704</v>
       </c>
-      <c r="C224" s="52" t="str">
+      <c r="C224" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2200</v>
       </c>
-      <c r="E224" s="44" t="s">
+      <c r="E224" s="43" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3517,33 +3518,33 @@
         <f t="shared" si="7"/>
         <v>8448</v>
       </c>
-      <c r="C225" s="52" t="str">
+      <c r="C225" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2100</v>
       </c>
-      <c r="E225" s="44"/>
+      <c r="E225" s="43"/>
     </row>
     <row r="226" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226">
         <f t="shared" si="7"/>
         <v>8192</v>
       </c>
-      <c r="C226" s="52" t="str">
+      <c r="C226" s="51" t="str">
         <f t="shared" si="6"/>
         <v>2000</v>
       </c>
-      <c r="E226" s="44"/>
+      <c r="E226" s="43"/>
     </row>
     <row r="227" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227">
         <f t="shared" si="7"/>
         <v>7936</v>
       </c>
-      <c r="C227" s="52" t="str">
+      <c r="C227" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1F00</v>
       </c>
-      <c r="E227" s="44"/>
+      <c r="E227" s="43"/>
       <c r="G227" s="37"/>
     </row>
     <row r="228" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3551,11 +3552,11 @@
         <f t="shared" ref="B228:B258" si="8">B227-256</f>
         <v>7680</v>
       </c>
-      <c r="C228" s="52" t="str">
+      <c r="C228" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1E00</v>
       </c>
-      <c r="E228" s="44"/>
+      <c r="E228" s="43"/>
       <c r="G228" s="38"/>
     </row>
     <row r="229" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3563,11 +3564,11 @@
         <f t="shared" si="8"/>
         <v>7424</v>
       </c>
-      <c r="C229" s="52" t="str">
+      <c r="C229" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1D00</v>
       </c>
-      <c r="E229" s="44"/>
+      <c r="E229" s="43"/>
       <c r="G229" s="38"/>
     </row>
     <row r="230" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3575,11 +3576,11 @@
         <f t="shared" si="8"/>
         <v>7168</v>
       </c>
-      <c r="C230" s="52" t="str">
+      <c r="C230" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1C00</v>
       </c>
-      <c r="E230" s="44"/>
+      <c r="E230" s="43"/>
       <c r="G230" s="38"/>
     </row>
     <row r="231" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3587,11 +3588,11 @@
         <f t="shared" si="8"/>
         <v>6912</v>
       </c>
-      <c r="C231" s="52" t="str">
+      <c r="C231" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1B00</v>
       </c>
-      <c r="E231" s="44" t="s">
+      <c r="E231" s="68" t="s">
         <v>18</v>
       </c>
       <c r="G231" s="38"/>
@@ -3601,7 +3602,7 @@
         <f t="shared" si="8"/>
         <v>6656</v>
       </c>
-      <c r="C232" s="52" t="str">
+      <c r="C232" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1A00</v>
       </c>
@@ -3613,7 +3614,7 @@
         <f t="shared" si="8"/>
         <v>6400</v>
       </c>
-      <c r="C233" s="52" t="str">
+      <c r="C233" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1900</v>
       </c>
@@ -3625,7 +3626,7 @@
         <f t="shared" si="8"/>
         <v>6144</v>
       </c>
-      <c r="C234" s="52" t="str">
+      <c r="C234" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1800</v>
       </c>
@@ -3637,7 +3638,7 @@
         <f t="shared" si="8"/>
         <v>5888</v>
       </c>
-      <c r="C235" s="52" t="str">
+      <c r="C235" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1700</v>
       </c>
@@ -3649,7 +3650,7 @@
         <f t="shared" si="8"/>
         <v>5632</v>
       </c>
-      <c r="C236" s="52" t="str">
+      <c r="C236" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1600</v>
       </c>
@@ -3661,7 +3662,7 @@
         <f t="shared" si="8"/>
         <v>5376</v>
       </c>
-      <c r="C237" s="52" t="str">
+      <c r="C237" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
@@ -3673,7 +3674,7 @@
         <f t="shared" si="8"/>
         <v>5120</v>
       </c>
-      <c r="C238" s="52" t="str">
+      <c r="C238" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1400</v>
       </c>
@@ -3685,7 +3686,7 @@
         <f t="shared" si="8"/>
         <v>4864</v>
       </c>
-      <c r="C239" s="52" t="str">
+      <c r="C239" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1300</v>
       </c>
@@ -3697,7 +3698,7 @@
         <f t="shared" si="8"/>
         <v>4608</v>
       </c>
-      <c r="C240" s="52" t="str">
+      <c r="C240" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1200</v>
       </c>
@@ -3709,7 +3710,7 @@
         <f t="shared" si="8"/>
         <v>4352</v>
       </c>
-      <c r="C241" s="52" t="str">
+      <c r="C241" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1100</v>
       </c>
@@ -3721,7 +3722,7 @@
         <f t="shared" si="8"/>
         <v>4096</v>
       </c>
-      <c r="C242" s="52" t="str">
+      <c r="C242" s="51" t="str">
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
@@ -3735,7 +3736,7 @@
         <f t="shared" si="8"/>
         <v>3840</v>
       </c>
-      <c r="C243" s="52" t="str">
+      <c r="C243" s="51" t="str">
         <f t="shared" si="6"/>
         <v>F00</v>
       </c>
@@ -3746,7 +3747,7 @@
         <f t="shared" si="8"/>
         <v>3584</v>
       </c>
-      <c r="C244" s="52" t="str">
+      <c r="C244" s="51" t="str">
         <f t="shared" si="6"/>
         <v>E00</v>
       </c>
@@ -3757,7 +3758,7 @@
         <f t="shared" si="8"/>
         <v>3328</v>
       </c>
-      <c r="C245" s="52" t="str">
+      <c r="C245" s="51" t="str">
         <f t="shared" si="6"/>
         <v>D00</v>
       </c>
@@ -3768,7 +3769,7 @@
         <f t="shared" si="8"/>
         <v>3072</v>
       </c>
-      <c r="C246" s="52" t="str">
+      <c r="C246" s="51" t="str">
         <f t="shared" si="6"/>
         <v>C00</v>
       </c>
@@ -3779,7 +3780,7 @@
         <f t="shared" si="8"/>
         <v>2816</v>
       </c>
-      <c r="C247" s="52" t="str">
+      <c r="C247" s="51" t="str">
         <f t="shared" si="6"/>
         <v>B00</v>
       </c>
@@ -3790,7 +3791,7 @@
         <f t="shared" si="8"/>
         <v>2560</v>
       </c>
-      <c r="C248" s="52" t="str">
+      <c r="C248" s="51" t="str">
         <f t="shared" si="6"/>
         <v>A00</v>
       </c>
@@ -3801,7 +3802,7 @@
         <f t="shared" si="8"/>
         <v>2304</v>
       </c>
-      <c r="C249" s="52" t="str">
+      <c r="C249" s="51" t="str">
         <f t="shared" si="6"/>
         <v>900</v>
       </c>
@@ -3812,11 +3813,11 @@
         <f t="shared" si="8"/>
         <v>2048</v>
       </c>
-      <c r="C250" s="52" t="str">
+      <c r="C250" s="51" t="str">
         <f t="shared" si="6"/>
         <v>800</v>
       </c>
-      <c r="E250" s="42" t="s">
+      <c r="E250" s="69" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3825,7 +3826,7 @@
         <f t="shared" si="8"/>
         <v>1792</v>
       </c>
-      <c r="C251" s="52" t="str">
+      <c r="C251" s="51" t="str">
         <f t="shared" si="6"/>
         <v>700</v>
       </c>
@@ -3836,7 +3837,7 @@
         <f t="shared" si="8"/>
         <v>1536</v>
       </c>
-      <c r="C252" s="52" t="str">
+      <c r="C252" s="51" t="str">
         <f t="shared" si="6"/>
         <v>600</v>
       </c>
@@ -3849,7 +3850,7 @@
         <f t="shared" si="8"/>
         <v>1280</v>
       </c>
-      <c r="C253" s="52" t="str">
+      <c r="C253" s="51" t="str">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
@@ -3862,7 +3863,7 @@
         <f t="shared" si="8"/>
         <v>1024</v>
       </c>
-      <c r="C254" s="52" t="str">
+      <c r="C254" s="51" t="str">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
@@ -3873,7 +3874,7 @@
         <f t="shared" si="8"/>
         <v>768</v>
       </c>
-      <c r="C255" s="52" t="str">
+      <c r="C255" s="51" t="str">
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
@@ -3886,7 +3887,7 @@
         <f t="shared" si="8"/>
         <v>512</v>
       </c>
-      <c r="C256" s="52" t="str">
+      <c r="C256" s="51" t="str">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
@@ -3899,7 +3900,7 @@
         <f t="shared" si="8"/>
         <v>256</v>
       </c>
-      <c r="C257" s="52" t="str">
+      <c r="C257" s="51" t="str">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
@@ -3908,14 +3909,14 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="57" t="s">
-        <v>35</v>
+      <c r="A258" s="56" t="s">
+        <v>34</v>
       </c>
       <c r="B258">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="C258" s="53" t="str">
+      <c r="C258" s="52" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Created separate boot app and refactoring
</commit_message>
<xml_diff>
--- a/Docs/Vortex Memory Map.xlsx
+++ b/Docs/Vortex Memory Map.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -79,12 +80,6 @@
   </si>
   <si>
     <t>Working Storage</t>
-  </si>
-  <si>
-    <t>(TCP Packets, etc)</t>
-  </si>
-  <si>
-    <t>Buffer</t>
   </si>
   <si>
     <t>Character ROM (seen by VIC)</t>
@@ -174,6 +169,12 @@
   </si>
   <si>
     <t>Music</t>
+  </si>
+  <si>
+    <t>More sprites</t>
+  </si>
+  <si>
+    <t>(Packet Buffers, etc)</t>
   </si>
 </sst>
 </file>
@@ -226,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,12 +308,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -338,6 +333,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -462,7 +469,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -471,7 +477,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -489,20 +494,22 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -512,31 +519,37 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,12 +558,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FFFF3300"/>
     </mruColors>
   </colors>
   <extLst>
@@ -850,13 +863,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E250" sqref="E250"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="56" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="49" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="5.140625" customWidth="1"/>
@@ -865,2468 +878,2657 @@
     <col min="7" max="7" width="34.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56"/>
-      <c r="C1" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="15" t="s">
-        <v>24</v>
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49"/>
+      <c r="C1" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>36</v>
+      <c r="A2" s="74" t="s">
+        <v>34</v>
       </c>
       <c r="B2">
         <v>65536</v>
       </c>
-      <c r="C2" s="53" t="str">
+      <c r="C2" s="46" t="str">
         <f>DEC2HEX(B2-1)</f>
         <v>FFFF</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="48"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74"/>
       <c r="B3">
         <f>B2-256</f>
         <v>65280</v>
       </c>
-      <c r="C3" s="54" t="str">
+      <c r="C3" s="47" t="str">
         <f t="shared" ref="C3:C66" si="0">DEC2HEX(B3)</f>
         <v>FF00</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="48"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="74"/>
       <c r="B4">
         <f t="shared" ref="B4:B67" si="1">B3-256</f>
         <v>65024</v>
       </c>
-      <c r="C4" s="54" t="str">
+      <c r="C4" s="47" t="str">
         <f t="shared" si="0"/>
         <v>FE00</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="48"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="74"/>
       <c r="B5">
         <f t="shared" si="1"/>
         <v>64768</v>
       </c>
-      <c r="C5" s="54" t="str">
+      <c r="C5" s="47" t="str">
         <f t="shared" si="0"/>
         <v>FD00</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="48"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="74"/>
       <c r="B6">
         <f t="shared" si="1"/>
         <v>64512</v>
       </c>
-      <c r="C6" s="54" t="str">
+      <c r="C6" s="47" t="str">
         <f t="shared" si="0"/>
         <v>FC00</v>
       </c>
-      <c r="E6" s="45"/>
-      <c r="F6" s="48"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="74"/>
       <c r="B7">
         <f t="shared" si="1"/>
         <v>64256</v>
       </c>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="47" t="str">
         <f t="shared" si="0"/>
         <v>FB00</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="48"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="74"/>
       <c r="B8">
         <f t="shared" si="1"/>
         <v>64000</v>
       </c>
-      <c r="C8" s="54" t="str">
+      <c r="C8" s="47" t="str">
         <f t="shared" si="0"/>
         <v>FA00</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="48"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="74"/>
       <c r="B9">
         <f t="shared" si="1"/>
         <v>63744</v>
       </c>
-      <c r="C9" s="54" t="str">
+      <c r="C9" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F900</v>
       </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="48"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="74"/>
       <c r="B10">
         <f t="shared" si="1"/>
         <v>63488</v>
       </c>
-      <c r="C10" s="54" t="str">
+      <c r="C10" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F800</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="48"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="74"/>
       <c r="B11">
         <f t="shared" si="1"/>
         <v>63232</v>
       </c>
-      <c r="C11" s="54" t="str">
+      <c r="C11" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F700</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="48"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="42"/>
     </row>
     <row r="12" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="74"/>
       <c r="B12">
         <f t="shared" si="1"/>
         <v>62976</v>
       </c>
-      <c r="C12" s="54" t="str">
+      <c r="C12" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F600</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="48"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="74"/>
       <c r="B13">
         <f t="shared" si="1"/>
         <v>62720</v>
       </c>
-      <c r="C13" s="54" t="str">
+      <c r="C13" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F500</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="48"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74"/>
       <c r="B14">
         <f t="shared" si="1"/>
         <v>62464</v>
       </c>
-      <c r="C14" s="54" t="str">
+      <c r="C14" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F400</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="48"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="74"/>
       <c r="B15">
         <f t="shared" si="1"/>
         <v>62208</v>
       </c>
-      <c r="C15" s="54" t="str">
+      <c r="C15" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F300</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="48"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="74"/>
       <c r="B16">
         <f t="shared" si="1"/>
         <v>61952</v>
       </c>
-      <c r="C16" s="54" t="str">
+      <c r="C16" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F200</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="48"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
       <c r="B17">
         <f t="shared" si="1"/>
         <v>61696</v>
       </c>
-      <c r="C17" s="54" t="str">
+      <c r="C17" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F100</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="48"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="74"/>
       <c r="B18">
         <f t="shared" si="1"/>
         <v>61440</v>
       </c>
-      <c r="C18" s="54" t="str">
+      <c r="C18" s="47" t="str">
         <f t="shared" si="0"/>
         <v>F000</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="48"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="74"/>
       <c r="B19">
         <f t="shared" si="1"/>
         <v>61184</v>
       </c>
-      <c r="C19" s="54" t="str">
+      <c r="C19" s="47" t="str">
         <f t="shared" si="0"/>
         <v>EF00</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="48"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="74"/>
       <c r="B20">
         <f t="shared" si="1"/>
         <v>60928</v>
       </c>
-      <c r="C20" s="54" t="str">
+      <c r="C20" s="47" t="str">
         <f t="shared" si="0"/>
         <v>EE00</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="48"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="57"/>
+      <c r="A21" s="75"/>
       <c r="B21">
         <f t="shared" si="1"/>
         <v>60672</v>
       </c>
-      <c r="C21" s="54" t="str">
+      <c r="C21" s="47" t="str">
         <f t="shared" si="0"/>
         <v>ED00</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="48"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="57"/>
+      <c r="A22" s="75"/>
       <c r="B22">
         <f t="shared" si="1"/>
         <v>60416</v>
       </c>
-      <c r="C22" s="54" t="str">
+      <c r="C22" s="47" t="str">
         <f t="shared" si="0"/>
         <v>EC00</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="48"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="57"/>
+      <c r="A23" s="75"/>
       <c r="B23">
         <f t="shared" si="1"/>
         <v>60160</v>
       </c>
-      <c r="C23" s="54" t="str">
+      <c r="C23" s="47" t="str">
         <f t="shared" si="0"/>
         <v>EB00</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="48"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="42"/>
     </row>
     <row r="24" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
+      <c r="A24" s="75"/>
       <c r="B24">
         <f t="shared" si="1"/>
         <v>59904</v>
       </c>
-      <c r="C24" s="54" t="str">
+      <c r="C24" s="47" t="str">
         <f t="shared" si="0"/>
         <v>EA00</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="48"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="42"/>
     </row>
     <row r="25" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="57"/>
+      <c r="A25" s="75"/>
       <c r="B25">
         <f t="shared" si="1"/>
         <v>59648</v>
       </c>
-      <c r="C25" s="54" t="str">
+      <c r="C25" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E900</v>
       </c>
-      <c r="E25" s="45"/>
-      <c r="F25" s="48"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="42"/>
     </row>
     <row r="26" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="57"/>
+      <c r="A26" s="75"/>
       <c r="B26">
         <f t="shared" si="1"/>
         <v>59392</v>
       </c>
-      <c r="C26" s="54" t="str">
+      <c r="C26" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E800</v>
       </c>
-      <c r="E26" s="45"/>
-      <c r="F26" s="48"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="42"/>
     </row>
     <row r="27" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="74"/>
       <c r="B27">
         <f t="shared" si="1"/>
         <v>59136</v>
       </c>
-      <c r="C27" s="54" t="str">
+      <c r="C27" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E700</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="48"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="42"/>
     </row>
     <row r="28" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="74"/>
       <c r="B28">
         <f t="shared" si="1"/>
         <v>58880</v>
       </c>
-      <c r="C28" s="54" t="str">
+      <c r="C28" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E600</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="48"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="42"/>
     </row>
     <row r="29" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="74"/>
       <c r="B29">
         <f t="shared" si="1"/>
         <v>58624</v>
       </c>
-      <c r="C29" s="54" t="str">
+      <c r="C29" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E500</v>
       </c>
-      <c r="E29" s="45"/>
-      <c r="F29" s="48"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="74"/>
       <c r="B30">
         <f t="shared" si="1"/>
         <v>58368</v>
       </c>
-      <c r="C30" s="54" t="str">
+      <c r="C30" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E400</v>
       </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="48"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="42"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="74"/>
       <c r="B31">
         <f t="shared" si="1"/>
         <v>58112</v>
       </c>
-      <c r="C31" s="54" t="str">
+      <c r="C31" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E300</v>
       </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="48"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="42"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="74"/>
       <c r="B32">
         <f t="shared" si="1"/>
         <v>57856</v>
       </c>
-      <c r="C32" s="54" t="str">
+      <c r="C32" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E200</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="48"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="39"/>
+      <c r="F32" s="42"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="74"/>
       <c r="B33">
         <f t="shared" si="1"/>
         <v>57600</v>
       </c>
-      <c r="C33" s="54" t="str">
+      <c r="C33" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E100</v>
       </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="48"/>
-    </row>
-    <row r="34" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="39"/>
+      <c r="F33" s="42"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="74"/>
       <c r="B34">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C34" s="54" t="str">
+      <c r="C34" s="47" t="str">
         <f t="shared" si="0"/>
         <v>E000</v>
       </c>
-      <c r="E34" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="48"/>
-    </row>
-    <row r="35" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="42"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="74"/>
       <c r="B35">
         <f t="shared" si="1"/>
         <v>57088</v>
       </c>
-      <c r="C35" s="54" t="str">
+      <c r="C35" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DF00</v>
       </c>
-      <c r="E35" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="43"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="74"/>
       <c r="B36">
         <f t="shared" si="1"/>
         <v>56832</v>
       </c>
-      <c r="C36" s="54" t="str">
+      <c r="C36" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DE00</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="27"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="74"/>
       <c r="B37">
         <f t="shared" si="1"/>
         <v>56576</v>
       </c>
-      <c r="C37" s="54" t="str">
+      <c r="C37" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DD00</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="74"/>
       <c r="B38">
         <f t="shared" si="1"/>
         <v>56320</v>
       </c>
-      <c r="C38" s="54" t="str">
+      <c r="C38" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DC00</v>
       </c>
-      <c r="E38" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="74"/>
       <c r="B39">
         <f t="shared" si="1"/>
         <v>56064</v>
       </c>
-      <c r="C39" s="54" t="str">
+      <c r="C39" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DB00</v>
       </c>
       <c r="E39" s="9"/>
-      <c r="G39" s="13"/>
-    </row>
-    <row r="40" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="74"/>
       <c r="B40">
         <f t="shared" si="1"/>
         <v>55808</v>
       </c>
-      <c r="C40" s="54" t="str">
+      <c r="C40" s="47" t="str">
         <f t="shared" si="0"/>
         <v>DA00</v>
       </c>
       <c r="E40" s="10"/>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="41" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="74"/>
       <c r="B41">
         <f t="shared" si="1"/>
         <v>55552</v>
       </c>
-      <c r="C41" s="54" t="str">
+      <c r="C41" s="47" t="str">
         <f t="shared" si="0"/>
         <v>D900</v>
       </c>
       <c r="E41" s="10"/>
-      <c r="G41" s="13"/>
-    </row>
-    <row r="42" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="74"/>
       <c r="B42">
         <f t="shared" si="1"/>
         <v>55296</v>
       </c>
-      <c r="C42" s="54" t="str">
+      <c r="C42" s="47" t="str">
         <f t="shared" si="0"/>
         <v>D800</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="74"/>
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>55040</v>
+      </c>
+      <c r="C43" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D700</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="74"/>
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>54784</v>
+      </c>
+      <c r="C44" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D600</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="74"/>
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>54528</v>
+      </c>
+      <c r="C45" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D500</v>
+      </c>
+      <c r="E45" s="29"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="74"/>
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>54272</v>
+      </c>
+      <c r="C46" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D400</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="74"/>
+      <c r="B47">
+        <f t="shared" si="1"/>
+        <v>54016</v>
+      </c>
+      <c r="C47" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D300</v>
+      </c>
+      <c r="E47" s="31"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="74"/>
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>53760</v>
+      </c>
+      <c r="C48" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D200</v>
+      </c>
+      <c r="E48" s="32"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="74"/>
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>53504</v>
+      </c>
+      <c r="C49" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D100</v>
+      </c>
+      <c r="E49" s="32"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="74"/>
+      <c r="B50">
+        <f t="shared" si="1"/>
+        <v>53248</v>
+      </c>
+      <c r="C50" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>D000</v>
+      </c>
+      <c r="E50" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="13"/>
-    </row>
-    <row r="43" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <f t="shared" si="1"/>
-        <v>55040</v>
-      </c>
-      <c r="C43" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D700</v>
-      </c>
-      <c r="E43" s="30"/>
-      <c r="G43" s="13"/>
-    </row>
-    <row r="44" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <f t="shared" si="1"/>
-        <v>54784</v>
-      </c>
-      <c r="C44" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D600</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="G44" s="13"/>
-    </row>
-    <row r="45" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <f t="shared" si="1"/>
-        <v>54528</v>
-      </c>
-      <c r="C45" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D500</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="G45" s="13"/>
-    </row>
-    <row r="46" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <f t="shared" si="1"/>
-        <v>54272</v>
-      </c>
-      <c r="C46" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D400</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" s="13"/>
-    </row>
-    <row r="47" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <f t="shared" si="1"/>
-        <v>54016</v>
-      </c>
-      <c r="C47" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D300</v>
-      </c>
-      <c r="E47" s="33"/>
-      <c r="G47" s="13"/>
-    </row>
-    <row r="48" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <f t="shared" si="1"/>
-        <v>53760</v>
-      </c>
-      <c r="C48" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D200</v>
-      </c>
-      <c r="E48" s="34"/>
-      <c r="G48" s="13"/>
-    </row>
-    <row r="49" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <f t="shared" si="1"/>
-        <v>53504</v>
-      </c>
-      <c r="C49" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D100</v>
-      </c>
-      <c r="E49" s="34"/>
-      <c r="G49" s="13"/>
-    </row>
-    <row r="50" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <f t="shared" si="1"/>
-        <v>53248</v>
-      </c>
-      <c r="C50" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>D000</v>
-      </c>
-      <c r="E50" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="74"/>
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>52992</v>
+      </c>
+      <c r="C51" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CF00</v>
+      </c>
+      <c r="E51" s="59"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="74"/>
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>52736</v>
+      </c>
+      <c r="C52" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CE00</v>
+      </c>
+      <c r="E52" s="60"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="74"/>
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>52480</v>
+      </c>
+      <c r="C53" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CD00</v>
+      </c>
+      <c r="E53" s="60"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="74"/>
+      <c r="B54">
+        <f t="shared" si="1"/>
+        <v>52224</v>
+      </c>
+      <c r="C54" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CC00</v>
+      </c>
+      <c r="E54" s="60"/>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="74"/>
+      <c r="B55">
+        <f t="shared" si="1"/>
+        <v>51968</v>
+      </c>
+      <c r="C55" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CB00</v>
+      </c>
+      <c r="E55" s="60"/>
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="74"/>
+      <c r="B56">
+        <f t="shared" si="1"/>
+        <v>51712</v>
+      </c>
+      <c r="C56" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>CA00</v>
+      </c>
+      <c r="E56" s="60"/>
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="74"/>
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>51456</v>
+      </c>
+      <c r="C57" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C900</v>
+      </c>
+      <c r="E57" s="60"/>
+    </row>
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="74"/>
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>51200</v>
+      </c>
+      <c r="C58" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C800</v>
+      </c>
+      <c r="E58" s="60"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="74"/>
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>50944</v>
+      </c>
+      <c r="C59" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C700</v>
+      </c>
+      <c r="E59" s="60"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="74"/>
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>50688</v>
+      </c>
+      <c r="C60" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C600</v>
+      </c>
+      <c r="E60" s="60"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="74"/>
+      <c r="B61">
+        <f t="shared" si="1"/>
+        <v>50432</v>
+      </c>
+      <c r="C61" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C500</v>
+      </c>
+      <c r="E61" s="60"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="74"/>
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>50176</v>
+      </c>
+      <c r="C62" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C400</v>
+      </c>
+      <c r="E62" s="60"/>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="74"/>
+      <c r="B63">
+        <f t="shared" si="1"/>
+        <v>49920</v>
+      </c>
+      <c r="C63" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C300</v>
+      </c>
+      <c r="E63" s="60"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="74"/>
+      <c r="B64">
+        <f t="shared" si="1"/>
+        <v>49664</v>
+      </c>
+      <c r="C64" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C200</v>
+      </c>
+      <c r="E64" s="60"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="74"/>
+      <c r="B65">
+        <f t="shared" si="1"/>
+        <v>49408</v>
+      </c>
+      <c r="C65" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>C100</v>
+      </c>
+      <c r="E65" s="60"/>
+    </row>
+    <row r="66" spans="1:7" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="51">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+      <c r="C66" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>C000</v>
+      </c>
+      <c r="E66" s="77"/>
+      <c r="G66" s="52"/>
+    </row>
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="71" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <f t="shared" si="1"/>
-        <v>52992</v>
-      </c>
-      <c r="C51" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CF00</v>
-      </c>
-      <c r="E51" s="18"/>
-    </row>
-    <row r="52" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <f t="shared" si="1"/>
-        <v>52736</v>
-      </c>
-      <c r="C52" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CE00</v>
-      </c>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <f t="shared" si="1"/>
-        <v>52480</v>
-      </c>
-      <c r="C53" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CD00</v>
-      </c>
-      <c r="E53" s="19"/>
-    </row>
-    <row r="54" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <f t="shared" si="1"/>
-        <v>52224</v>
-      </c>
-      <c r="C54" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CC00</v>
-      </c>
-      <c r="E54" s="19"/>
-    </row>
-    <row r="55" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <f t="shared" si="1"/>
-        <v>51968</v>
-      </c>
-      <c r="C55" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CB00</v>
-      </c>
-      <c r="E55" s="19"/>
-    </row>
-    <row r="56" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56">
-        <f t="shared" si="1"/>
-        <v>51712</v>
-      </c>
-      <c r="C56" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>CA00</v>
-      </c>
-      <c r="E56" s="19"/>
-    </row>
-    <row r="57" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <f t="shared" si="1"/>
-        <v>51456</v>
-      </c>
-      <c r="C57" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C900</v>
-      </c>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <f t="shared" si="1"/>
-        <v>51200</v>
-      </c>
-      <c r="C58" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C800</v>
-      </c>
-      <c r="E58" s="19"/>
-    </row>
-    <row r="59" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <f t="shared" si="1"/>
-        <v>50944</v>
-      </c>
-      <c r="C59" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C700</v>
-      </c>
-      <c r="E59" s="19"/>
-    </row>
-    <row r="60" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60">
-        <f t="shared" si="1"/>
-        <v>50688</v>
-      </c>
-      <c r="C60" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C600</v>
-      </c>
-      <c r="E60" s="19"/>
-    </row>
-    <row r="61" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61">
-        <f t="shared" si="1"/>
-        <v>50432</v>
-      </c>
-      <c r="C61" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C500</v>
-      </c>
-      <c r="E61" s="19"/>
-    </row>
-    <row r="62" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62">
-        <f t="shared" si="1"/>
-        <v>50176</v>
-      </c>
-      <c r="C62" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C400</v>
-      </c>
-      <c r="E62" s="19"/>
-    </row>
-    <row r="63" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63">
-        <f t="shared" si="1"/>
-        <v>49920</v>
-      </c>
-      <c r="C63" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C300</v>
-      </c>
-      <c r="E63" s="19"/>
-    </row>
-    <row r="64" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64">
-        <f t="shared" si="1"/>
-        <v>49664</v>
-      </c>
-      <c r="C64" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C200</v>
-      </c>
-      <c r="E64" s="19"/>
-    </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65">
-        <f t="shared" si="1"/>
-        <v>49408</v>
-      </c>
-      <c r="C65" s="54" t="str">
-        <f t="shared" si="0"/>
-        <v>C100</v>
-      </c>
-      <c r="E65" s="19"/>
-    </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="B66">
-        <f t="shared" si="1"/>
-        <v>49152</v>
-      </c>
-      <c r="C66" s="55" t="str">
-        <f t="shared" si="0"/>
-        <v>C000</v>
-      </c>
-      <c r="E66" s="36"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="56" t="s">
-        <v>37</v>
-      </c>
       <c r="B67">
         <f t="shared" si="1"/>
         <v>48896</v>
       </c>
-      <c r="C67" s="50" t="str">
+      <c r="C67" s="44" t="str">
         <f t="shared" ref="C67:C130" si="2">DEC2HEX(B67)</f>
         <v>BF00</v>
       </c>
-      <c r="E67" s="64"/>
-    </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="55"/>
+    </row>
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="71"/>
       <c r="B68">
         <f t="shared" ref="B68:B131" si="3">B67-256</f>
         <v>48640</v>
       </c>
-      <c r="C68" s="51" t="str">
+      <c r="C68" s="44" t="str">
         <f t="shared" si="2"/>
         <v>BE00</v>
       </c>
-      <c r="E68" s="65"/>
-    </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="55"/>
+    </row>
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="71"/>
       <c r="B69">
         <f t="shared" si="3"/>
         <v>48384</v>
       </c>
-      <c r="C69" s="51" t="str">
+      <c r="C69" s="44" t="str">
         <f t="shared" si="2"/>
         <v>BD00</v>
       </c>
-      <c r="E69" s="65"/>
-    </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="55"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="71"/>
       <c r="B70">
         <f t="shared" si="3"/>
         <v>48128</v>
       </c>
-      <c r="C70" s="51" t="str">
+      <c r="C70" s="44" t="str">
         <f t="shared" si="2"/>
         <v>BC00</v>
       </c>
-      <c r="E70" s="65"/>
-    </row>
-    <row r="71" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="55"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="71"/>
       <c r="B71">
         <f t="shared" si="3"/>
         <v>47872</v>
       </c>
-      <c r="C71" s="51" t="str">
+      <c r="C71" s="44" t="str">
         <f t="shared" si="2"/>
         <v>BB00</v>
       </c>
-      <c r="E71" s="65"/>
-    </row>
-    <row r="72" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="55"/>
+    </row>
+    <row r="72" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="71"/>
       <c r="B72">
         <f t="shared" si="3"/>
         <v>47616</v>
       </c>
-      <c r="C72" s="51" t="str">
+      <c r="C72" s="44" t="str">
         <f t="shared" si="2"/>
         <v>BA00</v>
       </c>
-      <c r="E72" s="65"/>
-    </row>
-    <row r="73" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="55"/>
+    </row>
+    <row r="73" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="71"/>
       <c r="B73">
         <f t="shared" si="3"/>
         <v>47360</v>
       </c>
-      <c r="C73" s="51" t="str">
+      <c r="C73" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B900</v>
       </c>
-      <c r="E73" s="65"/>
-    </row>
-    <row r="74" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="55"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="71"/>
       <c r="B74">
         <f t="shared" si="3"/>
         <v>47104</v>
       </c>
-      <c r="C74" s="51" t="str">
+      <c r="C74" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B800</v>
       </c>
-      <c r="E74" s="65"/>
-    </row>
-    <row r="75" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="55"/>
+    </row>
+    <row r="75" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="71"/>
       <c r="B75">
         <f t="shared" si="3"/>
         <v>46848</v>
       </c>
-      <c r="C75" s="51" t="str">
+      <c r="C75" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B700</v>
       </c>
-      <c r="E75" s="65"/>
-    </row>
-    <row r="76" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="55"/>
+    </row>
+    <row r="76" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="71"/>
       <c r="B76">
         <f t="shared" si="3"/>
         <v>46592</v>
       </c>
-      <c r="C76" s="51" t="str">
+      <c r="C76" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B600</v>
       </c>
-      <c r="E76" s="65"/>
-    </row>
-    <row r="77" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="55"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="71"/>
       <c r="B77">
         <f t="shared" si="3"/>
         <v>46336</v>
       </c>
-      <c r="C77" s="51" t="str">
+      <c r="C77" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B500</v>
       </c>
-      <c r="E77" s="65"/>
-    </row>
-    <row r="78" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="55"/>
+    </row>
+    <row r="78" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="71"/>
       <c r="B78">
         <f t="shared" si="3"/>
         <v>46080</v>
       </c>
-      <c r="C78" s="51" t="str">
+      <c r="C78" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B400</v>
       </c>
-      <c r="E78" s="65"/>
-    </row>
-    <row r="79" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="55"/>
+    </row>
+    <row r="79" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="71"/>
       <c r="B79">
         <f t="shared" si="3"/>
         <v>45824</v>
       </c>
-      <c r="C79" s="51" t="str">
+      <c r="C79" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B300</v>
       </c>
-      <c r="E79" s="65"/>
-    </row>
-    <row r="80" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="55"/>
+    </row>
+    <row r="80" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="71"/>
       <c r="B80">
         <f t="shared" si="3"/>
         <v>45568</v>
       </c>
-      <c r="C80" s="51" t="str">
+      <c r="C80" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B200</v>
       </c>
-      <c r="E80" s="65"/>
+      <c r="E80" s="55"/>
     </row>
     <row r="81" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="71"/>
       <c r="B81">
         <f t="shared" si="3"/>
         <v>45312</v>
       </c>
-      <c r="C81" s="51" t="str">
+      <c r="C81" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B100</v>
       </c>
-      <c r="E81" s="65"/>
+      <c r="E81" s="55"/>
     </row>
     <row r="82" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="71"/>
       <c r="B82">
         <f t="shared" si="3"/>
         <v>45056</v>
       </c>
-      <c r="C82" s="51" t="str">
+      <c r="C82" s="44" t="str">
         <f t="shared" si="2"/>
         <v>B000</v>
       </c>
-      <c r="E82" s="65"/>
+      <c r="E82" s="55"/>
     </row>
     <row r="83" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="71"/>
       <c r="B83">
         <f t="shared" si="3"/>
         <v>44800</v>
       </c>
-      <c r="C83" s="51" t="str">
+      <c r="C83" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AF00</v>
       </c>
-      <c r="E83" s="65"/>
+      <c r="E83" s="55"/>
     </row>
     <row r="84" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="71"/>
       <c r="B84">
         <f t="shared" si="3"/>
         <v>44544</v>
       </c>
-      <c r="C84" s="51" t="str">
+      <c r="C84" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AE00</v>
       </c>
-      <c r="E84" s="65"/>
+      <c r="E84" s="55"/>
     </row>
     <row r="85" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="71"/>
       <c r="B85">
         <f t="shared" si="3"/>
         <v>44288</v>
       </c>
-      <c r="C85" s="51" t="str">
+      <c r="C85" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AD00</v>
       </c>
-      <c r="E85" s="65"/>
+      <c r="E85" s="55"/>
     </row>
     <row r="86" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="71"/>
       <c r="B86">
         <f t="shared" si="3"/>
         <v>44032</v>
       </c>
-      <c r="C86" s="51" t="str">
+      <c r="C86" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AC00</v>
       </c>
-      <c r="E86" s="65"/>
+      <c r="E86" s="55"/>
     </row>
     <row r="87" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="71"/>
       <c r="B87">
         <f t="shared" si="3"/>
         <v>43776</v>
       </c>
-      <c r="C87" s="51" t="str">
+      <c r="C87" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AB00</v>
       </c>
-      <c r="E87" s="65"/>
+      <c r="E87" s="55"/>
     </row>
     <row r="88" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="71"/>
       <c r="B88">
         <f t="shared" si="3"/>
         <v>43520</v>
       </c>
-      <c r="C88" s="51" t="str">
+      <c r="C88" s="44" t="str">
         <f t="shared" si="2"/>
         <v>AA00</v>
       </c>
-      <c r="E88" s="65"/>
+      <c r="E88" s="55"/>
     </row>
     <row r="89" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="71"/>
       <c r="B89">
         <f t="shared" si="3"/>
         <v>43264</v>
       </c>
-      <c r="C89" s="51" t="str">
+      <c r="C89" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A900</v>
       </c>
-      <c r="E89" s="65"/>
+      <c r="E89" s="55"/>
     </row>
     <row r="90" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="71"/>
       <c r="B90">
         <f t="shared" si="3"/>
         <v>43008</v>
       </c>
-      <c r="C90" s="51" t="str">
+      <c r="C90" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A800</v>
       </c>
-      <c r="E90" s="65"/>
+      <c r="E90" s="55"/>
     </row>
     <row r="91" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="71"/>
       <c r="B91">
         <f t="shared" si="3"/>
         <v>42752</v>
       </c>
-      <c r="C91" s="51" t="str">
+      <c r="C91" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A700</v>
       </c>
-      <c r="E91" s="65"/>
+      <c r="E91" s="55"/>
     </row>
     <row r="92" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="71"/>
       <c r="B92">
         <f t="shared" si="3"/>
         <v>42496</v>
       </c>
-      <c r="C92" s="51" t="str">
+      <c r="C92" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A600</v>
       </c>
-      <c r="E92" s="65"/>
+      <c r="E92" s="55"/>
     </row>
     <row r="93" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="57"/>
+      <c r="A93" s="72"/>
       <c r="B93">
         <f t="shared" si="3"/>
         <v>42240</v>
       </c>
-      <c r="C93" s="51" t="str">
+      <c r="C93" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A500</v>
       </c>
-      <c r="E93" s="65"/>
+      <c r="E93" s="55"/>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="57"/>
+      <c r="A94" s="72"/>
       <c r="B94">
         <f t="shared" si="3"/>
         <v>41984</v>
       </c>
-      <c r="C94" s="51" t="str">
+      <c r="C94" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A400</v>
       </c>
-      <c r="E94" s="65"/>
+      <c r="E94" s="55"/>
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="57"/>
+      <c r="A95" s="72"/>
       <c r="B95">
         <f t="shared" si="3"/>
         <v>41728</v>
       </c>
-      <c r="C95" s="51" t="str">
+      <c r="C95" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A300</v>
       </c>
-      <c r="E95" s="65"/>
+      <c r="E95" s="55"/>
     </row>
     <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="57"/>
+      <c r="A96" s="72"/>
       <c r="B96">
         <f t="shared" si="3"/>
         <v>41472</v>
       </c>
-      <c r="C96" s="51" t="str">
+      <c r="C96" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A200</v>
       </c>
-      <c r="E96" s="65"/>
+      <c r="E96" s="55"/>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="57"/>
+      <c r="A97" s="72"/>
       <c r="B97">
         <f t="shared" si="3"/>
         <v>41216</v>
       </c>
-      <c r="C97" s="51" t="str">
+      <c r="C97" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A100</v>
       </c>
-      <c r="E97" s="65"/>
+      <c r="E97" s="55"/>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="57"/>
+      <c r="A98" s="72"/>
       <c r="B98">
         <f t="shared" si="3"/>
         <v>40960</v>
       </c>
-      <c r="C98" s="51" t="str">
+      <c r="C98" s="44" t="str">
         <f t="shared" si="2"/>
         <v>A000</v>
       </c>
-      <c r="E98" s="66" t="s">
-        <v>42</v>
+      <c r="E98" s="56" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="71"/>
       <c r="B99">
         <f t="shared" si="3"/>
         <v>40704</v>
       </c>
-      <c r="C99" s="51" t="str">
+      <c r="C99" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9F00</v>
       </c>
-      <c r="E99" s="19"/>
-      <c r="G99" s="37"/>
+      <c r="E99" s="60"/>
+      <c r="G99" s="34"/>
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="71"/>
       <c r="B100">
         <f t="shared" si="3"/>
         <v>40448</v>
       </c>
-      <c r="C100" s="51" t="str">
+      <c r="C100" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9E00</v>
       </c>
-      <c r="E100" s="19"/>
-      <c r="G100" s="38"/>
+      <c r="E100" s="60"/>
+      <c r="G100" s="35"/>
     </row>
     <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="71"/>
       <c r="B101">
         <f t="shared" si="3"/>
         <v>40192</v>
       </c>
-      <c r="C101" s="51" t="str">
+      <c r="C101" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9D00</v>
       </c>
-      <c r="E101" s="19"/>
-      <c r="G101" s="38"/>
+      <c r="E101" s="60"/>
+      <c r="G101" s="35"/>
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="71"/>
       <c r="B102">
         <f t="shared" si="3"/>
         <v>39936</v>
       </c>
-      <c r="C102" s="51" t="str">
+      <c r="C102" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9C00</v>
       </c>
-      <c r="E102" s="19"/>
-      <c r="G102" s="38"/>
+      <c r="E102" s="60"/>
+      <c r="G102" s="35"/>
     </row>
     <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="71"/>
       <c r="B103">
         <f t="shared" si="3"/>
         <v>39680</v>
       </c>
-      <c r="C103" s="51" t="str">
+      <c r="C103" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9B00</v>
       </c>
-      <c r="E103" s="19"/>
-      <c r="G103" s="38"/>
+      <c r="E103" s="60"/>
+      <c r="G103" s="35"/>
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="71"/>
       <c r="B104">
         <f t="shared" si="3"/>
         <v>39424</v>
       </c>
-      <c r="C104" s="51" t="str">
+      <c r="C104" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9A00</v>
       </c>
-      <c r="E104" s="19"/>
-      <c r="G104" s="38"/>
+      <c r="E104" s="60"/>
+      <c r="G104" s="35"/>
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="71"/>
       <c r="B105">
         <f t="shared" si="3"/>
         <v>39168</v>
       </c>
-      <c r="C105" s="51" t="str">
+      <c r="C105" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9900</v>
       </c>
-      <c r="E105" s="19"/>
-      <c r="G105" s="38"/>
+      <c r="E105" s="60"/>
+      <c r="G105" s="35"/>
     </row>
     <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="71"/>
       <c r="B106">
         <f t="shared" si="3"/>
         <v>38912</v>
       </c>
-      <c r="C106" s="51" t="str">
+      <c r="C106" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9800</v>
       </c>
-      <c r="E106" s="19"/>
-      <c r="G106" s="38"/>
+      <c r="E106" s="60"/>
+      <c r="G106" s="35"/>
     </row>
     <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="71"/>
       <c r="B107">
         <f t="shared" si="3"/>
         <v>38656</v>
       </c>
-      <c r="C107" s="51" t="str">
+      <c r="C107" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9700</v>
       </c>
-      <c r="E107" s="19"/>
-      <c r="G107" s="38"/>
+      <c r="E107" s="60"/>
+      <c r="G107" s="35"/>
     </row>
     <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="71"/>
       <c r="B108">
         <f t="shared" si="3"/>
         <v>38400</v>
       </c>
-      <c r="C108" s="51" t="str">
+      <c r="C108" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9600</v>
       </c>
-      <c r="E108" s="19"/>
-      <c r="G108" s="38"/>
+      <c r="E108" s="60"/>
+      <c r="G108" s="35"/>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="71"/>
       <c r="B109">
         <f t="shared" si="3"/>
         <v>38144</v>
       </c>
-      <c r="C109" s="51" t="str">
+      <c r="C109" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9500</v>
       </c>
-      <c r="E109" s="19"/>
-      <c r="G109" s="38"/>
+      <c r="E109" s="60"/>
+      <c r="G109" s="35"/>
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="71"/>
       <c r="B110">
         <f t="shared" si="3"/>
         <v>37888</v>
       </c>
-      <c r="C110" s="51" t="str">
+      <c r="C110" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9400</v>
       </c>
-      <c r="E110" s="19"/>
-      <c r="G110" s="38"/>
+      <c r="E110" s="60"/>
+      <c r="G110" s="35"/>
     </row>
     <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="71"/>
       <c r="B111">
         <f t="shared" si="3"/>
         <v>37632</v>
       </c>
-      <c r="C111" s="51" t="str">
+      <c r="C111" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9300</v>
       </c>
-      <c r="E111" s="19"/>
-      <c r="G111" s="38"/>
+      <c r="E111" s="60"/>
+      <c r="G111" s="35"/>
     </row>
     <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="71"/>
       <c r="B112">
         <f t="shared" si="3"/>
         <v>37376</v>
       </c>
-      <c r="C112" s="51" t="str">
+      <c r="C112" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9200</v>
       </c>
-      <c r="E112" s="19"/>
-      <c r="G112" s="38"/>
-    </row>
-    <row r="113" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E112" s="60"/>
+      <c r="G112" s="35"/>
+    </row>
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="71"/>
       <c r="B113">
         <f t="shared" si="3"/>
         <v>37120</v>
       </c>
-      <c r="C113" s="51" t="str">
+      <c r="C113" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9100</v>
       </c>
-      <c r="E113" s="19"/>
-      <c r="G113" s="38"/>
-    </row>
-    <row r="114" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E113" s="60"/>
+      <c r="G113" s="35"/>
+    </row>
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="71"/>
       <c r="B114">
         <f t="shared" si="3"/>
         <v>36864</v>
       </c>
-      <c r="C114" s="51" t="str">
+      <c r="C114" s="44" t="str">
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="E114" s="19"/>
-      <c r="G114" s="39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E114" s="60"/>
+      <c r="G114" s="36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="71"/>
       <c r="B115">
         <f t="shared" si="3"/>
         <v>36608</v>
       </c>
-      <c r="C115" s="51" t="str">
+      <c r="C115" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8F00</v>
       </c>
-      <c r="E115" s="19"/>
-    </row>
-    <row r="116" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E115" s="60"/>
+    </row>
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="71"/>
       <c r="B116">
         <f t="shared" si="3"/>
         <v>36352</v>
       </c>
-      <c r="C116" s="51" t="str">
+      <c r="C116" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8E00</v>
       </c>
-      <c r="E116" s="19"/>
-    </row>
-    <row r="117" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E116" s="60"/>
+    </row>
+    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="71"/>
       <c r="B117">
         <f t="shared" si="3"/>
         <v>36096</v>
       </c>
-      <c r="C117" s="51" t="str">
+      <c r="C117" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8D00</v>
       </c>
-      <c r="E117" s="19"/>
-    </row>
-    <row r="118" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E117" s="60"/>
+    </row>
+    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="71"/>
       <c r="B118">
         <f t="shared" si="3"/>
         <v>35840</v>
       </c>
-      <c r="C118" s="51" t="str">
+      <c r="C118" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8C00</v>
       </c>
-      <c r="E118" s="19"/>
-    </row>
-    <row r="119" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E118" s="60"/>
+    </row>
+    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="71"/>
       <c r="B119">
         <f t="shared" si="3"/>
         <v>35584</v>
       </c>
-      <c r="C119" s="51" t="str">
+      <c r="C119" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8B00</v>
       </c>
-      <c r="E119" s="19"/>
-    </row>
-    <row r="120" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E119" s="60"/>
+    </row>
+    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="71"/>
       <c r="B120">
         <f t="shared" si="3"/>
         <v>35328</v>
       </c>
-      <c r="C120" s="51" t="str">
+      <c r="C120" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8A00</v>
       </c>
-      <c r="E120" s="19"/>
-    </row>
-    <row r="121" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E120" s="60"/>
+    </row>
+    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="71"/>
       <c r="B121">
         <f t="shared" si="3"/>
         <v>35072</v>
       </c>
-      <c r="C121" s="51" t="str">
+      <c r="C121" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8900</v>
       </c>
-      <c r="E121" s="19"/>
-    </row>
-    <row r="122" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E121" s="60"/>
+    </row>
+    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="71"/>
       <c r="B122">
         <f t="shared" si="3"/>
         <v>34816</v>
       </c>
-      <c r="C122" s="51" t="str">
+      <c r="C122" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8800</v>
       </c>
-      <c r="E122" s="19"/>
-    </row>
-    <row r="123" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E122" s="60"/>
+    </row>
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="71"/>
       <c r="B123">
         <f t="shared" si="3"/>
         <v>34560</v>
       </c>
-      <c r="C123" s="51" t="str">
+      <c r="C123" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8700</v>
       </c>
-      <c r="E123" s="19"/>
-    </row>
-    <row r="124" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E123" s="60"/>
+    </row>
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="71"/>
       <c r="B124">
         <f t="shared" si="3"/>
         <v>34304</v>
       </c>
-      <c r="C124" s="51" t="str">
+      <c r="C124" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8600</v>
       </c>
-      <c r="E124" s="19"/>
-    </row>
-    <row r="125" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E124" s="60"/>
+    </row>
+    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="71"/>
       <c r="B125">
         <f t="shared" si="3"/>
         <v>34048</v>
       </c>
-      <c r="C125" s="51" t="str">
+      <c r="C125" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8500</v>
       </c>
-      <c r="E125" s="19"/>
-    </row>
-    <row r="126" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E125" s="60"/>
+    </row>
+    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="71"/>
       <c r="B126">
         <f t="shared" si="3"/>
         <v>33792</v>
       </c>
-      <c r="C126" s="51" t="str">
+      <c r="C126" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8400</v>
       </c>
-      <c r="E126" s="19"/>
-    </row>
-    <row r="127" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E126" s="60"/>
+    </row>
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="71"/>
       <c r="B127">
         <f t="shared" si="3"/>
         <v>33536</v>
       </c>
-      <c r="C127" s="51" t="str">
+      <c r="C127" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8300</v>
       </c>
-      <c r="E127" s="19"/>
-    </row>
-    <row r="128" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E127" s="60"/>
+    </row>
+    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="71"/>
       <c r="B128">
         <f t="shared" si="3"/>
         <v>33280</v>
       </c>
-      <c r="C128" s="51" t="str">
+      <c r="C128" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8200</v>
       </c>
-      <c r="E128" s="19"/>
-    </row>
-    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E128" s="60"/>
+    </row>
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="71"/>
       <c r="B129">
         <f t="shared" si="3"/>
         <v>33024</v>
       </c>
-      <c r="C129" s="51" t="str">
+      <c r="C129" s="44" t="str">
         <f t="shared" si="2"/>
         <v>8100</v>
       </c>
-      <c r="E129" s="19"/>
-    </row>
-    <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="B130">
+      <c r="E129" s="60"/>
+    </row>
+    <row r="130" spans="1:7" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B130" s="51">
         <f t="shared" si="3"/>
         <v>32768</v>
       </c>
-      <c r="C130" s="52" t="str">
+      <c r="C130" s="45" t="str">
         <f t="shared" si="2"/>
         <v>8000</v>
       </c>
-      <c r="E130" s="19"/>
-    </row>
-    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="56" t="s">
-        <v>38</v>
+      <c r="E130" s="70"/>
+      <c r="G130" s="52"/>
+    </row>
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="65" t="s">
+        <v>36</v>
       </c>
       <c r="B131">
         <f t="shared" si="3"/>
         <v>32512</v>
       </c>
-      <c r="C131" s="53" t="str">
+      <c r="C131" s="47" t="str">
         <f t="shared" ref="C131:C194" si="4">DEC2HEX(B131)</f>
         <v>7F00</v>
       </c>
-      <c r="E131" s="19"/>
-    </row>
-    <row r="132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E131" s="60"/>
+    </row>
+    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="65"/>
       <c r="B132">
         <f t="shared" ref="B132:B195" si="5">B131-256</f>
         <v>32256</v>
       </c>
-      <c r="C132" s="54" t="str">
+      <c r="C132" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7E00</v>
       </c>
-      <c r="E132" s="19"/>
-    </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E132" s="22"/>
+    </row>
+    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="65"/>
       <c r="B133">
         <f t="shared" si="5"/>
         <v>32000</v>
       </c>
-      <c r="C133" s="54" t="str">
+      <c r="C133" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7D00</v>
       </c>
-      <c r="E133" s="19"/>
-    </row>
-    <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E133" s="23"/>
+    </row>
+    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="65"/>
       <c r="B134">
         <f t="shared" si="5"/>
         <v>31744</v>
       </c>
-      <c r="C134" s="54" t="str">
+      <c r="C134" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7C00</v>
       </c>
-      <c r="E134" s="19"/>
-    </row>
-    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E134" s="23"/>
+    </row>
+    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="65"/>
       <c r="B135">
         <f t="shared" si="5"/>
         <v>31488</v>
       </c>
-      <c r="C135" s="54" t="str">
+      <c r="C135" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7B00</v>
       </c>
-      <c r="E135" s="19"/>
-    </row>
-    <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E135" s="23"/>
+    </row>
+    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="65"/>
       <c r="B136">
         <f t="shared" si="5"/>
         <v>31232</v>
       </c>
-      <c r="C136" s="54" t="str">
+      <c r="C136" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7A00</v>
       </c>
-      <c r="E136" s="19"/>
-    </row>
-    <row r="137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E136" s="23"/>
+    </row>
+    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="65"/>
       <c r="B137">
         <f t="shared" si="5"/>
         <v>30976</v>
       </c>
-      <c r="C137" s="54" t="str">
+      <c r="C137" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7900</v>
       </c>
-      <c r="E137" s="19"/>
-    </row>
-    <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E137" s="23"/>
+    </row>
+    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="65"/>
       <c r="B138">
         <f t="shared" si="5"/>
         <v>30720</v>
       </c>
-      <c r="C138" s="54" t="str">
+      <c r="C138" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7800</v>
       </c>
-      <c r="E138" s="19"/>
-    </row>
-    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E138" s="23"/>
+    </row>
+    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="65"/>
       <c r="B139">
         <f t="shared" si="5"/>
         <v>30464</v>
       </c>
-      <c r="C139" s="54" t="str">
+      <c r="C139" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7700</v>
       </c>
-      <c r="E139" s="19"/>
-    </row>
-    <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E139" s="23"/>
+    </row>
+    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="65"/>
       <c r="B140">
         <f t="shared" si="5"/>
         <v>30208</v>
       </c>
-      <c r="C140" s="54" t="str">
+      <c r="C140" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7600</v>
       </c>
-      <c r="E140" s="19"/>
-    </row>
-    <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E140" s="23"/>
+    </row>
+    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="65"/>
       <c r="B141">
         <f t="shared" si="5"/>
         <v>29952</v>
       </c>
-      <c r="C141" s="54" t="str">
+      <c r="C141" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7500</v>
       </c>
-      <c r="E141" s="19"/>
-    </row>
-    <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E141" s="23"/>
+    </row>
+    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="65"/>
       <c r="B142">
         <f t="shared" si="5"/>
         <v>29696</v>
       </c>
-      <c r="C142" s="54" t="str">
+      <c r="C142" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7400</v>
       </c>
-      <c r="E142" s="19"/>
-    </row>
-    <row r="143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E142" s="23"/>
+    </row>
+    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="65"/>
       <c r="B143">
         <f t="shared" si="5"/>
         <v>29440</v>
       </c>
-      <c r="C143" s="54" t="str">
+      <c r="C143" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7300</v>
       </c>
-      <c r="E143" s="19"/>
-    </row>
-    <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E143" s="23"/>
+    </row>
+    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="65"/>
       <c r="B144">
         <f t="shared" si="5"/>
         <v>29184</v>
       </c>
-      <c r="C144" s="54" t="str">
+      <c r="C144" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7200</v>
       </c>
-      <c r="E144" s="19"/>
+      <c r="E144" s="23"/>
     </row>
     <row r="145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="65"/>
       <c r="B145">
         <f t="shared" si="5"/>
         <v>28928</v>
       </c>
-      <c r="C145" s="54" t="str">
+      <c r="C145" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7100</v>
       </c>
-      <c r="E145" s="19"/>
+      <c r="E145" s="23"/>
     </row>
     <row r="146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="65"/>
       <c r="B146">
         <f t="shared" si="5"/>
         <v>28672</v>
       </c>
-      <c r="C146" s="54" t="str">
+      <c r="C146" s="47" t="str">
         <f t="shared" si="4"/>
         <v>7000</v>
       </c>
-      <c r="E146" s="19"/>
+      <c r="E146" s="23"/>
     </row>
     <row r="147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="65"/>
       <c r="B147">
         <f t="shared" si="5"/>
         <v>28416</v>
       </c>
-      <c r="C147" s="54" t="str">
+      <c r="C147" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6F00</v>
       </c>
-      <c r="E147" s="19"/>
+      <c r="E147" s="23"/>
     </row>
     <row r="148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="65"/>
       <c r="B148">
         <f t="shared" si="5"/>
         <v>28160</v>
       </c>
-      <c r="C148" s="54" t="str">
+      <c r="C148" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6E00</v>
       </c>
-      <c r="E148" s="19"/>
+      <c r="E148" s="23"/>
     </row>
     <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A149" s="57"/>
+      <c r="A149" s="66"/>
       <c r="B149">
         <f t="shared" si="5"/>
         <v>27904</v>
       </c>
-      <c r="C149" s="54" t="str">
+      <c r="C149" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6D00</v>
       </c>
-      <c r="E149" s="19"/>
+      <c r="E149" s="24" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A150" s="57"/>
+      <c r="A150" s="66"/>
       <c r="B150">
         <f t="shared" si="5"/>
         <v>27648</v>
       </c>
-      <c r="C150" s="54" t="str">
+      <c r="C150" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6C00</v>
       </c>
-      <c r="E150" s="24"/>
+      <c r="E150" s="22"/>
     </row>
     <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A151" s="57"/>
+      <c r="A151" s="66"/>
       <c r="B151">
         <f t="shared" si="5"/>
         <v>27392</v>
       </c>
-      <c r="C151" s="54" t="str">
+      <c r="C151" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6B00</v>
       </c>
-      <c r="E151" s="25"/>
+      <c r="E151" s="23"/>
     </row>
     <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A152" s="57"/>
+      <c r="A152" s="66"/>
       <c r="B152">
         <f t="shared" si="5"/>
         <v>27136</v>
       </c>
-      <c r="C152" s="54" t="str">
+      <c r="C152" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6A00</v>
       </c>
-      <c r="E152" s="25"/>
+      <c r="E152" s="23"/>
     </row>
     <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A153" s="57"/>
+      <c r="A153" s="66"/>
       <c r="B153">
         <f t="shared" si="5"/>
         <v>26880</v>
       </c>
-      <c r="C153" s="54" t="str">
+      <c r="C153" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6900</v>
       </c>
-      <c r="E153" s="25"/>
+      <c r="E153" s="23"/>
     </row>
     <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A154" s="57"/>
+      <c r="A154" s="66"/>
       <c r="B154">
         <f t="shared" si="5"/>
         <v>26624</v>
       </c>
-      <c r="C154" s="54" t="str">
+      <c r="C154" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6800</v>
       </c>
-      <c r="E154" s="25"/>
+      <c r="E154" s="23"/>
     </row>
     <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="65"/>
       <c r="B155">
         <f t="shared" si="5"/>
         <v>26368</v>
       </c>
-      <c r="C155" s="54" t="str">
+      <c r="C155" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6700</v>
       </c>
-      <c r="E155" s="25"/>
+      <c r="E155" s="23"/>
     </row>
     <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="65"/>
       <c r="B156">
         <f t="shared" si="5"/>
         <v>26112</v>
       </c>
-      <c r="C156" s="54" t="str">
+      <c r="C156" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6600</v>
       </c>
-      <c r="E156" s="25"/>
+      <c r="E156" s="23"/>
     </row>
     <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="65"/>
       <c r="B157">
         <f t="shared" si="5"/>
         <v>25856</v>
       </c>
-      <c r="C157" s="54" t="str">
+      <c r="C157" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6500</v>
       </c>
-      <c r="E157" s="25"/>
+      <c r="E157" s="23"/>
     </row>
     <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="65"/>
       <c r="B158">
         <f t="shared" si="5"/>
         <v>25600</v>
       </c>
-      <c r="C158" s="54" t="str">
+      <c r="C158" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6400</v>
       </c>
-      <c r="E158" s="25"/>
+      <c r="E158" s="23"/>
     </row>
     <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="65"/>
       <c r="B159">
         <f t="shared" si="5"/>
         <v>25344</v>
       </c>
-      <c r="C159" s="54" t="str">
+      <c r="C159" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6300</v>
       </c>
-      <c r="E159" s="25"/>
+      <c r="E159" s="23"/>
     </row>
     <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="65"/>
       <c r="B160">
         <f t="shared" si="5"/>
         <v>25088</v>
       </c>
-      <c r="C160" s="54" t="str">
+      <c r="C160" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6200</v>
       </c>
-      <c r="E160" s="25"/>
-    </row>
-    <row r="161" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E160" s="23"/>
+    </row>
+    <row r="161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="65"/>
       <c r="B161">
         <f t="shared" si="5"/>
         <v>24832</v>
       </c>
-      <c r="C161" s="54" t="str">
+      <c r="C161" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6100</v>
       </c>
-      <c r="E161" s="25"/>
-    </row>
-    <row r="162" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E161" s="23"/>
+    </row>
+    <row r="162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="65"/>
       <c r="B162">
         <f t="shared" si="5"/>
         <v>24576</v>
       </c>
-      <c r="C162" s="54" t="str">
+      <c r="C162" s="47" t="str">
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
-      <c r="E162" s="25"/>
-    </row>
-    <row r="163" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E162" s="23"/>
+    </row>
+    <row r="163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="65"/>
       <c r="B163">
         <f t="shared" si="5"/>
         <v>24320</v>
       </c>
-      <c r="C163" s="54" t="str">
+      <c r="C163" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5F00</v>
       </c>
-      <c r="E163" s="25"/>
-    </row>
-    <row r="164" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E163" s="23"/>
+    </row>
+    <row r="164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="65"/>
       <c r="B164">
         <f t="shared" si="5"/>
         <v>24064</v>
       </c>
-      <c r="C164" s="54" t="str">
+      <c r="C164" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5E00</v>
       </c>
-      <c r="E164" s="25"/>
-    </row>
-    <row r="165" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E164" s="23"/>
+    </row>
+    <row r="165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="65"/>
       <c r="B165">
         <f t="shared" si="5"/>
         <v>23808</v>
       </c>
-      <c r="C165" s="54" t="str">
+      <c r="C165" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5D00</v>
       </c>
-      <c r="E165" s="25"/>
-    </row>
-    <row r="166" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E165" s="23"/>
+    </row>
+    <row r="166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="65"/>
       <c r="B166">
         <f t="shared" si="5"/>
         <v>23552</v>
       </c>
-      <c r="C166" s="54" t="str">
+      <c r="C166" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5C00</v>
       </c>
-      <c r="E166" s="25"/>
-    </row>
-    <row r="167" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E166" s="23"/>
+    </row>
+    <row r="167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="65"/>
       <c r="B167">
         <f t="shared" si="5"/>
         <v>23296</v>
       </c>
-      <c r="C167" s="54" t="str">
+      <c r="C167" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5B00</v>
       </c>
-      <c r="E167" s="25"/>
-    </row>
-    <row r="168" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E167" s="23"/>
+    </row>
+    <row r="168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="65"/>
       <c r="B168">
         <f t="shared" si="5"/>
         <v>23040</v>
       </c>
-      <c r="C168" s="54" t="str">
+      <c r="C168" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5A00</v>
       </c>
-      <c r="E168" s="25"/>
-    </row>
-    <row r="169" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E168" s="23"/>
+    </row>
+    <row r="169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="65"/>
       <c r="B169">
         <f t="shared" si="5"/>
         <v>22784</v>
       </c>
-      <c r="C169" s="54" t="str">
+      <c r="C169" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5900</v>
       </c>
-      <c r="E169" s="25"/>
-    </row>
-    <row r="170" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E169" s="23"/>
+    </row>
+    <row r="170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="65"/>
       <c r="B170">
         <f t="shared" si="5"/>
         <v>22528</v>
       </c>
-      <c r="C170" s="54" t="str">
+      <c r="C170" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5800</v>
       </c>
-      <c r="E170" s="25"/>
-    </row>
-    <row r="171" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E170" s="23"/>
+    </row>
+    <row r="171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="65"/>
       <c r="B171">
         <f t="shared" si="5"/>
         <v>22272</v>
       </c>
-      <c r="C171" s="54" t="str">
+      <c r="C171" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5700</v>
       </c>
-      <c r="E171" s="25"/>
-    </row>
-    <row r="172" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E171" s="23"/>
+    </row>
+    <row r="172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="65"/>
       <c r="B172">
         <f t="shared" si="5"/>
         <v>22016</v>
       </c>
-      <c r="C172" s="54" t="str">
+      <c r="C172" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5600</v>
       </c>
-      <c r="E172" s="25"/>
-    </row>
-    <row r="173" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E172" s="23"/>
+    </row>
+    <row r="173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="65"/>
       <c r="B173">
         <f t="shared" si="5"/>
         <v>21760</v>
       </c>
-      <c r="C173" s="54" t="str">
+      <c r="C173" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5500</v>
       </c>
-      <c r="E173" s="25"/>
-    </row>
-    <row r="174" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E173" s="23"/>
+    </row>
+    <row r="174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="65"/>
       <c r="B174">
         <f t="shared" si="5"/>
         <v>21504</v>
       </c>
-      <c r="C174" s="54" t="str">
+      <c r="C174" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5400</v>
       </c>
-      <c r="E174" s="25"/>
-    </row>
-    <row r="175" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E174" s="23"/>
+    </row>
+    <row r="175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="65"/>
       <c r="B175">
         <f t="shared" si="5"/>
         <v>21248</v>
       </c>
-      <c r="C175" s="54" t="str">
+      <c r="C175" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5300</v>
       </c>
-      <c r="E175" s="25"/>
-    </row>
-    <row r="176" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E175" s="23"/>
+    </row>
+    <row r="176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="65"/>
       <c r="B176">
         <f t="shared" si="5"/>
         <v>20992</v>
       </c>
-      <c r="C176" s="54" t="str">
+      <c r="C176" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5200</v>
       </c>
-      <c r="E176" s="25"/>
-    </row>
-    <row r="177" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E176" s="23"/>
+    </row>
+    <row r="177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="65"/>
       <c r="B177">
         <f t="shared" si="5"/>
         <v>20736</v>
       </c>
-      <c r="C177" s="54" t="str">
+      <c r="C177" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5100</v>
       </c>
-      <c r="E177" s="25"/>
-    </row>
-    <row r="178" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E177" s="23"/>
+    </row>
+    <row r="178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="65"/>
       <c r="B178">
         <f t="shared" si="5"/>
         <v>20480</v>
       </c>
-      <c r="C178" s="54" t="str">
+      <c r="C178" s="47" t="str">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
-      <c r="E178" s="25"/>
-    </row>
-    <row r="179" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E178" s="23"/>
+    </row>
+    <row r="179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="65"/>
       <c r="B179">
         <f t="shared" si="5"/>
         <v>20224</v>
       </c>
-      <c r="C179" s="54" t="str">
+      <c r="C179" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4F00</v>
       </c>
-      <c r="E179" s="25"/>
-    </row>
-    <row r="180" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E179" s="23"/>
+    </row>
+    <row r="180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="65"/>
       <c r="B180">
         <f t="shared" si="5"/>
         <v>19968</v>
       </c>
-      <c r="C180" s="54" t="str">
+      <c r="C180" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4E00</v>
       </c>
-      <c r="E180" s="25"/>
-    </row>
-    <row r="181" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E180" s="23"/>
+    </row>
+    <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="65"/>
       <c r="B181">
         <f t="shared" si="5"/>
         <v>19712</v>
       </c>
-      <c r="C181" s="54" t="str">
+      <c r="C181" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4D00</v>
       </c>
-      <c r="E181" s="25"/>
-    </row>
-    <row r="182" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E181" s="23"/>
+    </row>
+    <row r="182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="65"/>
       <c r="B182">
         <f t="shared" si="5"/>
         <v>19456</v>
       </c>
-      <c r="C182" s="54" t="str">
+      <c r="C182" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4C00</v>
       </c>
-      <c r="E182" s="26" t="s">
+      <c r="E182" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="65"/>
+      <c r="B183">
+        <f t="shared" si="5"/>
+        <v>19200</v>
+      </c>
+      <c r="C183" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>4B00</v>
+      </c>
+      <c r="E183" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="183" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183">
-        <f t="shared" si="5"/>
-        <v>19200</v>
-      </c>
-      <c r="C183" s="54" t="str">
-        <f t="shared" si="4"/>
-        <v>4B00</v>
-      </c>
-      <c r="E183" s="67" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="184" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="65"/>
       <c r="B184">
         <f t="shared" si="5"/>
         <v>18944</v>
       </c>
-      <c r="C184" s="54" t="str">
+      <c r="C184" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4A00</v>
       </c>
-      <c r="E184" s="62"/>
-    </row>
-    <row r="185" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E184" s="53"/>
+    </row>
+    <row r="185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="65"/>
       <c r="B185">
         <f t="shared" si="5"/>
         <v>18688</v>
       </c>
-      <c r="C185" s="54" t="str">
+      <c r="C185" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4900</v>
       </c>
-      <c r="E185" s="62"/>
-    </row>
-    <row r="186" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E185" s="53"/>
+    </row>
+    <row r="186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="65"/>
       <c r="B186">
         <f t="shared" si="5"/>
         <v>18432</v>
       </c>
-      <c r="C186" s="54" t="str">
+      <c r="C186" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4800</v>
       </c>
-      <c r="E186" s="63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="187" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E186" s="54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="65"/>
       <c r="B187">
         <f t="shared" si="5"/>
         <v>18176</v>
       </c>
-      <c r="C187" s="54" t="str">
+      <c r="C187" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4700</v>
       </c>
-      <c r="E187" s="21"/>
-    </row>
-    <row r="188" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E187" s="19"/>
+    </row>
+    <row r="188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="65"/>
       <c r="B188">
         <f t="shared" si="5"/>
         <v>17920</v>
       </c>
-      <c r="C188" s="54" t="str">
+      <c r="C188" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4600</v>
       </c>
-      <c r="E188" s="22"/>
-    </row>
-    <row r="189" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E188" s="20"/>
+    </row>
+    <row r="189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="65"/>
       <c r="B189">
         <f t="shared" si="5"/>
         <v>17664</v>
       </c>
-      <c r="C189" s="54" t="str">
+      <c r="C189" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4500</v>
       </c>
-      <c r="E189" s="22"/>
-    </row>
-    <row r="190" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E189" s="20"/>
+    </row>
+    <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="65"/>
       <c r="B190">
         <f t="shared" si="5"/>
         <v>17408</v>
       </c>
-      <c r="C190" s="54" t="str">
+      <c r="C190" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4400</v>
       </c>
-      <c r="E190" s="22"/>
-    </row>
-    <row r="191" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E190" s="20"/>
+    </row>
+    <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="65"/>
       <c r="B191">
         <f t="shared" si="5"/>
         <v>17152</v>
       </c>
-      <c r="C191" s="54" t="str">
+      <c r="C191" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4300</v>
       </c>
-      <c r="E191" s="22"/>
-    </row>
-    <row r="192" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E191" s="20"/>
+    </row>
+    <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="65"/>
       <c r="B192">
         <f t="shared" si="5"/>
         <v>16896</v>
       </c>
-      <c r="C192" s="54" t="str">
+      <c r="C192" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4200</v>
       </c>
-      <c r="E192" s="22"/>
+      <c r="E192" s="20"/>
     </row>
     <row r="193" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="65"/>
       <c r="B193">
         <f t="shared" si="5"/>
         <v>16640</v>
       </c>
-      <c r="C193" s="54" t="str">
+      <c r="C193" s="47" t="str">
         <f t="shared" si="4"/>
         <v>4100</v>
       </c>
-      <c r="E193" s="22"/>
-    </row>
-    <row r="194" spans="1:7" s="60" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="59" t="s">
+      <c r="E193" s="20"/>
+    </row>
+    <row r="194" spans="1:7" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B194" s="51">
+        <f t="shared" si="5"/>
+        <v>16384</v>
+      </c>
+      <c r="C194" s="48" t="str">
+        <f t="shared" si="4"/>
+        <v>4000</v>
+      </c>
+      <c r="E194" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B194" s="60">
-        <f t="shared" si="5"/>
-        <v>16384</v>
-      </c>
-      <c r="C194" s="55" t="str">
-        <f t="shared" si="4"/>
-        <v>4000</v>
-      </c>
-      <c r="E194" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G194" s="61"/>
+      <c r="G194" s="52"/>
     </row>
     <row r="195" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="56" t="s">
-        <v>34</v>
+      <c r="A195" s="67" t="s">
+        <v>32</v>
       </c>
       <c r="B195">
         <f t="shared" si="5"/>
         <v>16128</v>
       </c>
-      <c r="C195" s="51" t="str">
+      <c r="C195" s="44" t="str">
         <f t="shared" ref="C195:C258" si="6">DEC2HEX(B195)</f>
         <v>3F00</v>
       </c>
-      <c r="E195" s="19"/>
+      <c r="E195" s="17"/>
     </row>
     <row r="196" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="67"/>
       <c r="B196">
         <f t="shared" ref="B196:B227" si="7">B195-256</f>
         <v>15872</v>
       </c>
-      <c r="C196" s="51" t="str">
+      <c r="C196" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3E00</v>
       </c>
-      <c r="E196" s="19"/>
+      <c r="E196" s="17"/>
     </row>
     <row r="197" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="67"/>
       <c r="B197">
         <f t="shared" si="7"/>
         <v>15616</v>
       </c>
-      <c r="C197" s="51" t="str">
+      <c r="C197" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3D00</v>
       </c>
-      <c r="E197" s="19"/>
+      <c r="E197" s="17"/>
     </row>
     <row r="198" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="67"/>
       <c r="B198">
         <f t="shared" si="7"/>
         <v>15360</v>
       </c>
-      <c r="C198" s="51" t="str">
+      <c r="C198" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3C00</v>
       </c>
-      <c r="E198" s="19"/>
+      <c r="E198" s="17"/>
     </row>
     <row r="199" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="67"/>
       <c r="B199">
         <f t="shared" si="7"/>
         <v>15104</v>
       </c>
-      <c r="C199" s="51" t="str">
+      <c r="C199" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3B00</v>
       </c>
-      <c r="E199" s="19"/>
+      <c r="E199" s="17"/>
     </row>
     <row r="200" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="67"/>
       <c r="B200">
         <f t="shared" si="7"/>
         <v>14848</v>
       </c>
-      <c r="C200" s="51" t="str">
+      <c r="C200" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3A00</v>
       </c>
-      <c r="E200" s="19"/>
+      <c r="E200" s="17"/>
     </row>
     <row r="201" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="67"/>
       <c r="B201">
         <f t="shared" si="7"/>
         <v>14592</v>
       </c>
-      <c r="C201" s="51" t="str">
+      <c r="C201" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3900</v>
       </c>
-      <c r="E201" s="19"/>
+      <c r="E201" s="17"/>
     </row>
     <row r="202" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="67"/>
       <c r="B202">
         <f t="shared" si="7"/>
         <v>14336</v>
       </c>
-      <c r="C202" s="51" t="str">
+      <c r="C202" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3800</v>
       </c>
-      <c r="E202" s="19"/>
+      <c r="E202" s="17"/>
     </row>
     <row r="203" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="67"/>
       <c r="B203">
         <f t="shared" si="7"/>
         <v>14080</v>
       </c>
-      <c r="C203" s="51" t="str">
+      <c r="C203" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3700</v>
       </c>
-      <c r="E203" s="19"/>
+      <c r="E203" s="17"/>
     </row>
     <row r="204" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="67"/>
       <c r="B204">
         <f t="shared" si="7"/>
         <v>13824</v>
       </c>
-      <c r="C204" s="51" t="str">
+      <c r="C204" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3600</v>
       </c>
-      <c r="E204" s="19"/>
+      <c r="E204" s="17"/>
     </row>
     <row r="205" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="67"/>
       <c r="B205">
         <f t="shared" si="7"/>
         <v>13568</v>
       </c>
-      <c r="C205" s="51" t="str">
+      <c r="C205" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3500</v>
       </c>
-      <c r="E205" s="19"/>
+      <c r="E205" s="17"/>
     </row>
     <row r="206" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="67"/>
       <c r="B206">
         <f t="shared" si="7"/>
         <v>13312</v>
       </c>
-      <c r="C206" s="51" t="str">
+      <c r="C206" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3400</v>
       </c>
-      <c r="E206" s="19"/>
+      <c r="E206" s="17"/>
     </row>
     <row r="207" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="67"/>
       <c r="B207">
         <f t="shared" si="7"/>
         <v>13056</v>
       </c>
-      <c r="C207" s="51" t="str">
+      <c r="C207" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3300</v>
       </c>
-      <c r="E207" s="19"/>
+      <c r="E207" s="17"/>
     </row>
     <row r="208" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="67"/>
       <c r="B208">
         <f t="shared" si="7"/>
         <v>12800</v>
       </c>
-      <c r="C208" s="51" t="str">
+      <c r="C208" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3200</v>
       </c>
-      <c r="E208" s="19"/>
+      <c r="E208" s="17"/>
     </row>
     <row r="209" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="67"/>
       <c r="B209">
         <f t="shared" si="7"/>
         <v>12544</v>
       </c>
-      <c r="C209" s="51" t="str">
+      <c r="C209" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3100</v>
       </c>
-      <c r="E209" s="19"/>
+      <c r="E209" s="17"/>
       <c r="M209" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="67"/>
       <c r="B210">
         <f t="shared" si="7"/>
         <v>12288</v>
       </c>
-      <c r="C210" s="51" t="str">
+      <c r="C210" s="44" t="str">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
-      <c r="E210" s="20" t="s">
-        <v>44</v>
+      <c r="E210" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="M210" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="67"/>
       <c r="B211">
         <f t="shared" si="7"/>
         <v>12032</v>
       </c>
-      <c r="C211" s="51" t="str">
+      <c r="C211" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2F00</v>
       </c>
@@ -3335,509 +3537,543 @@
       </c>
     </row>
     <row r="212" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="67"/>
       <c r="B212">
         <f t="shared" si="7"/>
         <v>11776</v>
       </c>
-      <c r="C212" s="51" t="str">
+      <c r="C212" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2E00</v>
       </c>
-      <c r="E212" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="E212" s="62"/>
       <c r="M212" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="67"/>
       <c r="B213">
         <f t="shared" si="7"/>
         <v>11520</v>
       </c>
-      <c r="C213" s="51" t="str">
+      <c r="C213" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2D00</v>
       </c>
+      <c r="E213" s="61"/>
       <c r="M213" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="67"/>
       <c r="B214">
         <f t="shared" si="7"/>
         <v>11264</v>
       </c>
-      <c r="C214" s="51" t="str">
+      <c r="C214" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2C00</v>
       </c>
-      <c r="E214" s="42"/>
+      <c r="E214" s="61"/>
       <c r="M214" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="215" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="67"/>
       <c r="B215">
         <f t="shared" si="7"/>
         <v>11008</v>
       </c>
-      <c r="C215" s="51" t="str">
+      <c r="C215" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2B00</v>
       </c>
-      <c r="E215" s="43"/>
+      <c r="E215" s="64"/>
       <c r="M215" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="216" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="67"/>
       <c r="B216">
         <f t="shared" si="7"/>
         <v>10752</v>
       </c>
-      <c r="C216" s="51" t="str">
+      <c r="C216" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2A00</v>
       </c>
-      <c r="E216" s="43"/>
+      <c r="E216" s="61"/>
       <c r="M216" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="57"/>
+      <c r="A217" s="68"/>
       <c r="B217">
         <f t="shared" si="7"/>
         <v>10496</v>
       </c>
-      <c r="C217" s="51" t="str">
+      <c r="C217" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2900</v>
       </c>
-      <c r="E217" s="43"/>
+      <c r="E217" s="61"/>
       <c r="M217" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A218" s="57"/>
+      <c r="A218" s="68"/>
       <c r="B218">
         <f t="shared" si="7"/>
         <v>10240</v>
       </c>
-      <c r="C218" s="51" t="str">
+      <c r="C218" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2800</v>
       </c>
-      <c r="E218" s="43"/>
+      <c r="E218" s="61"/>
       <c r="M218" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A219" s="57"/>
+      <c r="A219" s="68"/>
       <c r="B219">
         <f t="shared" si="7"/>
         <v>9984</v>
       </c>
-      <c r="C219" s="51" t="str">
+      <c r="C219" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2700</v>
       </c>
-      <c r="E219" s="43"/>
+      <c r="E219" s="61"/>
       <c r="M219" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="57"/>
+      <c r="A220" s="68"/>
       <c r="B220">
         <f t="shared" si="7"/>
         <v>9728</v>
       </c>
-      <c r="C220" s="51" t="str">
+      <c r="C220" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2600</v>
       </c>
-      <c r="E220" s="43"/>
+      <c r="E220" s="61"/>
       <c r="M220" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="221" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A221" s="57"/>
+      <c r="A221" s="68"/>
       <c r="B221">
         <f t="shared" si="7"/>
         <v>9472</v>
       </c>
-      <c r="C221" s="51" t="str">
+      <c r="C221" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2500</v>
       </c>
-      <c r="E221" s="43"/>
+      <c r="E221" s="61"/>
     </row>
     <row r="222" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A222" s="57"/>
+      <c r="A222" s="68"/>
       <c r="B222">
         <f t="shared" si="7"/>
         <v>9216</v>
       </c>
-      <c r="C222" s="51" t="str">
+      <c r="C222" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2400</v>
       </c>
-      <c r="E222" s="43"/>
+      <c r="E222" s="61"/>
     </row>
     <row r="223" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="67"/>
       <c r="B223">
         <f t="shared" si="7"/>
         <v>8960</v>
       </c>
-      <c r="C223" s="51" t="str">
+      <c r="C223" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2300</v>
       </c>
-      <c r="E223" s="43"/>
+      <c r="E223" s="61"/>
     </row>
     <row r="224" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="67"/>
       <c r="B224">
         <f t="shared" si="7"/>
         <v>8704</v>
       </c>
-      <c r="C224" s="51" t="str">
+      <c r="C224" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2200</v>
       </c>
-      <c r="E224" s="43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="225" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E224" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="67"/>
       <c r="B225">
         <f t="shared" si="7"/>
         <v>8448</v>
       </c>
-      <c r="C225" s="51" t="str">
+      <c r="C225" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2100</v>
       </c>
-      <c r="E225" s="43"/>
-    </row>
-    <row r="226" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E225" s="61"/>
+    </row>
+    <row r="226" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="67"/>
       <c r="B226">
         <f t="shared" si="7"/>
         <v>8192</v>
       </c>
-      <c r="C226" s="51" t="str">
+      <c r="C226" s="44" t="str">
         <f t="shared" si="6"/>
         <v>2000</v>
       </c>
-      <c r="E226" s="43"/>
-    </row>
-    <row r="227" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E226" s="63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="67"/>
       <c r="B227">
         <f t="shared" si="7"/>
         <v>7936</v>
       </c>
-      <c r="C227" s="51" t="str">
+      <c r="C227" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1F00</v>
       </c>
-      <c r="E227" s="43"/>
-      <c r="G227" s="37"/>
-    </row>
-    <row r="228" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E227" s="37"/>
+      <c r="G227" s="34"/>
+    </row>
+    <row r="228" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="67"/>
       <c r="B228">
         <f t="shared" ref="B228:B258" si="8">B227-256</f>
         <v>7680</v>
       </c>
-      <c r="C228" s="51" t="str">
+      <c r="C228" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1E00</v>
       </c>
-      <c r="E228" s="43"/>
-      <c r="G228" s="38"/>
-    </row>
-    <row r="229" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E228" s="37"/>
+      <c r="G228" s="35"/>
+    </row>
+    <row r="229" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="67"/>
       <c r="B229">
         <f t="shared" si="8"/>
         <v>7424</v>
       </c>
-      <c r="C229" s="51" t="str">
+      <c r="C229" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1D00</v>
       </c>
-      <c r="E229" s="43"/>
-      <c r="G229" s="38"/>
-    </row>
-    <row r="230" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E229" s="37"/>
+      <c r="G229" s="35"/>
+    </row>
+    <row r="230" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="67"/>
       <c r="B230">
         <f t="shared" si="8"/>
         <v>7168</v>
       </c>
-      <c r="C230" s="51" t="str">
+      <c r="C230" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1C00</v>
       </c>
-      <c r="E230" s="43"/>
-      <c r="G230" s="38"/>
-    </row>
-    <row r="231" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E230" s="37"/>
+      <c r="G230" s="35"/>
+    </row>
+    <row r="231" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="67"/>
       <c r="B231">
         <f t="shared" si="8"/>
         <v>6912</v>
       </c>
-      <c r="C231" s="51" t="str">
+      <c r="C231" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1B00</v>
       </c>
-      <c r="E231" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="G231" s="38"/>
-    </row>
-    <row r="232" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E231" s="37"/>
+      <c r="G231" s="35"/>
+    </row>
+    <row r="232" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="67"/>
       <c r="B232">
         <f t="shared" si="8"/>
         <v>6656</v>
       </c>
-      <c r="C232" s="51" t="str">
+      <c r="C232" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1A00</v>
       </c>
-      <c r="E232" s="40"/>
-      <c r="G232" s="38"/>
-    </row>
-    <row r="233" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E232" s="37"/>
+      <c r="G232" s="35"/>
+    </row>
+    <row r="233" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="67"/>
       <c r="B233">
         <f t="shared" si="8"/>
         <v>6400</v>
       </c>
-      <c r="C233" s="51" t="str">
+      <c r="C233" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1900</v>
       </c>
-      <c r="E233" s="41"/>
-      <c r="G233" s="38"/>
-    </row>
-    <row r="234" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E233" s="37"/>
+      <c r="G233" s="35"/>
+    </row>
+    <row r="234" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="67"/>
       <c r="B234">
         <f t="shared" si="8"/>
         <v>6144</v>
       </c>
-      <c r="C234" s="51" t="str">
+      <c r="C234" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1800</v>
       </c>
-      <c r="E234" s="41"/>
-      <c r="G234" s="38"/>
-    </row>
-    <row r="235" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E234" s="37"/>
+      <c r="G234" s="35"/>
+    </row>
+    <row r="235" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="67"/>
       <c r="B235">
         <f t="shared" si="8"/>
         <v>5888</v>
       </c>
-      <c r="C235" s="51" t="str">
+      <c r="C235" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1700</v>
       </c>
-      <c r="E235" s="41"/>
-      <c r="G235" s="38"/>
-    </row>
-    <row r="236" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E235" s="37"/>
+      <c r="G235" s="35"/>
+    </row>
+    <row r="236" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="67"/>
       <c r="B236">
         <f t="shared" si="8"/>
         <v>5632</v>
       </c>
-      <c r="C236" s="51" t="str">
+      <c r="C236" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1600</v>
       </c>
-      <c r="E236" s="41"/>
-      <c r="G236" s="38"/>
-    </row>
-    <row r="237" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E236" s="37"/>
+      <c r="G236" s="35"/>
+    </row>
+    <row r="237" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="67"/>
       <c r="B237">
         <f t="shared" si="8"/>
         <v>5376</v>
       </c>
-      <c r="C237" s="51" t="str">
+      <c r="C237" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
-      <c r="E237" s="41"/>
-      <c r="G237" s="38"/>
-    </row>
-    <row r="238" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E237" s="37"/>
+      <c r="G237" s="35"/>
+    </row>
+    <row r="238" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="67"/>
       <c r="B238">
         <f t="shared" si="8"/>
         <v>5120</v>
       </c>
-      <c r="C238" s="51" t="str">
+      <c r="C238" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1400</v>
       </c>
-      <c r="E238" s="41"/>
-      <c r="G238" s="38"/>
-    </row>
-    <row r="239" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E238" s="37"/>
+      <c r="G238" s="35"/>
+    </row>
+    <row r="239" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="67"/>
       <c r="B239">
         <f t="shared" si="8"/>
         <v>4864</v>
       </c>
-      <c r="C239" s="51" t="str">
+      <c r="C239" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1300</v>
       </c>
-      <c r="E239" s="41"/>
-      <c r="G239" s="38"/>
-    </row>
-    <row r="240" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E239" s="37"/>
+      <c r="G239" s="35"/>
+    </row>
+    <row r="240" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="67"/>
       <c r="B240">
         <f t="shared" si="8"/>
         <v>4608</v>
       </c>
-      <c r="C240" s="51" t="str">
+      <c r="C240" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1200</v>
       </c>
-      <c r="E240" s="41"/>
-      <c r="G240" s="38"/>
-    </row>
-    <row r="241" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E240" s="37"/>
+      <c r="G240" s="35"/>
+    </row>
+    <row r="241" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="67"/>
       <c r="B241">
         <f t="shared" si="8"/>
         <v>4352</v>
       </c>
-      <c r="C241" s="51" t="str">
+      <c r="C241" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1100</v>
       </c>
-      <c r="E241" s="41"/>
-      <c r="G241" s="38"/>
-    </row>
-    <row r="242" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E241" s="37"/>
+      <c r="G241" s="35"/>
+    </row>
+    <row r="242" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="67"/>
       <c r="B242">
         <f t="shared" si="8"/>
         <v>4096</v>
       </c>
-      <c r="C242" s="51" t="str">
+      <c r="C242" s="44" t="str">
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="E242" s="41"/>
-      <c r="G242" s="39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="243" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E242" s="37"/>
+      <c r="G242" s="36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="67"/>
       <c r="B243">
         <f t="shared" si="8"/>
         <v>3840</v>
       </c>
-      <c r="C243" s="51" t="str">
+      <c r="C243" s="44" t="str">
         <f t="shared" si="6"/>
         <v>F00</v>
       </c>
-      <c r="E243" s="41"/>
-    </row>
-    <row r="244" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E243" s="37"/>
+    </row>
+    <row r="244" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="67"/>
       <c r="B244">
         <f t="shared" si="8"/>
         <v>3584</v>
       </c>
-      <c r="C244" s="51" t="str">
+      <c r="C244" s="44" t="str">
         <f t="shared" si="6"/>
         <v>E00</v>
       </c>
-      <c r="E244" s="41"/>
-    </row>
-    <row r="245" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E244" s="37"/>
+    </row>
+    <row r="245" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="67"/>
       <c r="B245">
         <f t="shared" si="8"/>
         <v>3328</v>
       </c>
-      <c r="C245" s="51" t="str">
+      <c r="C245" s="44" t="str">
         <f t="shared" si="6"/>
         <v>D00</v>
       </c>
-      <c r="E245" s="41"/>
-    </row>
-    <row r="246" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E245" s="37"/>
+    </row>
+    <row r="246" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="67"/>
       <c r="B246">
         <f t="shared" si="8"/>
         <v>3072</v>
       </c>
-      <c r="C246" s="51" t="str">
+      <c r="C246" s="44" t="str">
         <f t="shared" si="6"/>
         <v>C00</v>
       </c>
-      <c r="E246" s="41"/>
-    </row>
-    <row r="247" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E246" s="37"/>
+    </row>
+    <row r="247" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="67"/>
       <c r="B247">
         <f t="shared" si="8"/>
         <v>2816</v>
       </c>
-      <c r="C247" s="51" t="str">
+      <c r="C247" s="44" t="str">
         <f t="shared" si="6"/>
         <v>B00</v>
       </c>
-      <c r="E247" s="41"/>
-    </row>
-    <row r="248" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E247" s="37"/>
+    </row>
+    <row r="248" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="67"/>
       <c r="B248">
         <f t="shared" si="8"/>
         <v>2560</v>
       </c>
-      <c r="C248" s="51" t="str">
+      <c r="C248" s="44" t="str">
         <f t="shared" si="6"/>
         <v>A00</v>
       </c>
-      <c r="E248" s="41"/>
-    </row>
-    <row r="249" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E248" s="37"/>
+    </row>
+    <row r="249" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="67"/>
       <c r="B249">
         <f t="shared" si="8"/>
         <v>2304</v>
       </c>
-      <c r="C249" s="51" t="str">
+      <c r="C249" s="44" t="str">
         <f t="shared" si="6"/>
         <v>900</v>
       </c>
-      <c r="E249" s="41"/>
-    </row>
-    <row r="250" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E249" s="37"/>
+    </row>
+    <row r="250" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="67"/>
       <c r="B250">
         <f t="shared" si="8"/>
         <v>2048</v>
       </c>
-      <c r="C250" s="51" t="str">
+      <c r="C250" s="44" t="str">
         <f t="shared" si="6"/>
         <v>800</v>
       </c>
-      <c r="E250" s="69" t="s">
+      <c r="E250" s="58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="251" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="67"/>
       <c r="B251">
         <f t="shared" si="8"/>
         <v>1792</v>
       </c>
-      <c r="C251" s="51" t="str">
+      <c r="C251" s="44" t="str">
         <f t="shared" si="6"/>
         <v>700</v>
       </c>
       <c r="E251" s="3"/>
     </row>
-    <row r="252" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="67"/>
       <c r="B252">
         <f t="shared" si="8"/>
         <v>1536</v>
       </c>
-      <c r="C252" s="51" t="str">
+      <c r="C252" s="44" t="str">
         <f t="shared" si="6"/>
         <v>600</v>
       </c>
@@ -3845,12 +4081,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="67"/>
       <c r="B253">
         <f t="shared" si="8"/>
         <v>1280</v>
       </c>
-      <c r="C253" s="51" t="str">
+      <c r="C253" s="44" t="str">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
@@ -3858,23 +4095,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="67"/>
       <c r="B254">
         <f t="shared" si="8"/>
         <v>1024</v>
       </c>
-      <c r="C254" s="51" t="str">
+      <c r="C254" s="44" t="str">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="E254" s="4"/>
     </row>
-    <row r="255" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="67"/>
       <c r="B255">
         <f t="shared" si="8"/>
         <v>768</v>
       </c>
-      <c r="C255" s="51" t="str">
+      <c r="C255" s="44" t="str">
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
@@ -3882,12 +4121,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="67"/>
       <c r="B256">
         <f t="shared" si="8"/>
         <v>512</v>
       </c>
-      <c r="C256" s="51" t="str">
+      <c r="C256" s="44" t="str">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
@@ -3896,11 +4136,12 @@
       </c>
     </row>
     <row r="257" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="67"/>
       <c r="B257">
         <f t="shared" si="8"/>
         <v>256</v>
       </c>
-      <c r="C257" s="51" t="str">
+      <c r="C257" s="44" t="str">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
@@ -3909,14 +4150,14 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="56" t="s">
-        <v>34</v>
+      <c r="A258" s="67" t="s">
+        <v>32</v>
       </c>
       <c r="B258">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="C258" s="52" t="str">
+      <c r="C258" s="45" t="str">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>

</xml_diff>